<commit_message>
Show fuel economy standards for gasoline HDVs in web app, as it is used in reference scenarios (for buses)
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\Desktop\eps-1.4.3-california-WipF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-california\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -8242,7 +8242,7 @@
         <v>198</v>
       </c>
       <c r="I42" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J42" s="64" t="str">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Restore coal consumption graph and relable it "coal and petcoke"
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="18960" windowHeight="5940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="18960" windowHeight="5940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9803" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9809" uniqueCount="1394">
   <si>
     <t>Short Name</t>
   </si>
@@ -3874,12 +3874,6 @@
   </si>
   <si>
     <t>Output Industrial Fuel Use by Fuel[heat if]; Output Industrial Fuel Use by Fuel[biomass if]; Output Industrial Fuel Use by Fuel[petroleum diesel if]; Output Industrial Fuel Use by Fuel[natural gas if]; Output Industrial Fuel Use by Fuel[coal if]; Output Industrial Fuel Use by Fuel[electricity if]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Coal</t>
-  </si>
-  <si>
-    <t>Output Fuel Costs per Unit Energy by Sector[ coal,district heating sector]; Output Fuel Costs per Unit Energy by Sector[ coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[ coal,industry sector]</t>
   </si>
   <si>
     <t>Energy Related CO2 Emissions from Petroleum Fuels; Energy Related CO2 Emissions by Fuel[natural gas]; Energy Related CO2 Emissions by Fuel[lignite]; Energy Related CO2 Emissions by Fuel[ coal]</t>
@@ -4394,6 +4388,18 @@
   </si>
   <si>
     <t xml:space="preserve">**Description:** This policy causes grid-scale electricity storage from chemical batteries to grow at the specified percentage, annually, above the amount predicted in the BAU Scenario. // **Guidance for setting values:** Reflecting the latest planning work done by state energy agencies to support reaching the 60% renewable electricity goal, the BAU scenario builds to a level of 12,400 MW of battery storage in 2030. </t>
+  </si>
+  <si>
+    <t>millions of short tons / year</t>
+  </si>
+  <si>
+    <t>Coal and Petcoke</t>
+  </si>
+  <si>
+    <t>Output Total  Coal and Petcoke Consumption</t>
+  </si>
+  <si>
+    <t>Output Fuel Costs per Unit Energy by Sector[coal,district heating sector]; Output Fuel Costs per Unit Energy by Sector[coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[coal,industry sector]</t>
   </si>
 </sst>
 </file>
@@ -5979,9 +5985,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6517,7 +6523,7 @@
         <v>495</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="Q9" s="47" t="s">
         <v>496</v>
@@ -6585,7 +6591,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="Q10" s="34" t="str">
         <f t="shared" si="5"/>
@@ -6653,7 +6659,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="Q11" s="34" t="str">
         <f t="shared" si="5"/>
@@ -7173,7 +7179,7 @@
         <v>482</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="Q21" s="47" t="s">
         <v>483</v>
@@ -7237,7 +7243,7 @@
         <v>482</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="Q22" s="51"/>
       <c r="R22" s="51"/>
@@ -7295,7 +7301,7 @@
         <v>482</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="Q23" s="51"/>
       <c r="R23" s="51"/>
@@ -7755,7 +7761,7 @@
         <v>457</v>
       </c>
       <c r="P33" s="26" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="Q33" s="26" t="s">
         <v>211</v>
@@ -7800,7 +7806,7 @@
         <v>1208</v>
       </c>
       <c r="K34" s="50" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -7845,7 +7851,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K35" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L35" s="37">
         <f>L$36</f>
@@ -7907,7 +7913,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K36" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L36" s="32">
         <v>0</v>
@@ -7922,7 +7928,7 @@
         <v>126</v>
       </c>
       <c r="P36" s="107" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="Q36" s="26" t="s">
         <v>213</v>
@@ -7931,10 +7937,10 @@
         <v>214</v>
       </c>
       <c r="S36" s="105" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="T36" s="26" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="45">
@@ -7973,7 +7979,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K37" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L37" s="37">
         <f>L$36</f>
@@ -7991,7 +7997,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P37" s="96" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="Q37" s="37" t="str">
         <f t="shared" si="13"/>
@@ -8040,7 +8046,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K38" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L38" s="37">
         <f>L$36</f>
@@ -8059,7 +8065,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P38" s="96" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="12"/>
@@ -8100,7 +8106,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K39" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
@@ -8146,7 +8152,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K40" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
@@ -8191,7 +8197,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K41" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L41" s="34">
         <v>0</v>
@@ -8206,7 +8212,7 @@
         <v>126</v>
       </c>
       <c r="P41" s="96" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="Q41" s="28"/>
       <c r="R41" s="28"/>
@@ -8249,7 +8255,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K42" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L42" s="34">
         <f>L$36</f>
@@ -8267,7 +8273,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P42" s="108" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="Q42" s="28" t="str">
         <f>Q$36</f>
@@ -8316,7 +8322,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K43" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L43" s="34">
         <f>L$36</f>
@@ -8334,7 +8340,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P43" s="108" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="Q43" s="28" t="str">
         <f>Q$36</f>
@@ -8385,7 +8391,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K44" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="35"/>
@@ -8431,7 +8437,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K45" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="35"/>
@@ -8477,7 +8483,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K46" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -8520,7 +8526,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K47" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="36"/>
@@ -8566,7 +8572,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K48" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L48" s="34"/>
       <c r="M48" s="36"/>
@@ -8612,7 +8618,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K49" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L49" s="34"/>
       <c r="M49" s="36"/>
@@ -8658,7 +8664,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K50" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L50" s="34"/>
       <c r="M50" s="36"/>
@@ -8706,14 +8712,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K51" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L51" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M51" s="36" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="N51" s="34">
         <f>N$36</f>
@@ -8775,7 +8781,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K52" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
@@ -8818,7 +8824,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K53" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L53" s="34"/>
       <c r="M53" s="36"/>
@@ -8864,7 +8870,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K54" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L54" s="34"/>
       <c r="M54" s="36"/>
@@ -8910,7 +8916,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K55" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L55" s="34"/>
       <c r="M55" s="36"/>
@@ -8956,7 +8962,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K56" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L56" s="34"/>
       <c r="M56" s="36"/>
@@ -9004,14 +9010,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K57" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L57" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M57" s="36" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="N57" s="34">
         <f>N$36</f>
@@ -9073,7 +9079,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K58" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
@@ -9116,7 +9122,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K59" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L59" s="34"/>
       <c r="M59" s="36"/>
@@ -9162,7 +9168,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K60" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L60" s="34"/>
       <c r="M60" s="36"/>
@@ -9208,7 +9214,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K61" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="36"/>
@@ -9254,7 +9260,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K62" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="36"/>
@@ -9302,14 +9308,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K63" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L63" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M63" s="36" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="N63" s="34">
         <f>N$36</f>
@@ -9371,7 +9377,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K64" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -9414,7 +9420,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K65" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L65" s="34"/>
       <c r="M65" s="36"/>
@@ -9462,14 +9468,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K66" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L66" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M66" s="36" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="N66" s="34">
         <f>N$36</f>
@@ -9531,7 +9537,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K67" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L67" s="34"/>
       <c r="M67" s="36"/>
@@ -9577,7 +9583,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K68" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L68" s="34"/>
       <c r="M68" s="36"/>
@@ -9623,7 +9629,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K69" s="64" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="L69" s="34"/>
       <c r="M69" s="36"/>
@@ -9674,7 +9680,7 @@
         <v>501</v>
       </c>
       <c r="P70" s="26" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="Q70" s="26" t="s">
         <v>502</v>
@@ -9732,7 +9738,7 @@
         <v>40</v>
       </c>
       <c r="P71" s="107" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="Q71" s="26" t="s">
         <v>215</v>
@@ -9796,7 +9802,7 @@
         <v>% of TDM package implemented</v>
       </c>
       <c r="P72" s="107" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="Q72" s="31" t="str">
         <f t="shared" si="18"/>
@@ -9855,7 +9861,7 @@
         <v>128</v>
       </c>
       <c r="P73" s="26" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="Q73" s="26" t="s">
         <v>217</v>
@@ -9917,7 +9923,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q74" s="31" t="str">
         <f t="shared" si="21"/>
@@ -9981,7 +9987,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P75" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q75" s="31" t="str">
         <f t="shared" si="21"/>
@@ -10041,7 +10047,7 @@
         <v>34</v>
       </c>
       <c r="P76" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q76" s="26" t="s">
         <v>219</v>
@@ -10110,7 +10116,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P77" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q77" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10187,7 +10193,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P78" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q78" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10264,7 +10270,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P79" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q79" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10341,7 +10347,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P80" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q80" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10418,7 +10424,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P81" s="26" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="Q81" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11416,7 +11422,7 @@
         <v>31</v>
       </c>
       <c r="P94" s="26" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="Q94" s="26" t="s">
         <v>221</v>
@@ -11469,7 +11475,7 @@
         <v>296</v>
       </c>
       <c r="P95" s="26" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="Q95" s="26" t="s">
         <v>297</v>
@@ -11478,7 +11484,7 @@
         <v>298</v>
       </c>
       <c r="S95" s="12" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="T95" s="12" t="s">
         <v>436</v>
@@ -11532,7 +11538,7 @@
         <v>301</v>
       </c>
       <c r="S96" s="101" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="T96" s="28"/>
     </row>
@@ -11560,7 +11566,7 @@
         <v>1166</v>
       </c>
       <c r="K97" s="72" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="L97" s="38">
         <v>0</v>
@@ -13070,7 +13076,7 @@
         <v>37</v>
       </c>
       <c r="P125" s="26" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="Q125" s="26" t="s">
         <v>229</v>
@@ -13079,10 +13085,10 @@
         <v>230</v>
       </c>
       <c r="S125" s="105" t="s">
+        <v>1319</v>
+      </c>
+      <c r="T125" s="26" t="s">
         <v>1321</v>
-      </c>
-      <c r="T125" s="26" t="s">
-        <v>1323</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="57" customHeight="1">
@@ -13678,7 +13684,7 @@
         <v>32</v>
       </c>
       <c r="P138" s="26" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="Q138" s="26" t="s">
         <v>233</v>
@@ -13687,7 +13693,7 @@
         <v>234</v>
       </c>
       <c r="S138" s="5" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="T138" s="26" t="s">
         <v>186</v>
@@ -13723,7 +13729,7 @@
         <v>0</v>
       </c>
       <c r="M139" s="32" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="N139" s="32">
         <v>0.01</v>
@@ -13732,7 +13738,7 @@
         <v>148</v>
       </c>
       <c r="P139" s="26" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="Q139" s="26" t="s">
         <v>235</v>
@@ -15702,7 +15708,7 @@
         <v>285</v>
       </c>
       <c r="P182" s="26" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="Q182" s="12" t="s">
         <v>548</v>
@@ -15711,7 +15717,7 @@
         <v>286</v>
       </c>
       <c r="S182" s="105" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="T182" s="12"/>
     </row>
@@ -15720,7 +15726,7 @@
         <v>7</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C183" s="26" t="s">
         <v>344</v>
@@ -15736,7 +15742,7 @@
         <v>49</v>
       </c>
       <c r="J183" s="50" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="K183" s="50" t="s">
         <v>610</v>
@@ -15754,7 +15760,7 @@
         <v>38</v>
       </c>
       <c r="P183" s="26" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="Q183" s="26" t="s">
         <v>238</v>
@@ -16359,7 +16365,7 @@
         <v>37</v>
       </c>
       <c r="P194" s="26" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="Q194" s="26" t="s">
         <v>242</v>
@@ -16519,7 +16525,7 @@
         <v>34</v>
       </c>
       <c r="P197" s="103" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="Q197" s="26" t="s">
         <v>248</v>
@@ -16531,7 +16537,7 @@
         <v>561</v>
       </c>
       <c r="T197" s="105" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="198" spans="1:20" s="6" customFormat="1" ht="60">
@@ -16584,7 +16590,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P198" s="26" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="Q198" s="26" t="s">
         <v>248</v>
@@ -16652,7 +16658,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P199" s="26" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="Q199" s="26" t="s">
         <v>248</v>
@@ -16720,7 +16726,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P200" s="26" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="Q200" s="26" t="s">
         <v>248</v>
@@ -16788,7 +16794,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P201" s="26" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="Q201" s="26" t="s">
         <v>248</v>
@@ -16922,7 +16928,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P203" s="26" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="Q203" s="26" t="s">
         <v>248</v>
@@ -16990,7 +16996,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P204" s="26" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="Q204" s="26" t="s">
         <v>248</v>
@@ -17096,7 +17102,7 @@
         <v>33</v>
       </c>
       <c r="P206" s="26" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="Q206" s="26" t="s">
         <v>252</v>
@@ -17114,7 +17120,7 @@
         <v>8</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C207" s="26" t="s">
         <v>362</v>
@@ -17148,7 +17154,7 @@
         <v>363</v>
       </c>
       <c r="P207" s="26" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="Q207" s="26" t="s">
         <v>252</v>
@@ -17157,10 +17163,10 @@
         <v>253</v>
       </c>
       <c r="S207" s="54" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="T207" s="106" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="208" spans="1:20" ht="90">
@@ -17964,7 +17970,7 @@
         <v>37</v>
       </c>
       <c r="P223" s="26" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="Q223" s="26" t="s">
         <v>272</v>
@@ -17973,7 +17979,7 @@
         <v>273</v>
       </c>
       <c r="S223" s="54" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="T223" s="26"/>
     </row>
@@ -18020,7 +18026,7 @@
         <v>172</v>
       </c>
       <c r="P224" s="26" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="Q224" s="26" t="s">
         <v>274</v>
@@ -18086,7 +18092,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P225" s="26" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="Q225" s="28" t="str">
         <f t="shared" ref="Q225:R229" si="63">Q$224</f>
@@ -18150,7 +18156,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P226" s="26" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="Q226" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18214,7 +18220,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P227" s="26" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="Q227" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18278,7 +18284,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P228" s="26" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="Q228" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18482,7 +18488,7 @@
         <v>175</v>
       </c>
       <c r="P232" s="12" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="Q232" s="12" t="s">
         <v>278</v>
@@ -18546,7 +18552,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P233" s="12" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="Q233" s="12" t="s">
         <v>278</v>
@@ -18610,7 +18616,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P234" s="12" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>278</v>
@@ -18762,7 +18768,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P237" s="12" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="Q237" s="12" t="s">
         <v>278</v>
@@ -20034,7 +20040,7 @@
         <v>35</v>
       </c>
       <c r="P263" s="26" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="Q263" s="26" t="s">
         <v>282</v>
@@ -20098,7 +20104,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P264" s="26" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="Q264" s="26" t="s">
         <v>282</v>
@@ -20162,7 +20168,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P265" s="26" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="Q265" s="26" t="s">
         <v>282</v>
@@ -20226,7 +20232,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P266" s="26" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="Q266" s="26" t="s">
         <v>282</v>
@@ -20290,7 +20296,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P267" s="26" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="Q267" s="26" t="s">
         <v>282</v>
@@ -20354,7 +20360,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P268" s="26" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="Q268" s="26" t="s">
         <v>282</v>
@@ -20411,7 +20417,7 @@
         <v>35</v>
       </c>
       <c r="P269" s="12" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="Q269" s="26" t="s">
         <v>282</v>
@@ -20469,7 +20475,7 @@
         <v>35</v>
       </c>
       <c r="P270" s="12" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="Q270" s="26" t="s">
         <v>282</v>
@@ -20533,7 +20539,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P271" s="12" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="Q271" s="26" t="s">
         <v>282</v>
@@ -20597,7 +20603,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P272" s="12" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="Q272" s="26" t="s">
         <v>282</v>
@@ -20661,7 +20667,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P273" s="12" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="Q273" s="26" t="s">
         <v>282</v>
@@ -20725,7 +20731,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P274" s="12" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="Q274" s="26" t="s">
         <v>282</v>
@@ -20789,7 +20795,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P275" s="12" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="Q275" s="26" t="s">
         <v>282</v>
@@ -20853,7 +20859,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P276" s="12" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="Q276" s="26" t="s">
         <v>282</v>
@@ -20917,7 +20923,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P277" s="12" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="Q277" s="26" t="s">
         <v>282</v>
@@ -20981,7 +20987,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P278" s="12" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="Q278" s="26" t="s">
         <v>282</v>
@@ -21045,7 +21051,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P279" s="12" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="Q279" s="26" t="s">
         <v>282</v>
@@ -21109,7 +21115,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P280" s="12" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="Q280" s="26" t="s">
         <v>282</v>
@@ -21167,7 +21173,7 @@
         <v>35</v>
       </c>
       <c r="P281" s="12" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="Q281" s="26" t="s">
         <v>282</v>
@@ -21231,7 +21237,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P282" s="12" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="Q282" s="26" t="s">
         <v>282</v>
@@ -21295,7 +21301,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P283" s="12" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="Q283" s="26" t="s">
         <v>282</v>
@@ -21359,7 +21365,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P284" s="12" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="Q284" s="26" t="s">
         <v>282</v>
@@ -21423,7 +21429,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P285" s="12" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="Q285" s="26" t="s">
         <v>282</v>
@@ -21487,7 +21493,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P286" s="12" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="Q286" s="26" t="s">
         <v>282</v>
@@ -21551,7 +21557,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P287" s="12" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="Q287" s="26" t="s">
         <v>282</v>
@@ -21615,7 +21621,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P288" s="12" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="Q288" s="26" t="s">
         <v>282</v>
@@ -21673,7 +21679,7 @@
         <v>35</v>
       </c>
       <c r="P289" s="12" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="Q289" s="26" t="s">
         <v>282</v>
@@ -21737,7 +21743,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P290" s="12" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="Q290" s="26" t="s">
         <v>282</v>
@@ -21801,7 +21807,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P291" s="12" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="Q291" s="26" t="s">
         <v>282</v>
@@ -21865,7 +21871,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P292" s="12" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="Q292" s="26" t="s">
         <v>282</v>
@@ -21929,7 +21935,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P293" s="12" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="Q293" s="26" t="s">
         <v>282</v>
@@ -21993,7 +21999,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P294" s="12" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="Q294" s="26" t="s">
         <v>282</v>
@@ -22049,7 +22055,7 @@
         <v>36</v>
       </c>
       <c r="P295" s="26" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="Q295" s="26" t="s">
         <v>282</v>
@@ -22113,7 +22119,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P296" s="26" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="Q296" s="26" t="s">
         <v>282</v>
@@ -22219,7 +22225,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P298" s="26" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="Q298" s="26" t="s">
         <v>282</v>
@@ -22283,7 +22289,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P299" s="26" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="Q299" s="26" t="s">
         <v>282</v>
@@ -22347,7 +22353,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P300" s="26" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="Q300" s="26" t="s">
         <v>282</v>
@@ -22403,7 +22409,7 @@
         <v>36</v>
       </c>
       <c r="P301" s="26" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="Q301" s="26" t="s">
         <v>282</v>
@@ -22461,7 +22467,7 @@
         <v>36</v>
       </c>
       <c r="P302" s="26" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="Q302" s="26" t="s">
         <v>282</v>
@@ -22525,7 +22531,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P303" s="26" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="Q303" s="26" t="s">
         <v>282</v>
@@ -22589,7 +22595,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P304" s="26" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="Q304" s="26" t="s">
         <v>282</v>
@@ -22829,7 +22835,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P309" s="26" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="Q309" s="26" t="s">
         <v>282</v>
@@ -22893,7 +22899,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P310" s="26" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="Q310" s="26" t="s">
         <v>282</v>
@@ -22957,7 +22963,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P311" s="26" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="Q311" s="26" t="s">
         <v>282</v>
@@ -23057,7 +23063,7 @@
         <v>36</v>
       </c>
       <c r="P313" s="26" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="Q313" s="26" t="s">
         <v>282</v>
@@ -23121,7 +23127,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P314" s="26" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="Q314" s="26" t="s">
         <v>282</v>
@@ -23185,7 +23191,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P315" s="26" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="Q315" s="26" t="s">
         <v>282</v>
@@ -23249,7 +23255,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P316" s="26" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="Q316" s="26" t="s">
         <v>282</v>
@@ -23313,7 +23319,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P317" s="26" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="Q317" s="26" t="s">
         <v>282</v>
@@ -23377,7 +23383,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P318" s="26" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="Q318" s="26" t="s">
         <v>282</v>
@@ -23441,7 +23447,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P319" s="26" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="Q319" s="26" t="s">
         <v>282</v>
@@ -23505,7 +23511,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P320" s="26" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="Q320" s="26" t="s">
         <v>282</v>
@@ -23563,7 +23569,7 @@
         <v>36</v>
       </c>
       <c r="P321" s="26" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="Q321" s="26" t="s">
         <v>282</v>
@@ -23627,7 +23633,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P322" s="26" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="Q322" s="26" t="s">
         <v>282</v>
@@ -23691,7 +23697,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P323" s="26" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="Q323" s="26" t="s">
         <v>282</v>
@@ -23755,7 +23761,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P324" s="26" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="Q324" s="26" t="s">
         <v>282</v>
@@ -23819,7 +23825,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P325" s="26" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="Q325" s="26" t="s">
         <v>282</v>
@@ -23883,7 +23889,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P326" s="26" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="Q326" s="26" t="s">
         <v>282</v>
@@ -24035,11 +24041,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24521,10 +24527,10 @@
         <v>422</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="H21" s="72" t="s">
         <v>755</v>
@@ -24575,7 +24581,7 @@
         <v>427</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C24" s="72" t="s">
         <v>74</v>
@@ -24587,7 +24593,7 @@
         <v>1131</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="H24" s="72"/>
     </row>
@@ -24648,7 +24654,7 @@
         <v>713</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>74</v>
@@ -24660,13 +24666,13 @@
         <v>1132</v>
       </c>
       <c r="F27" s="52" t="s">
+        <v>1259</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>1260</v>
+      </c>
+      <c r="H27" s="72" t="s">
         <v>1261</v>
-      </c>
-      <c r="G27" s="52" t="s">
-        <v>1262</v>
-      </c>
-      <c r="H27" s="72" t="s">
-        <v>1263</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45">
@@ -24674,7 +24680,7 @@
         <v>713</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C28" s="72" t="s">
         <v>74</v>
@@ -24686,13 +24692,13 @@
         <v>1132</v>
       </c>
       <c r="F28" s="52" t="s">
+        <v>1262</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H28" s="72" t="s">
         <v>1264</v>
-      </c>
-      <c r="G28" s="52" t="s">
-        <v>1265</v>
-      </c>
-      <c r="H28" s="72" t="s">
-        <v>1266</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="90">
@@ -24712,7 +24718,7 @@
         <v>1132</v>
       </c>
       <c r="F29" s="52" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="G29" s="52" t="s">
         <v>782</v>
@@ -24780,10 +24786,10 @@
         <v>424</v>
       </c>
       <c r="F32" s="72" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="H32" s="72" t="s">
         <v>669</v>
@@ -24806,10 +24812,10 @@
         <v>424</v>
       </c>
       <c r="F33" s="72" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="H33" s="72" t="s">
         <v>670</v>
@@ -24832,10 +24838,10 @@
         <v>425</v>
       </c>
       <c r="F34" s="72" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="G34" s="52" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="H34" s="72" t="s">
         <v>476</v>
@@ -24858,10 +24864,10 @@
         <v>425</v>
       </c>
       <c r="F35" s="72" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="H35" s="72" t="s">
         <v>477</v>
@@ -25355,7 +25361,7 @@
         <v>1241</v>
       </c>
       <c r="G54" s="104" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="H54" s="72" t="s">
         <v>1210</v>
@@ -25534,13 +25540,13 @@
         <v>479</v>
       </c>
       <c r="F61" s="72" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="G61" s="52" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="H61" s="72" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -25569,7 +25575,7 @@
         <v>454</v>
       </c>
       <c r="B63" s="73" t="s">
-        <v>99</v>
+        <v>1391</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>72</v>
@@ -25578,10 +25584,10 @@
         <v>73</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>784</v>
+        <v>1390</v>
       </c>
       <c r="F63" s="72" t="s">
-        <v>677</v>
+        <v>1392</v>
       </c>
       <c r="H63" s="72"/>
     </row>
@@ -25590,7 +25596,7 @@
         <v>454</v>
       </c>
       <c r="B64" s="73" t="s">
-        <v>674</v>
+        <v>99</v>
       </c>
       <c r="C64" s="72" t="s">
         <v>72</v>
@@ -25599,10 +25605,10 @@
         <v>73</v>
       </c>
       <c r="E64" s="71" t="s">
-        <v>675</v>
+        <v>784</v>
       </c>
       <c r="F64" s="72" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="H64" s="72"/>
     </row>
@@ -25611,7 +25617,7 @@
         <v>454</v>
       </c>
       <c r="B65" s="73" t="s">
-        <v>744</v>
+        <v>674</v>
       </c>
       <c r="C65" s="72" t="s">
         <v>72</v>
@@ -25623,42 +25629,37 @@
         <v>675</v>
       </c>
       <c r="F65" s="72" t="s">
+        <v>676</v>
+      </c>
+      <c r="H65" s="72"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="73" t="s">
+        <v>454</v>
+      </c>
+      <c r="B66" s="73" t="s">
+        <v>744</v>
+      </c>
+      <c r="C66" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" s="71" t="s">
+        <v>675</v>
+      </c>
+      <c r="F66" s="72" t="s">
         <v>785</v>
       </c>
-      <c r="H65" s="72"/>
-    </row>
-    <row r="66" spans="1:8" ht="60">
-      <c r="A66" s="75" t="s">
-        <v>745</v>
-      </c>
-      <c r="B66" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="C66" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="D66" s="72" t="s">
-        <v>757</v>
-      </c>
-      <c r="E66" s="72" t="s">
-        <v>1133</v>
-      </c>
-      <c r="F66" s="72" t="s">
-        <v>786</v>
-      </c>
-      <c r="G66" s="52" t="s">
-        <v>787</v>
-      </c>
-      <c r="H66" s="72" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="45">
+      <c r="H66" s="72"/>
+    </row>
+    <row r="67" spans="1:8" ht="60">
       <c r="A67" s="75" t="s">
         <v>745</v>
       </c>
       <c r="B67" s="73" t="s">
-        <v>1242</v>
+        <v>105</v>
       </c>
       <c r="C67" s="72" t="s">
         <v>74</v>
@@ -25667,24 +25668,24 @@
         <v>757</v>
       </c>
       <c r="E67" s="72" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="F67" s="72" t="s">
-        <v>1243</v>
+        <v>786</v>
       </c>
       <c r="G67" s="52" t="s">
-        <v>1101</v>
+        <v>787</v>
       </c>
       <c r="H67" s="72" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="75">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="45">
       <c r="A68" s="75" t="s">
         <v>745</v>
       </c>
       <c r="B68" s="73" t="s">
-        <v>99</v>
+        <v>949</v>
       </c>
       <c r="C68" s="72" t="s">
         <v>74</v>
@@ -25693,24 +25694,24 @@
         <v>757</v>
       </c>
       <c r="E68" s="72" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="F68" s="72" t="s">
-        <v>790</v>
+        <v>1393</v>
       </c>
       <c r="G68" s="52" t="s">
-        <v>789</v>
+        <v>1101</v>
       </c>
       <c r="H68" s="72" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="75">
       <c r="A69" s="75" t="s">
         <v>745</v>
       </c>
       <c r="B69" s="73" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C69" s="72" t="s">
         <v>74</v>
@@ -25719,24 +25720,24 @@
         <v>757</v>
       </c>
       <c r="E69" s="72" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F69" s="72" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="G69" s="52" t="s">
-        <v>402</v>
-      </c>
-      <c r="H69" s="27">
-        <v>969696</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="45">
+        <v>789</v>
+      </c>
+      <c r="H69" s="72" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="75" t="s">
         <v>745</v>
       </c>
       <c r="B70" s="73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" s="72" t="s">
         <v>74</v>
@@ -25748,89 +25749,94 @@
         <v>1136</v>
       </c>
       <c r="F70" s="72" t="s">
+        <v>792</v>
+      </c>
+      <c r="G70" s="52" t="s">
+        <v>402</v>
+      </c>
+      <c r="H70" s="27">
+        <v>969696</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="45">
+      <c r="A71" s="75" t="s">
+        <v>745</v>
+      </c>
+      <c r="B71" s="73" t="s">
+        <v>108</v>
+      </c>
+      <c r="C71" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" s="72" t="s">
+        <v>757</v>
+      </c>
+      <c r="E71" s="72" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F71" s="72" t="s">
         <v>1105</v>
       </c>
-      <c r="G70" s="52" t="s">
+      <c r="G71" s="52" t="s">
         <v>1106</v>
       </c>
-      <c r="H70" s="72" t="s">
+      <c r="H71" s="72" t="s">
         <v>1107</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="30">
-      <c r="A71" s="75" t="s">
-        <v>746</v>
-      </c>
-      <c r="B71" s="73" t="s">
-        <v>747</v>
-      </c>
-      <c r="C71" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="E71" s="72" t="s">
-        <v>1137</v>
-      </c>
-      <c r="F71" s="72" t="s">
-        <v>793</v>
-      </c>
-      <c r="H71" s="72"/>
     </row>
     <row r="72" spans="1:8" ht="30">
       <c r="A72" s="75" t="s">
         <v>746</v>
       </c>
       <c r="B72" s="73" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C72" s="72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D72" s="72" t="s">
         <v>73</v>
       </c>
       <c r="E72" s="72" t="s">
-        <v>1239</v>
+        <v>1137</v>
       </c>
       <c r="F72" s="72" t="s">
-        <v>797</v>
-      </c>
-      <c r="G72" s="52" t="s">
-        <v>798</v>
-      </c>
-      <c r="H72" s="72" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>793</v>
+      </c>
+      <c r="H72" s="72"/>
+    </row>
+    <row r="73" spans="1:8" ht="30">
       <c r="A73" s="75" t="s">
         <v>746</v>
       </c>
       <c r="B73" s="73" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C73" s="72" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D73" s="72" t="s">
         <v>73</v>
       </c>
       <c r="E73" s="72" t="s">
-        <v>1138</v>
+        <v>1239</v>
       </c>
       <c r="F73" s="72" t="s">
-        <v>794</v>
-      </c>
-      <c r="H73" s="72"/>
+        <v>797</v>
+      </c>
+      <c r="G73" s="52" t="s">
+        <v>798</v>
+      </c>
+      <c r="H73" s="72" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="75" t="s">
         <v>746</v>
       </c>
       <c r="B74" s="73" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C74" s="72" t="s">
         <v>72</v>
@@ -25842,7 +25848,7 @@
         <v>1138</v>
       </c>
       <c r="F74" s="72" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H74" s="72"/>
     </row>
@@ -25851,7 +25857,7 @@
         <v>746</v>
       </c>
       <c r="B75" s="73" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C75" s="72" t="s">
         <v>72</v>
@@ -25863,9 +25869,30 @@
         <v>1138</v>
       </c>
       <c r="F75" s="72" t="s">
+        <v>795</v>
+      </c>
+      <c r="H75" s="72"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="75" t="s">
+        <v>746</v>
+      </c>
+      <c r="B76" s="73" t="s">
+        <v>751</v>
+      </c>
+      <c r="C76" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" s="72" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" s="72" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F76" s="72" t="s">
         <v>796</v>
       </c>
-      <c r="H75" s="72"/>
+      <c r="H76" s="72"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -25915,18 +25942,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work on aligning output graph data series with series that actually contain data
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -3450,25 +3450,10 @@
     <t>reduce-soft-costs.html</t>
   </si>
   <si>
-    <t>District Heating Sector, Electricity Sector, Industry Sector</t>
-  </si>
-  <si>
-    <t>620e7a, ffff00, 969696</t>
-  </si>
-  <si>
     <t>trillion passenger-miles / year</t>
   </si>
   <si>
     <t>trillion freight ton-miles / year</t>
-  </si>
-  <si>
-    <t>Output Fuel Costs per Unit Energy by Sector[petroleum diesel,electricity sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,transportation sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,industry sector]</t>
-  </si>
-  <si>
-    <t>Electricity Sector, Transportation Sector, Industry Sector</t>
-  </si>
-  <si>
-    <t>ffff00, c01b00, 969696</t>
   </si>
   <si>
     <t>Output Vehicles in Millions[LDVs,freight,diesel vehicle]; Output Vehicles in Millions[LDVs,freight,gasoline vehicle]; Output Vehicles in Millions[LDVs,freight,natural gas vehicle]; Output Vehicles in Millions[LDVs,freight,battery electric vehicle]</t>
@@ -3877,9 +3862,6 @@
   </si>
   <si>
     <t>Energy Related CO2 Emissions from Petroleum Fuels; Energy Related CO2 Emissions by Fuel[natural gas]; Energy Related CO2 Emissions by Fuel[lignite]; Energy Related CO2 Emissions by Fuel[ coal]</t>
-  </si>
-  <si>
-    <t>Petroleum, Natural Gas, Lignite,  Coal</t>
   </si>
   <si>
     <t>Output Electricity Generation by Type[geothermal es]; Output Electricity Generation by Type[biomass es]; Output Electricity Generation by Type[solar thermal es]; Output Distributed Solar PV Output; Output Electricity Generation by Type[solar PV es]; Output Electricity Generation by Type[onshore wind es]; Output Electricity Generation by Type[offshore wind es]; Output Electricity Generation by Type[hydro es]; Output Electricity Generation by Type[nuclear es]; Output Non Solar Distributed Output; Output Electricity Generation by Type[petroleum es]; Output Electricity Generation by Type[natural gas peaker es]; Output Electricity Generation by Type[natural gas nonpeaker es]; Output Electricity Generation by Type[lignite es]; Output Electricity Generation by Type[ coal es]; Output Net Imports of Electricity</t>
@@ -4399,7 +4381,25 @@
     <t>Output Total  Coal and Petcoke Consumption</t>
   </si>
   <si>
-    <t>Output Fuel Costs per Unit Energy by Sector[coal,district heating sector]; Output Fuel Costs per Unit Energy by Sector[coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[coal,industry sector]</t>
+    <t>Output Fuel Costs per Unit Energy by Sector[coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[coal,industry sector]</t>
+  </si>
+  <si>
+    <t>Electricity Sector, Industry Sector</t>
+  </si>
+  <si>
+    <t>ffff00, 969696</t>
+  </si>
+  <si>
+    <t>Output Fuel Costs per Unit Energy by Sector[petroleum diesel,commercial buildings sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,residential buildings sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,electricity sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,transportation sector]; Output Fuel Costs per Unit Energy by Sector[petroleum diesel,industry sector]</t>
+  </si>
+  <si>
+    <t>Commercial Buildings Sector, Residential Buildings Sector, Electricity Sector, Transportation Sector, Industry Sector</t>
+  </si>
+  <si>
+    <t>00b050, 087bf1, ffff00, c01b00, 969696</t>
+  </si>
+  <si>
+    <t>Petroleum, Natural Gas, Lignite, Hard Coal</t>
   </si>
 </sst>
 </file>
@@ -6081,10 +6081,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1182</v>
+        <v>1177</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1183</v>
+        <v>1178</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>43</v>
@@ -6099,10 +6099,10 @@
         <v>49</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L2" s="90">
         <v>0</v>
@@ -6114,16 +6114,16 @@
         <v>0.02</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>1186</v>
+        <v>1181</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>1187</v>
+        <v>1182</v>
       </c>
       <c r="Q2" s="47" t="s">
-        <v>1188</v>
+        <v>1183</v>
       </c>
       <c r="R2" s="91" t="s">
-        <v>1189</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="3" customFormat="1" ht="75">
@@ -6156,7 +6156,7 @@
         <v>Conventional Pollutant Standard</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L3" s="92">
         <f t="shared" si="1"/>
@@ -6175,7 +6175,7 @@
         <v>% reduction in emissions</v>
       </c>
       <c r="P3" s="26" t="s">
-        <v>1190</v>
+        <v>1185</v>
       </c>
       <c r="Q3" s="6" t="str">
         <f t="shared" si="1"/>
@@ -6216,7 +6216,7 @@
         <v>Conventional Pollutant Standard</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L4" s="92">
         <f t="shared" si="1"/>
@@ -6235,7 +6235,7 @@
         <v>% reduction in emissions</v>
       </c>
       <c r="P4" s="26" t="s">
-        <v>1191</v>
+        <v>1186</v>
       </c>
       <c r="Q4" s="6" t="str">
         <f t="shared" si="1"/>
@@ -6276,7 +6276,7 @@
         <v>Conventional Pollutant Standard</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L5" s="92">
         <f t="shared" si="1"/>
@@ -6295,7 +6295,7 @@
         <v>% reduction in emissions</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>1192</v>
+        <v>1187</v>
       </c>
       <c r="Q5" s="6" t="str">
         <f t="shared" si="1"/>
@@ -6336,7 +6336,7 @@
         <v>Conventional Pollutant Standard</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L6" s="92">
         <f t="shared" si="1"/>
@@ -6355,7 +6355,7 @@
         <v>% reduction in emissions</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>1193</v>
+        <v>1188</v>
       </c>
       <c r="Q6" s="6" t="str">
         <f t="shared" si="1"/>
@@ -6396,7 +6396,7 @@
         <v>Conventional Pollutant Standard</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>1185</v>
+        <v>1180</v>
       </c>
       <c r="L7" s="92">
         <f t="shared" si="1"/>
@@ -6415,7 +6415,7 @@
         <v>% reduction in emissions</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>1194</v>
+        <v>1189</v>
       </c>
       <c r="Q7" s="6" t="str">
         <f t="shared" si="1"/>
@@ -6523,7 +6523,7 @@
         <v>495</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
       <c r="Q9" s="47" t="s">
         <v>496</v>
@@ -6532,7 +6532,7 @@
         <v>497</v>
       </c>
       <c r="S9" s="93" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="T9" s="12"/>
     </row>
@@ -6559,7 +6559,7 @@
         <v>95</v>
       </c>
       <c r="G10" s="73" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="H10" s="29">
         <v>197</v>
@@ -6591,7 +6591,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="Q10" s="34" t="str">
         <f t="shared" si="5"/>
@@ -6659,7 +6659,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="Q11" s="34" t="str">
         <f t="shared" si="5"/>
@@ -7073,7 +7073,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P19" s="26" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="Q19" s="34" t="str">
         <f t="shared" ref="Q19:R19" si="9">Q$9</f>
@@ -7179,7 +7179,7 @@
         <v>482</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="Q21" s="47" t="s">
         <v>483</v>
@@ -7215,7 +7215,7 @@
         <v>95</v>
       </c>
       <c r="G22" s="73" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="H22" s="76">
         <v>205</v>
@@ -7243,7 +7243,7 @@
         <v>482</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="Q22" s="51"/>
       <c r="R22" s="51"/>
@@ -7301,7 +7301,7 @@
         <v>482</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="Q23" s="51"/>
       <c r="R23" s="51"/>
@@ -7761,7 +7761,7 @@
         <v>457</v>
       </c>
       <c r="P33" s="26" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="Q33" s="26" t="s">
         <v>211</v>
@@ -7781,7 +7781,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>1207</v>
+        <v>1202</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>340</v>
@@ -7803,10 +7803,10 @@
         <v>50</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>1208</v>
+        <v>1203</v>
       </c>
       <c r="K34" s="50" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -7851,7 +7851,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K35" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L35" s="37">
         <f>L$36</f>
@@ -7870,7 +7870,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P35" s="96" t="s">
-        <v>1209</v>
+        <v>1204</v>
       </c>
       <c r="Q35" s="26"/>
       <c r="R35" s="12"/>
@@ -7913,7 +7913,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K36" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L36" s="32">
         <v>0</v>
@@ -7928,7 +7928,7 @@
         <v>126</v>
       </c>
       <c r="P36" s="107" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
       <c r="Q36" s="26" t="s">
         <v>213</v>
@@ -7937,10 +7937,10 @@
         <v>214</v>
       </c>
       <c r="S36" s="105" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="T36" s="26" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="45">
@@ -7966,7 +7966,7 @@
         <v>556</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>1115</v>
+        <v>1110</v>
       </c>
       <c r="H37" s="27">
         <v>199</v>
@@ -7979,7 +7979,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K37" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L37" s="37">
         <f>L$36</f>
@@ -7997,7 +7997,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P37" s="96" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="Q37" s="37" t="str">
         <f t="shared" si="13"/>
@@ -8046,7 +8046,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K38" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L38" s="37">
         <f>L$36</f>
@@ -8065,7 +8065,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P38" s="96" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="12"/>
@@ -8106,7 +8106,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K39" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
@@ -8152,7 +8152,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K40" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
@@ -8197,7 +8197,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K41" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L41" s="34">
         <v>0</v>
@@ -8212,7 +8212,7 @@
         <v>126</v>
       </c>
       <c r="P41" s="96" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="Q41" s="28"/>
       <c r="R41" s="28"/>
@@ -8255,7 +8255,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K42" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L42" s="34">
         <f>L$36</f>
@@ -8273,7 +8273,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P42" s="108" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="Q42" s="28" t="str">
         <f>Q$36</f>
@@ -8322,7 +8322,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K43" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L43" s="34">
         <f>L$36</f>
@@ -8340,7 +8340,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P43" s="108" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q43" s="28" t="str">
         <f>Q$36</f>
@@ -8391,7 +8391,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K44" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="35"/>
@@ -8437,7 +8437,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K45" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="35"/>
@@ -8483,7 +8483,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K46" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -8526,7 +8526,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K47" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="36"/>
@@ -8572,7 +8572,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K48" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L48" s="34"/>
       <c r="M48" s="36"/>
@@ -8618,7 +8618,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K49" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L49" s="34"/>
       <c r="M49" s="36"/>
@@ -8664,7 +8664,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K50" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L50" s="34"/>
       <c r="M50" s="36"/>
@@ -8712,14 +8712,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K51" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L51" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M51" s="36" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N51" s="34">
         <f>N$36</f>
@@ -8730,7 +8730,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P51" s="26" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
       <c r="Q51" s="28" t="str">
         <f>Q$36</f>
@@ -8781,7 +8781,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K52" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
@@ -8824,7 +8824,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K53" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L53" s="34"/>
       <c r="M53" s="36"/>
@@ -8870,7 +8870,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K54" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L54" s="34"/>
       <c r="M54" s="36"/>
@@ -8916,7 +8916,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K55" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L55" s="34"/>
       <c r="M55" s="36"/>
@@ -8962,7 +8962,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K56" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L56" s="34"/>
       <c r="M56" s="36"/>
@@ -9010,14 +9010,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K57" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L57" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M57" s="36" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N57" s="34">
         <f>N$36</f>
@@ -9028,7 +9028,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P57" s="26" t="s">
-        <v>1171</v>
+        <v>1166</v>
       </c>
       <c r="Q57" s="28" t="str">
         <f>Q$36</f>
@@ -9079,7 +9079,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K58" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
@@ -9122,7 +9122,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K59" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L59" s="34"/>
       <c r="M59" s="36"/>
@@ -9168,7 +9168,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K60" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L60" s="34"/>
       <c r="M60" s="36"/>
@@ -9214,7 +9214,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K61" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="36"/>
@@ -9260,7 +9260,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K62" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="36"/>
@@ -9308,14 +9308,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K63" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L63" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M63" s="36" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N63" s="34">
         <f>N$36</f>
@@ -9326,7 +9326,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P63" s="26" t="s">
-        <v>1170</v>
+        <v>1165</v>
       </c>
       <c r="Q63" s="28" t="str">
         <f>Q$36</f>
@@ -9377,7 +9377,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K64" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -9420,7 +9420,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K65" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L65" s="34"/>
       <c r="M65" s="36"/>
@@ -9468,14 +9468,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K66" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L66" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M66" s="36" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N66" s="34">
         <f>N$36</f>
@@ -9486,7 +9486,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P66" s="26" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
       <c r="Q66" s="28" t="str">
         <f>Q$36</f>
@@ -9537,7 +9537,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K67" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L67" s="34"/>
       <c r="M67" s="36"/>
@@ -9583,7 +9583,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K68" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L68" s="34"/>
       <c r="M68" s="36"/>
@@ -9629,7 +9629,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K69" s="64" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="L69" s="34"/>
       <c r="M69" s="36"/>
@@ -9680,7 +9680,7 @@
         <v>501</v>
       </c>
       <c r="P70" s="26" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="Q70" s="26" t="s">
         <v>502</v>
@@ -9692,7 +9692,7 @@
         <v>504</v>
       </c>
       <c r="T70" s="12" t="s">
-        <v>1204</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="71" spans="1:20" ht="60">
@@ -9738,7 +9738,7 @@
         <v>40</v>
       </c>
       <c r="P71" s="107" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="Q71" s="26" t="s">
         <v>215</v>
@@ -9802,7 +9802,7 @@
         <v>% of TDM package implemented</v>
       </c>
       <c r="P72" s="107" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="Q72" s="31" t="str">
         <f t="shared" si="18"/>
@@ -9861,7 +9861,7 @@
         <v>128</v>
       </c>
       <c r="P73" s="26" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="Q73" s="26" t="s">
         <v>217</v>
@@ -9923,7 +9923,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q74" s="31" t="str">
         <f t="shared" si="21"/>
@@ -9987,7 +9987,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P75" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q75" s="31" t="str">
         <f t="shared" si="21"/>
@@ -10047,7 +10047,7 @@
         <v>34</v>
       </c>
       <c r="P76" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q76" s="26" t="s">
         <v>219</v>
@@ -10116,7 +10116,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P77" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q77" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10193,7 +10193,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P78" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q78" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10270,7 +10270,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P79" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q79" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10347,7 +10347,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P80" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q80" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10424,7 +10424,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P81" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="Q81" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10502,7 +10502,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P82" s="26" t="s">
-        <v>1154</v>
+        <v>1149</v>
       </c>
       <c r="Q82" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10580,7 +10580,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P83" s="26" t="s">
-        <v>1155</v>
+        <v>1150</v>
       </c>
       <c r="Q83" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10658,7 +10658,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P84" s="26" t="s">
-        <v>1156</v>
+        <v>1151</v>
       </c>
       <c r="Q84" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10736,7 +10736,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P85" s="26" t="s">
-        <v>1157</v>
+        <v>1152</v>
       </c>
       <c r="Q85" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10814,7 +10814,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P86" s="26" t="s">
-        <v>1158</v>
+        <v>1153</v>
       </c>
       <c r="Q86" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10892,7 +10892,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P87" s="26" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
       <c r="Q87" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10970,7 +10970,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P88" s="26" t="s">
-        <v>1160</v>
+        <v>1155</v>
       </c>
       <c r="Q88" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11048,7 +11048,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P89" s="26" t="s">
-        <v>1161</v>
+        <v>1156</v>
       </c>
       <c r="Q89" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11126,7 +11126,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P90" s="26" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="Q90" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11204,7 +11204,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P91" s="26" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="Q91" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11282,7 +11282,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P92" s="26" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="Q92" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11360,7 +11360,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P93" s="26" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="Q93" s="28" t="str">
         <f t="shared" ref="Q93:S93" si="30">Q$76</f>
@@ -11422,7 +11422,7 @@
         <v>31</v>
       </c>
       <c r="P94" s="26" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="Q94" s="26" t="s">
         <v>221</v>
@@ -11475,7 +11475,7 @@
         <v>296</v>
       </c>
       <c r="P95" s="26" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="Q95" s="26" t="s">
         <v>297</v>
@@ -11484,7 +11484,7 @@
         <v>298</v>
       </c>
       <c r="S95" s="12" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="T95" s="12" t="s">
         <v>436</v>
@@ -11538,7 +11538,7 @@
         <v>301</v>
       </c>
       <c r="S96" s="101" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
       <c r="T96" s="28"/>
     </row>
@@ -11547,7 +11547,7 @@
         <v>80</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="C97" s="26" t="s">
         <v>141</v>
@@ -11563,10 +11563,10 @@
         <v>50</v>
       </c>
       <c r="J97" s="26" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="K97" s="72" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="L97" s="38">
         <v>0</v>
@@ -11581,7 +11581,7 @@
         <v>31</v>
       </c>
       <c r="P97" s="26" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="Q97" s="26" t="s">
         <v>223</v>
@@ -11638,7 +11638,7 @@
         <v>39</v>
       </c>
       <c r="P98" s="26" t="s">
-        <v>1221</v>
+        <v>1216</v>
       </c>
       <c r="Q98" s="26" t="s">
         <v>225</v>
@@ -11705,7 +11705,7 @@
         <v>% of existing building components</v>
       </c>
       <c r="P99" s="26" t="s">
-        <v>1222</v>
+        <v>1217</v>
       </c>
       <c r="Q99" s="26" t="s">
         <v>225</v>
@@ -11771,7 +11771,7 @@
         <v>% of existing building components</v>
       </c>
       <c r="P100" s="26" t="s">
-        <v>1223</v>
+        <v>1218</v>
       </c>
       <c r="Q100" s="26" t="s">
         <v>225</v>
@@ -11835,7 +11835,7 @@
         <v>% of existing building components</v>
       </c>
       <c r="P101" s="26" t="s">
-        <v>1224</v>
+        <v>1219</v>
       </c>
       <c r="Q101" s="26" t="s">
         <v>225</v>
@@ -11900,7 +11900,7 @@
         <v>% of existing building components</v>
       </c>
       <c r="P102" s="26" t="s">
-        <v>1225</v>
+        <v>1220</v>
       </c>
       <c r="Q102" s="26" t="s">
         <v>225</v>
@@ -11965,7 +11965,7 @@
         <v>% of existing building components</v>
       </c>
       <c r="P103" s="26" t="s">
-        <v>1226</v>
+        <v>1221</v>
       </c>
       <c r="Q103" s="26" t="s">
         <v>225</v>
@@ -12936,7 +12936,7 @@
         <v>308</v>
       </c>
       <c r="P122" s="26" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
       <c r="Q122" s="26" t="s">
         <v>310</v>
@@ -12988,7 +12988,7 @@
         <v>309</v>
       </c>
       <c r="P123" s="26" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
       <c r="Q123" s="26" t="s">
         <v>311</v>
@@ -13076,7 +13076,7 @@
         <v>37</v>
       </c>
       <c r="P125" s="26" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="Q125" s="26" t="s">
         <v>229</v>
@@ -13085,10 +13085,10 @@
         <v>230</v>
       </c>
       <c r="S125" s="105" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="T125" s="26" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="57" customHeight="1">
@@ -13684,7 +13684,7 @@
         <v>32</v>
       </c>
       <c r="P138" s="26" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="Q138" s="26" t="s">
         <v>233</v>
@@ -13693,7 +13693,7 @@
         <v>234</v>
       </c>
       <c r="S138" s="5" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="T138" s="26" t="s">
         <v>186</v>
@@ -13729,7 +13729,7 @@
         <v>0</v>
       </c>
       <c r="M139" s="32" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="N139" s="32">
         <v>0.01</v>
@@ -13738,7 +13738,7 @@
         <v>148</v>
       </c>
       <c r="P139" s="26" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
       <c r="Q139" s="26" t="s">
         <v>235</v>
@@ -13758,7 +13758,7 @@
         <v>7</v>
       </c>
       <c r="B140" s="26" t="s">
-        <v>1219</v>
+        <v>1214</v>
       </c>
       <c r="C140" s="26" t="s">
         <v>144</v>
@@ -13790,16 +13790,16 @@
         <v>31</v>
       </c>
       <c r="P140" s="5" t="s">
-        <v>1220</v>
+        <v>1215</v>
       </c>
       <c r="Q140" s="26" t="s">
-        <v>1218</v>
+        <v>1213</v>
       </c>
       <c r="R140" s="98" t="s">
         <v>239</v>
       </c>
       <c r="S140" s="99" t="s">
-        <v>1217</v>
+        <v>1212</v>
       </c>
       <c r="T140" s="28"/>
     </row>
@@ -15474,7 +15474,7 @@
         <v>292</v>
       </c>
       <c r="P178" s="26" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
       <c r="Q178" s="12" t="s">
         <v>547</v>
@@ -15708,7 +15708,7 @@
         <v>285</v>
       </c>
       <c r="P182" s="26" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="Q182" s="12" t="s">
         <v>548</v>
@@ -15717,7 +15717,7 @@
         <v>286</v>
       </c>
       <c r="S182" s="105" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="T182" s="12"/>
     </row>
@@ -15726,7 +15726,7 @@
         <v>7</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="C183" s="26" t="s">
         <v>344</v>
@@ -15742,7 +15742,7 @@
         <v>49</v>
       </c>
       <c r="J183" s="50" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="K183" s="50" t="s">
         <v>610</v>
@@ -15760,7 +15760,7 @@
         <v>38</v>
       </c>
       <c r="P183" s="26" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="Q183" s="26" t="s">
         <v>238</v>
@@ -15769,7 +15769,7 @@
         <v>239</v>
       </c>
       <c r="S183" s="60" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
       <c r="T183" s="26"/>
     </row>
@@ -16365,7 +16365,7 @@
         <v>37</v>
       </c>
       <c r="P194" s="26" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="Q194" s="26" t="s">
         <v>242</v>
@@ -16417,7 +16417,7 @@
         <v>37</v>
       </c>
       <c r="P195" s="26" t="s">
-        <v>1117</v>
+        <v>1112</v>
       </c>
       <c r="Q195" s="26" t="s">
         <v>244</v>
@@ -16525,7 +16525,7 @@
         <v>34</v>
       </c>
       <c r="P197" s="103" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="Q197" s="26" t="s">
         <v>248</v>
@@ -16537,7 +16537,7 @@
         <v>561</v>
       </c>
       <c r="T197" s="105" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="198" spans="1:20" s="6" customFormat="1" ht="60">
@@ -16590,7 +16590,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P198" s="26" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="Q198" s="26" t="s">
         <v>248</v>
@@ -16658,7 +16658,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P199" s="26" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="Q199" s="26" t="s">
         <v>248</v>
@@ -16726,7 +16726,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P200" s="26" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="Q200" s="26" t="s">
         <v>248</v>
@@ -16794,7 +16794,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P201" s="26" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="Q201" s="26" t="s">
         <v>248</v>
@@ -16928,7 +16928,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P203" s="26" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="Q203" s="26" t="s">
         <v>248</v>
@@ -16996,7 +16996,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P204" s="26" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="Q204" s="26" t="s">
         <v>248</v>
@@ -17060,7 +17060,7 @@
         <v>190</v>
       </c>
       <c r="T205" s="28" t="s">
-        <v>1118</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="206" spans="1:20" ht="60">
@@ -17102,7 +17102,7 @@
         <v>33</v>
       </c>
       <c r="P206" s="26" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="Q206" s="26" t="s">
         <v>252</v>
@@ -17120,7 +17120,7 @@
         <v>8</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
       <c r="C207" s="26" t="s">
         <v>362</v>
@@ -17154,7 +17154,7 @@
         <v>363</v>
       </c>
       <c r="P207" s="26" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="Q207" s="26" t="s">
         <v>252</v>
@@ -17163,10 +17163,10 @@
         <v>253</v>
       </c>
       <c r="S207" s="54" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="T207" s="106" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="208" spans="1:20" ht="90">
@@ -17208,7 +17208,7 @@
         <v>37</v>
       </c>
       <c r="P208" s="26" t="s">
-        <v>1179</v>
+        <v>1174</v>
       </c>
       <c r="Q208" s="26" t="s">
         <v>254</v>
@@ -17226,7 +17226,7 @@
         <v>8</v>
       </c>
       <c r="B209" s="26" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
       <c r="C209" s="26" t="s">
         <v>323</v>
@@ -17260,7 +17260,7 @@
         <v>37</v>
       </c>
       <c r="P209" s="26" t="s">
-        <v>1180</v>
+        <v>1175</v>
       </c>
       <c r="Q209" s="26" t="s">
         <v>256</v>
@@ -17312,7 +17312,7 @@
         <v>37</v>
       </c>
       <c r="P210" s="26" t="s">
-        <v>1124</v>
+        <v>1119</v>
       </c>
       <c r="Q210" s="26" t="s">
         <v>565</v>
@@ -17364,7 +17364,7 @@
         <v>37</v>
       </c>
       <c r="P211" s="26" t="s">
-        <v>1125</v>
+        <v>1120</v>
       </c>
       <c r="Q211" s="26" t="s">
         <v>258</v>
@@ -17382,7 +17382,7 @@
         <v>165</v>
       </c>
       <c r="B212" s="26" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="C212" s="26" t="s">
         <v>441</v>
@@ -17398,7 +17398,7 @@
         <v>49</v>
       </c>
       <c r="J212" s="72" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="K212" s="50" t="s">
         <v>597</v>
@@ -17416,7 +17416,7 @@
         <v>37</v>
       </c>
       <c r="P212" s="26" t="s">
-        <v>1153</v>
+        <v>1148</v>
       </c>
       <c r="Q212" s="26" t="s">
         <v>260</v>
@@ -17428,7 +17428,7 @@
         <v>190</v>
       </c>
       <c r="T212" s="26" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="213" spans="1:20" ht="60">
@@ -17436,7 +17436,7 @@
         <v>165</v>
       </c>
       <c r="B213" s="26" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="C213" s="26" t="s">
         <v>449</v>
@@ -17452,7 +17452,7 @@
         <v>49</v>
       </c>
       <c r="J213" s="72" t="s">
-        <v>1119</v>
+        <v>1114</v>
       </c>
       <c r="K213" s="50" t="s">
         <v>596</v>
@@ -17470,7 +17470,7 @@
         <v>37</v>
       </c>
       <c r="P213" s="26" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
       <c r="Q213" s="26" t="s">
         <v>364</v>
@@ -17480,7 +17480,7 @@
       </c>
       <c r="S213" s="54"/>
       <c r="T213" s="26" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="214" spans="1:20" ht="30">
@@ -17524,7 +17524,7 @@
         <v>165</v>
       </c>
       <c r="B215" s="26" t="s">
-        <v>1120</v>
+        <v>1115</v>
       </c>
       <c r="C215" s="26" t="s">
         <v>442</v>
@@ -17610,7 +17610,7 @@
         <v>37</v>
       </c>
       <c r="P216" s="26" t="s">
-        <v>1181</v>
+        <v>1176</v>
       </c>
       <c r="Q216" s="26" t="s">
         <v>264</v>
@@ -17662,7 +17662,7 @@
         <v>37</v>
       </c>
       <c r="P217" s="26" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="Q217" s="26" t="s">
         <v>266</v>
@@ -17674,7 +17674,7 @@
         <v>190</v>
       </c>
       <c r="T217" s="26" t="s">
-        <v>1122</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="218" spans="1:20" ht="75">
@@ -17716,7 +17716,7 @@
         <v>37</v>
       </c>
       <c r="P218" s="26" t="s">
-        <v>1126</v>
+        <v>1121</v>
       </c>
       <c r="Q218" s="26" t="s">
         <v>268</v>
@@ -17734,7 +17734,7 @@
         <v>165</v>
       </c>
       <c r="B219" s="26" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="C219" s="26" t="s">
         <v>444</v>
@@ -17750,7 +17750,7 @@
         <v>49</v>
       </c>
       <c r="J219" s="72" t="s">
-        <v>1123</v>
+        <v>1118</v>
       </c>
       <c r="K219" s="50" t="s">
         <v>590</v>
@@ -17768,7 +17768,7 @@
         <v>37</v>
       </c>
       <c r="P219" s="26" t="s">
-        <v>1206</v>
+        <v>1201</v>
       </c>
       <c r="Q219" s="26"/>
       <c r="R219" s="12"/>
@@ -17814,7 +17814,7 @@
         <v>37</v>
       </c>
       <c r="P220" s="26" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="Q220" s="26" t="s">
         <v>270</v>
@@ -17970,7 +17970,7 @@
         <v>37</v>
       </c>
       <c r="P223" s="26" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="Q223" s="26" t="s">
         <v>272</v>
@@ -17979,7 +17979,7 @@
         <v>273</v>
       </c>
       <c r="S223" s="54" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="T223" s="26"/>
     </row>
@@ -17988,7 +17988,7 @@
         <v>9</v>
       </c>
       <c r="B224" s="26" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="C224" s="26" t="s">
         <v>25</v>
@@ -18008,7 +18008,7 @@
         <v>49</v>
       </c>
       <c r="J224" s="50" t="s">
-        <v>1127</v>
+        <v>1122</v>
       </c>
       <c r="K224" s="50" t="s">
         <v>585</v>
@@ -18026,7 +18026,7 @@
         <v>172</v>
       </c>
       <c r="P224" s="26" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="Q224" s="26" t="s">
         <v>274</v>
@@ -18092,7 +18092,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P225" s="26" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="Q225" s="28" t="str">
         <f t="shared" ref="Q225:R229" si="63">Q$224</f>
@@ -18156,7 +18156,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P226" s="26" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="Q226" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18220,7 +18220,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P227" s="26" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="Q227" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18284,7 +18284,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P228" s="26" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="Q228" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18488,7 +18488,7 @@
         <v>175</v>
       </c>
       <c r="P232" s="12" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="Q232" s="12" t="s">
         <v>278</v>
@@ -18552,7 +18552,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P233" s="12" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="Q233" s="12" t="s">
         <v>278</v>
@@ -18616,7 +18616,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P234" s="12" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>278</v>
@@ -18768,7 +18768,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P237" s="12" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="Q237" s="12" t="s">
         <v>278</v>
@@ -20040,7 +20040,7 @@
         <v>35</v>
       </c>
       <c r="P263" s="26" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="Q263" s="26" t="s">
         <v>282</v>
@@ -20104,7 +20104,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P264" s="26" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Q264" s="26" t="s">
         <v>282</v>
@@ -20168,7 +20168,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P265" s="26" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="Q265" s="26" t="s">
         <v>282</v>
@@ -20232,7 +20232,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P266" s="26" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="Q266" s="26" t="s">
         <v>282</v>
@@ -20296,7 +20296,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P267" s="26" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="Q267" s="26" t="s">
         <v>282</v>
@@ -20360,7 +20360,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P268" s="26" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="Q268" s="26" t="s">
         <v>282</v>
@@ -20417,7 +20417,7 @@
         <v>35</v>
       </c>
       <c r="P269" s="12" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="Q269" s="26" t="s">
         <v>282</v>
@@ -20475,7 +20475,7 @@
         <v>35</v>
       </c>
       <c r="P270" s="12" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="Q270" s="26" t="s">
         <v>282</v>
@@ -20539,7 +20539,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P271" s="12" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="Q271" s="26" t="s">
         <v>282</v>
@@ -20603,7 +20603,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P272" s="12" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="Q272" s="26" t="s">
         <v>282</v>
@@ -20667,7 +20667,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P273" s="12" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="Q273" s="26" t="s">
         <v>282</v>
@@ -20731,7 +20731,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P274" s="12" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="Q274" s="26" t="s">
         <v>282</v>
@@ -20795,7 +20795,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P275" s="12" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="Q275" s="26" t="s">
         <v>282</v>
@@ -20859,7 +20859,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P276" s="12" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="Q276" s="26" t="s">
         <v>282</v>
@@ -20923,7 +20923,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P277" s="12" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="Q277" s="26" t="s">
         <v>282</v>
@@ -20987,7 +20987,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P278" s="12" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="Q278" s="26" t="s">
         <v>282</v>
@@ -21051,7 +21051,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P279" s="12" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="Q279" s="26" t="s">
         <v>282</v>
@@ -21115,7 +21115,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P280" s="12" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="Q280" s="26" t="s">
         <v>282</v>
@@ -21173,7 +21173,7 @@
         <v>35</v>
       </c>
       <c r="P281" s="12" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="Q281" s="26" t="s">
         <v>282</v>
@@ -21237,7 +21237,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P282" s="12" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="Q282" s="26" t="s">
         <v>282</v>
@@ -21301,7 +21301,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P283" s="12" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="Q283" s="26" t="s">
         <v>282</v>
@@ -21365,7 +21365,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P284" s="12" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="Q284" s="26" t="s">
         <v>282</v>
@@ -21429,7 +21429,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P285" s="12" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="Q285" s="26" t="s">
         <v>282</v>
@@ -21493,7 +21493,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P286" s="12" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="Q286" s="26" t="s">
         <v>282</v>
@@ -21557,7 +21557,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P287" s="12" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="Q287" s="26" t="s">
         <v>282</v>
@@ -21621,7 +21621,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P288" s="12" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="Q288" s="26" t="s">
         <v>282</v>
@@ -21679,7 +21679,7 @@
         <v>35</v>
       </c>
       <c r="P289" s="12" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="Q289" s="26" t="s">
         <v>282</v>
@@ -21743,7 +21743,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P290" s="12" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="Q290" s="26" t="s">
         <v>282</v>
@@ -21807,7 +21807,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P291" s="12" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="Q291" s="26" t="s">
         <v>282</v>
@@ -21871,7 +21871,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P292" s="12" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="Q292" s="26" t="s">
         <v>282</v>
@@ -21935,7 +21935,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P293" s="12" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="Q293" s="26" t="s">
         <v>282</v>
@@ -21999,7 +21999,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P294" s="12" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="Q294" s="26" t="s">
         <v>282</v>
@@ -22055,7 +22055,7 @@
         <v>36</v>
       </c>
       <c r="P295" s="26" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="Q295" s="26" t="s">
         <v>282</v>
@@ -22119,7 +22119,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P296" s="26" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
       <c r="Q296" s="26" t="s">
         <v>282</v>
@@ -22225,7 +22225,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P298" s="26" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="Q298" s="26" t="s">
         <v>282</v>
@@ -22289,7 +22289,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P299" s="26" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="Q299" s="26" t="s">
         <v>282</v>
@@ -22353,7 +22353,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P300" s="26" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="Q300" s="26" t="s">
         <v>282</v>
@@ -22409,7 +22409,7 @@
         <v>36</v>
       </c>
       <c r="P301" s="26" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
       <c r="Q301" s="26" t="s">
         <v>282</v>
@@ -22467,7 +22467,7 @@
         <v>36</v>
       </c>
       <c r="P302" s="26" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="Q302" s="26" t="s">
         <v>282</v>
@@ -22531,7 +22531,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P303" s="26" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="Q303" s="26" t="s">
         <v>282</v>
@@ -22595,7 +22595,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P304" s="26" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="Q304" s="26" t="s">
         <v>282</v>
@@ -22835,7 +22835,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P309" s="26" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="Q309" s="26" t="s">
         <v>282</v>
@@ -22899,7 +22899,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P310" s="26" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="Q310" s="26" t="s">
         <v>282</v>
@@ -22963,7 +22963,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P311" s="26" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="Q311" s="26" t="s">
         <v>282</v>
@@ -23063,7 +23063,7 @@
         <v>36</v>
       </c>
       <c r="P313" s="26" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="Q313" s="26" t="s">
         <v>282</v>
@@ -23127,7 +23127,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P314" s="26" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="Q314" s="26" t="s">
         <v>282</v>
@@ -23191,7 +23191,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P315" s="26" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="Q315" s="26" t="s">
         <v>282</v>
@@ -23255,7 +23255,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P316" s="26" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="Q316" s="26" t="s">
         <v>282</v>
@@ -23319,7 +23319,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P317" s="26" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="Q317" s="26" t="s">
         <v>282</v>
@@ -23383,7 +23383,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P318" s="26" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="Q318" s="26" t="s">
         <v>282</v>
@@ -23447,7 +23447,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P319" s="26" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="Q319" s="26" t="s">
         <v>282</v>
@@ -23511,7 +23511,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P320" s="26" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="Q320" s="26" t="s">
         <v>282</v>
@@ -23569,7 +23569,7 @@
         <v>36</v>
       </c>
       <c r="P321" s="26" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="Q321" s="26" t="s">
         <v>282</v>
@@ -23633,7 +23633,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P322" s="26" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="Q322" s="26" t="s">
         <v>282</v>
@@ -23697,7 +23697,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P323" s="26" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="Q323" s="26" t="s">
         <v>282</v>
@@ -23761,7 +23761,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P324" s="26" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="Q324" s="26" t="s">
         <v>282</v>
@@ -23825,7 +23825,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P325" s="26" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="Q325" s="26" t="s">
         <v>282</v>
@@ -23889,7 +23889,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P326" s="26" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="Q326" s="26" t="s">
         <v>282</v>
@@ -24044,8 +24044,8 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24145,13 +24145,13 @@
         <v>422</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
       <c r="G4" s="72" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>1197</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30">
@@ -24475,13 +24475,13 @@
         <v>422</v>
       </c>
       <c r="F19" s="72" t="s">
-        <v>1198</v>
+        <v>1193</v>
       </c>
       <c r="G19" s="52" t="s">
-        <v>1199</v>
+        <v>1194</v>
       </c>
       <c r="H19" s="72" t="s">
-        <v>1200</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="90">
@@ -24501,13 +24501,13 @@
         <v>422</v>
       </c>
       <c r="F20" s="72" t="s">
-        <v>1201</v>
+        <v>1196</v>
       </c>
       <c r="G20" s="52" t="s">
-        <v>1202</v>
+        <v>1197</v>
       </c>
       <c r="H20" s="72" t="s">
-        <v>1203</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30">
@@ -24527,10 +24527,10 @@
         <v>422</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>1242</v>
+        <v>1237</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>1243</v>
+        <v>1393</v>
       </c>
       <c r="H21" s="72" t="s">
         <v>755</v>
@@ -24569,7 +24569,7 @@
         <v>451</v>
       </c>
       <c r="E23" s="52" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="F23" s="52" t="s">
         <v>756</v>
@@ -24581,7 +24581,7 @@
         <v>427</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
       <c r="C24" s="72" t="s">
         <v>74</v>
@@ -24590,10 +24590,10 @@
         <v>451</v>
       </c>
       <c r="E24" s="52" t="s">
-        <v>1131</v>
+        <v>1126</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
       <c r="H24" s="72"/>
     </row>
@@ -24611,16 +24611,16 @@
         <v>73</v>
       </c>
       <c r="E25" s="52" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F25" s="52" t="s">
-        <v>1211</v>
+        <v>1206</v>
       </c>
       <c r="G25" s="52" t="s">
-        <v>1212</v>
+        <v>1207</v>
       </c>
       <c r="H25" s="72" t="s">
-        <v>1213</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="45">
@@ -24637,16 +24637,16 @@
         <v>73</v>
       </c>
       <c r="E26" s="52" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F26" s="52" t="s">
-        <v>1214</v>
+        <v>1209</v>
       </c>
       <c r="G26" s="52" t="s">
-        <v>1215</v>
+        <v>1210</v>
       </c>
       <c r="H26" s="72" t="s">
-        <v>1216</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45">
@@ -24654,7 +24654,7 @@
         <v>713</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>74</v>
@@ -24663,16 +24663,16 @@
         <v>73</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F27" s="52" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="H27" s="72" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45">
@@ -24680,7 +24680,7 @@
         <v>713</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
       <c r="C28" s="72" t="s">
         <v>74</v>
@@ -24689,16 +24689,16 @@
         <v>73</v>
       </c>
       <c r="E28" s="52" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F28" s="52" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="H28" s="72" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="90">
@@ -24715,10 +24715,10 @@
         <v>73</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F29" s="52" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="G29" s="52" t="s">
         <v>782</v>
@@ -24762,7 +24762,7 @@
         <v>73</v>
       </c>
       <c r="E31" s="72" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="F31" s="72" t="s">
         <v>76</v>
@@ -24786,10 +24786,10 @@
         <v>424</v>
       </c>
       <c r="F32" s="72" t="s">
-        <v>1244</v>
+        <v>1238</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="H32" s="72" t="s">
         <v>669</v>
@@ -24812,10 +24812,10 @@
         <v>424</v>
       </c>
       <c r="F33" s="72" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
       <c r="H33" s="72" t="s">
         <v>670</v>
@@ -24838,10 +24838,10 @@
         <v>425</v>
       </c>
       <c r="F34" s="72" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="G34" s="52" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="H34" s="72" t="s">
         <v>476</v>
@@ -24864,10 +24864,10 @@
         <v>425</v>
       </c>
       <c r="F35" s="72" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="H35" s="72" t="s">
         <v>477</v>
@@ -24887,16 +24887,16 @@
         <v>757</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="F36" s="72" t="s">
-        <v>1128</v>
+        <v>1123</v>
       </c>
       <c r="G36" s="52" t="s">
-        <v>1129</v>
+        <v>1124</v>
       </c>
       <c r="H36" s="72" t="s">
-        <v>1130</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30">
@@ -24939,7 +24939,7 @@
         <v>75</v>
       </c>
       <c r="E38" s="72" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="F38" s="72" t="s">
         <v>761</v>
@@ -24965,7 +24965,7 @@
         <v>75</v>
       </c>
       <c r="E39" s="72" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="F39" s="72" t="s">
         <v>764</v>
@@ -24994,13 +24994,13 @@
         <v>511</v>
       </c>
       <c r="F40" s="72" t="s">
-        <v>1145</v>
+        <v>1140</v>
       </c>
       <c r="G40" s="72" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
       <c r="H40" s="72" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="60">
@@ -25020,13 +25020,13 @@
         <v>767</v>
       </c>
       <c r="F41" s="72" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="G41" s="72" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="H41" s="72" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="45">
@@ -25034,7 +25034,7 @@
         <v>731</v>
       </c>
       <c r="B42" s="73" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="C42" s="72" t="s">
         <v>74</v>
@@ -25046,13 +25046,13 @@
         <v>767</v>
       </c>
       <c r="F42" s="72" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="G42" s="72" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="H42" s="72" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30">
@@ -25060,7 +25060,7 @@
         <v>731</v>
       </c>
       <c r="B43" s="73" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="C43" s="72" t="s">
         <v>74</v>
@@ -25072,13 +25072,13 @@
         <v>767</v>
       </c>
       <c r="F43" s="72" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="G43" s="72" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="H43" s="72" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30">
@@ -25124,13 +25124,13 @@
         <v>766</v>
       </c>
       <c r="F45" s="72" t="s">
-        <v>1142</v>
+        <v>1137</v>
       </c>
       <c r="G45" s="72" t="s">
-        <v>1143</v>
+        <v>1138</v>
       </c>
       <c r="H45" s="72" t="s">
-        <v>1144</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="45">
@@ -25147,16 +25147,16 @@
         <v>75</v>
       </c>
       <c r="E46" s="72" t="s">
-        <v>1227</v>
+        <v>1222</v>
       </c>
       <c r="F46" s="72" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="G46" s="72" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="H46" s="72" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="45">
@@ -25164,7 +25164,7 @@
         <v>734</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>1112</v>
+        <v>1107</v>
       </c>
       <c r="C47" s="72" t="s">
         <v>74</v>
@@ -25176,13 +25176,13 @@
         <v>766</v>
       </c>
       <c r="F47" s="72" t="s">
-        <v>1108</v>
+        <v>1103</v>
       </c>
       <c r="G47" s="72" t="s">
-        <v>1109</v>
+        <v>1104</v>
       </c>
       <c r="H47" s="72" t="s">
-        <v>1110</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="30">
@@ -25190,7 +25190,7 @@
         <v>734</v>
       </c>
       <c r="B48" s="73" t="s">
-        <v>1113</v>
+        <v>1108</v>
       </c>
       <c r="C48" s="72" t="s">
         <v>74</v>
@@ -25202,13 +25202,13 @@
         <v>766</v>
       </c>
       <c r="F48" s="72" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
       <c r="G48" s="72" t="s">
-        <v>1116</v>
+        <v>1111</v>
       </c>
       <c r="H48" s="72" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30">
@@ -25257,7 +25257,7 @@
         <v>546</v>
       </c>
       <c r="G50" s="72" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="H50" s="72" t="s">
         <v>512</v>
@@ -25294,7 +25294,7 @@
         <v>752</v>
       </c>
       <c r="B52" s="73" t="s">
-        <v>1228</v>
+        <v>1223</v>
       </c>
       <c r="C52" s="72" t="s">
         <v>74</v>
@@ -25306,10 +25306,10 @@
         <v>479</v>
       </c>
       <c r="F52" s="72" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="G52" s="72" t="s">
-        <v>1114</v>
+        <v>1109</v>
       </c>
       <c r="H52" s="72" t="s">
         <v>512</v>
@@ -25358,21 +25358,21 @@
         <v>479</v>
       </c>
       <c r="F54" s="72" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
       <c r="G54" s="104" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="H54" s="72" t="s">
-        <v>1210</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="75">
       <c r="A55" s="75" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="B55" s="73" t="s">
-        <v>1233</v>
+        <v>1228</v>
       </c>
       <c r="C55" s="72" t="s">
         <v>74</v>
@@ -25384,21 +25384,21 @@
         <v>422</v>
       </c>
       <c r="F55" s="72" t="s">
-        <v>1234</v>
+        <v>1229</v>
       </c>
       <c r="G55" s="52" t="s">
-        <v>1235</v>
+        <v>1230</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="45">
       <c r="A56" s="75" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="B56" s="73" t="s">
-        <v>1237</v>
+        <v>1232</v>
       </c>
       <c r="C56" s="72" t="s">
         <v>74</v>
@@ -25410,7 +25410,7 @@
         <v>422</v>
       </c>
       <c r="F56" s="72" t="s">
-        <v>1238</v>
+        <v>1233</v>
       </c>
       <c r="G56" s="52" t="s">
         <v>754</v>
@@ -25421,10 +25421,10 @@
     </row>
     <row r="57" spans="1:8" ht="60">
       <c r="A57" s="75" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="B57" s="73" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="C57" s="72" t="s">
         <v>74</v>
@@ -25436,21 +25436,21 @@
         <v>422</v>
       </c>
       <c r="F57" s="72" t="s">
-        <v>1240</v>
+        <v>1235</v>
       </c>
       <c r="G57" s="52" t="s">
-        <v>1235</v>
+        <v>1230</v>
       </c>
       <c r="H57" s="72" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="45">
       <c r="A58" s="75" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="B58" s="73" t="s">
-        <v>1232</v>
+        <v>1227</v>
       </c>
       <c r="C58" s="72" t="s">
         <v>74</v>
@@ -25514,13 +25514,13 @@
         <v>479</v>
       </c>
       <c r="F60" s="72" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="G60" s="52" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
       <c r="H60" s="72" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="60">
@@ -25540,13 +25540,13 @@
         <v>479</v>
       </c>
       <c r="F61" s="72" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="G61" s="52" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="H61" s="72" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -25575,7 +25575,7 @@
         <v>454</v>
       </c>
       <c r="B63" s="73" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>72</v>
@@ -25584,10 +25584,10 @@
         <v>73</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="F63" s="72" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="H63" s="72"/>
     </row>
@@ -25668,7 +25668,7 @@
         <v>757</v>
       </c>
       <c r="E67" s="72" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="F67" s="72" t="s">
         <v>786</v>
@@ -25680,7 +25680,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="45">
+    <row r="68" spans="1:8" ht="30">
       <c r="A68" s="75" t="s">
         <v>745</v>
       </c>
@@ -25694,16 +25694,16 @@
         <v>757</v>
       </c>
       <c r="E68" s="72" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="F68" s="72" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="G68" s="52" t="s">
-        <v>1101</v>
+        <v>1388</v>
       </c>
       <c r="H68" s="72" t="s">
-        <v>1102</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="75">
@@ -25720,7 +25720,7 @@
         <v>757</v>
       </c>
       <c r="E69" s="72" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="F69" s="72" t="s">
         <v>790</v>
@@ -25746,7 +25746,7 @@
         <v>757</v>
       </c>
       <c r="E70" s="72" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="F70" s="72" t="s">
         <v>792</v>
@@ -25758,7 +25758,7 @@
         <v>969696</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="45">
+    <row r="71" spans="1:8" ht="75">
       <c r="A71" s="75" t="s">
         <v>745</v>
       </c>
@@ -25772,16 +25772,16 @@
         <v>757</v>
       </c>
       <c r="E71" s="72" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="F71" s="72" t="s">
-        <v>1105</v>
+        <v>1390</v>
       </c>
       <c r="G71" s="52" t="s">
-        <v>1106</v>
+        <v>1391</v>
       </c>
       <c r="H71" s="72" t="s">
-        <v>1107</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="30">
@@ -25798,7 +25798,7 @@
         <v>73</v>
       </c>
       <c r="E72" s="72" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
       <c r="F72" s="72" t="s">
         <v>793</v>
@@ -25819,7 +25819,7 @@
         <v>73</v>
       </c>
       <c r="E73" s="72" t="s">
-        <v>1239</v>
+        <v>1234</v>
       </c>
       <c r="F73" s="72" t="s">
         <v>797</v>
@@ -25845,7 +25845,7 @@
         <v>73</v>
       </c>
       <c r="E74" s="72" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="F74" s="72" t="s">
         <v>794</v>
@@ -25866,7 +25866,7 @@
         <v>73</v>
       </c>
       <c r="E75" s="72" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="F75" s="72" t="s">
         <v>795</v>
@@ -25887,7 +25887,7 @@
         <v>73</v>
       </c>
       <c r="E76" s="72" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="F76" s="72" t="s">
         <v>796</v>
@@ -25942,18 +25942,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix subscript entries for "hard coal" in output graphs tab
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -3858,31 +3858,13 @@
     <t>Output Process Emissions in CO2e by Industry[cement and other carbonates]; Output Process Emissions in CO2e by Industry[mining]; Output Process Emissions in CO2e by Industry[chemicals]; Output Process Emissions in CO2e by Industry[iron and steel]; Output Process Emissions in CO2e by Industry[natural gas and petroleum systems]; Output Process Emissions in CO2e by Industry[other industries]</t>
   </si>
   <si>
-    <t>Output Industrial Fuel Use by Fuel[heat if]; Output Industrial Fuel Use by Fuel[biomass if]; Output Industrial Fuel Use by Fuel[petroleum diesel if]; Output Industrial Fuel Use by Fuel[natural gas if]; Output Industrial Fuel Use by Fuel[coal if]; Output Industrial Fuel Use by Fuel[electricity if]</t>
-  </si>
-  <si>
-    <t>Energy Related CO2 Emissions from Petroleum Fuels; Energy Related CO2 Emissions by Fuel[natural gas]; Energy Related CO2 Emissions by Fuel[lignite]; Energy Related CO2 Emissions by Fuel[ coal]</t>
-  </si>
-  <si>
-    <t>Output Electricity Generation by Type[geothermal es]; Output Electricity Generation by Type[biomass es]; Output Electricity Generation by Type[solar thermal es]; Output Distributed Solar PV Output; Output Electricity Generation by Type[solar PV es]; Output Electricity Generation by Type[onshore wind es]; Output Electricity Generation by Type[offshore wind es]; Output Electricity Generation by Type[hydro es]; Output Electricity Generation by Type[nuclear es]; Output Non Solar Distributed Output; Output Electricity Generation by Type[petroleum es]; Output Electricity Generation by Type[natural gas peaker es]; Output Electricity Generation by Type[natural gas nonpeaker es]; Output Electricity Generation by Type[lignite es]; Output Electricity Generation by Type[ coal es]; Output Net Imports of Electricity</t>
-  </si>
-  <si>
     <t>Geothermal, Biomass, Solar Thermal, Distributed Solar PV, Utility Solar PV, Onshore Wind, Offshore Wind, Hydro, Nuclear, Distributed Non-Solar, Petroleum, Natural Gas Peaker, Natural Gas Nonpeaker, Lignite,  Coal, Imported Electricity</t>
   </si>
   <si>
-    <t>Output Change in Electricity Generation by Type[geothermal es]; Output Change in Electricity Generation by Type[biomass es]; Output Change in Electricity Generation by Type[solar thermal es]; Output Change in Distributed Solar PV Output; Output Change in Electricity Generation by Type[solar PV es]; Output Change in Electricity Generation by Type[onshore wind es]; Output Change in Electricity Generation by Type[offshore wind es]; Output Change in Electricity Generation by Type[hydro es]; Output Change in Electricity Generation by Type[nuclear es]; Output Change in Electricity Generation by Type[petroleum es]; Output Change in Electricity Generation by Type[natural gas peaker es]; Output Change in Electricity Generation by Type[natural gas nonpeaker es]; Output Change in Electricity Generation by Type[lignite es]; Output Change in Electricity Generation by Type[ coal es]; Output Change in Net Imports of Electricity</t>
-  </si>
-  <si>
     <t>Geothermal, Biomass, Solar Thermal, Distributed Solar PV, Utility Solar PV, Onshore Wind, Offshore Wind, Hydro, Nuclear, Petroleum, Natural Gas Peaker, Natural Gas Nonpeaker, Lignite,  Coal, Imported Electricity</t>
   </si>
   <si>
-    <t>Output Electricity Generation Capacity[geothermal es]; Output Electricity Generation Capacity[biomass es]; Output Electricity Generation Capacity[solar thermal es]; Output Distributed Solar PV Capacity; Output Electricity Generation Capacity[solar PV es]; Output Electricity Generation Capacity[onshore wind es]; Output Electricity Generation Capacity[offshore wind es]; Output Electricity Generation Capacity[hydro es]; Output Electricity Generation Capacity[nuclear es]; Output Non Solar Distributed Capacity; Output Electricity Generation Capacity[petroleum es]; Output Electricity Generation Capacity[natural gas peaker es]; Output Electricity Generation Capacity[natural gas nonpeaker es]; Output Electricity Generation Capacity[lignite es]; Output Electricity Generation Capacity[ coal es]</t>
-  </si>
-  <si>
     <t>Geothermal, Biomass, Solar Thermal, Distributed Solar PV, Utility Solar PV, Onshore Wind, Offshore Wind, Hydro, Nuclear, Distributed Non-Solar, Petroleum, Natural Gas Peaker, Natural Gas Nonpeaker, Lignite,  Coal</t>
-  </si>
-  <si>
-    <t>Output Change in Electricity Generation Capacity[geothermal es]; Output Change in Electricity Generation Capacity[biomass es]; Output Change in Electricity Generation Capacity[solar thermal es]; Output Change in Distributed Solar Capacity; Output Change in Electricity Generation Capacity[solar PV es]; Output Change in Electricity Generation Capacity[onshore wind es]; Output Change in Electricity Generation Capacity[offshore wind es]; Output Change in Electricity Generation Capacity[hydro es]; Output Change in Electricity Generation Capacity[nuclear es]; Output Change in Electricity Generation Capacity[petroleum es]; Output Change in Electricity Generation Capacity[natural gas peaker es]; Output Change in Electricity Generation Capacity[natural gas nonpeaker es]; Output Change in Electricity Generation Capacity[lignite es]; Output Change in Electricity Generation Capacity[ coal es]</t>
   </si>
   <si>
     <t>Geothermal, Biomass, Solar Thermal, Distributed Solar PV, Utility Solar PV, Onshore Wind, Offshore Wind, Hydro, Nuclear, Petroleum, Natural Gas Peaker, Natural Gas Nonpeaker, Lignite,  Coal</t>
@@ -4381,9 +4363,6 @@
     <t>Output Total  Coal and Petcoke Consumption</t>
   </si>
   <si>
-    <t>Output Fuel Costs per Unit Energy by Sector[coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[coal,industry sector]</t>
-  </si>
-  <si>
     <t>Electricity Sector, Industry Sector</t>
   </si>
   <si>
@@ -4400,6 +4379,27 @@
   </si>
   <si>
     <t>Petroleum, Natural Gas, Lignite, Hard Coal</t>
+  </si>
+  <si>
+    <t>Energy Related CO2 Emissions from Petroleum Fuels; Energy Related CO2 Emissions by Fuel[natural gas]; Energy Related CO2 Emissions by Fuel[lignite]; Energy Related CO2 Emissions by Fuel[hard coal]</t>
+  </si>
+  <si>
+    <t>Output Electricity Generation by Type[geothermal es]; Output Electricity Generation by Type[biomass es]; Output Electricity Generation by Type[solar thermal es]; Output Distributed Solar PV Output; Output Electricity Generation by Type[solar PV es]; Output Electricity Generation by Type[onshore wind es]; Output Electricity Generation by Type[offshore wind es]; Output Electricity Generation by Type[hydro es]; Output Electricity Generation by Type[nuclear es]; Output Non Solar Distributed Output; Output Electricity Generation by Type[petroleum es]; Output Electricity Generation by Type[natural gas peaker es]; Output Electricity Generation by Type[natural gas nonpeaker es]; Output Electricity Generation by Type[lignite es]; Output Electricity Generation by Type[hard coal es]; Output Net Imports of Electricity</t>
+  </si>
+  <si>
+    <t>Output Change in Electricity Generation by Type[geothermal es]; Output Change in Electricity Generation by Type[biomass es]; Output Change in Electricity Generation by Type[solar thermal es]; Output Change in Distributed Solar PV Output; Output Change in Electricity Generation by Type[solar PV es]; Output Change in Electricity Generation by Type[onshore wind es]; Output Change in Electricity Generation by Type[offshore wind es]; Output Change in Electricity Generation by Type[hydro es]; Output Change in Electricity Generation by Type[nuclear es]; Output Change in Electricity Generation by Type[petroleum es]; Output Change in Electricity Generation by Type[natural gas peaker es]; Output Change in Electricity Generation by Type[natural gas nonpeaker es]; Output Change in Electricity Generation by Type[lignite es]; Output Change in Electricity Generation by Type[hard coal es]; Output Change in Net Imports of Electricity</t>
+  </si>
+  <si>
+    <t>Output Electricity Generation Capacity[geothermal es]; Output Electricity Generation Capacity[biomass es]; Output Electricity Generation Capacity[solar thermal es]; Output Distributed Solar PV Capacity; Output Electricity Generation Capacity[solar PV es]; Output Electricity Generation Capacity[onshore wind es]; Output Electricity Generation Capacity[offshore wind es]; Output Electricity Generation Capacity[hydro es]; Output Electricity Generation Capacity[nuclear es]; Output Non Solar Distributed Capacity; Output Electricity Generation Capacity[petroleum es]; Output Electricity Generation Capacity[natural gas peaker es]; Output Electricity Generation Capacity[natural gas nonpeaker es]; Output Electricity Generation Capacity[lignite es]; Output Electricity Generation Capacity[hard coal es]</t>
+  </si>
+  <si>
+    <t>Output Change in Electricity Generation Capacity[geothermal es]; Output Change in Electricity Generation Capacity[biomass es]; Output Change in Electricity Generation Capacity[solar thermal es]; Output Change in Distributed Solar Capacity; Output Change in Electricity Generation Capacity[solar PV es]; Output Change in Electricity Generation Capacity[onshore wind es]; Output Change in Electricity Generation Capacity[offshore wind es]; Output Change in Electricity Generation Capacity[hydro es]; Output Change in Electricity Generation Capacity[nuclear es]; Output Change in Electricity Generation Capacity[petroleum es]; Output Change in Electricity Generation Capacity[natural gas peaker es]; Output Change in Electricity Generation Capacity[natural gas nonpeaker es]; Output Change in Electricity Generation Capacity[lignite es]; Output Change in Electricity Generation Capacity[hard coal es]</t>
+  </si>
+  <si>
+    <t>Output Industrial Fuel Use by Fuel[heat if]; Output Industrial Fuel Use by Fuel[biomass if]; Output Industrial Fuel Use by Fuel[petroleum diesel if]; Output Industrial Fuel Use by Fuel[natural gas if]; Output Industrial Fuel Use by Fuel[hard coal if]; Output Industrial Fuel Use by Fuel[electricity if]</t>
+  </si>
+  <si>
+    <t>Output Fuel Costs per Unit Energy by Sector[hard coal,electricity sector]; Output Fuel Costs per Unit Energy by Sector[hard coal,industry sector]</t>
   </si>
 </sst>
 </file>
@@ -6523,7 +6523,7 @@
         <v>495</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
       <c r="Q9" s="47" t="s">
         <v>496</v>
@@ -6591,7 +6591,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P10" s="26" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
       <c r="Q10" s="34" t="str">
         <f t="shared" si="5"/>
@@ -6659,7 +6659,7 @@
         <v>% of new vehicles sold</v>
       </c>
       <c r="P11" s="26" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
       <c r="Q11" s="34" t="str">
         <f t="shared" si="5"/>
@@ -7179,7 +7179,7 @@
         <v>482</v>
       </c>
       <c r="P21" s="26" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="Q21" s="47" t="s">
         <v>483</v>
@@ -7243,7 +7243,7 @@
         <v>482</v>
       </c>
       <c r="P22" s="26" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="Q22" s="51"/>
       <c r="R22" s="51"/>
@@ -7301,7 +7301,7 @@
         <v>482</v>
       </c>
       <c r="P23" s="26" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="Q23" s="51"/>
       <c r="R23" s="51"/>
@@ -7761,7 +7761,7 @@
         <v>457</v>
       </c>
       <c r="P33" s="26" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="Q33" s="26" t="s">
         <v>211</v>
@@ -7806,7 +7806,7 @@
         <v>1203</v>
       </c>
       <c r="K34" s="50" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
@@ -7851,7 +7851,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K35" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L35" s="37">
         <f>L$36</f>
@@ -7913,7 +7913,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K36" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L36" s="32">
         <v>0</v>
@@ -7928,7 +7928,7 @@
         <v>126</v>
       </c>
       <c r="P36" s="107" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="Q36" s="26" t="s">
         <v>213</v>
@@ -7937,10 +7937,10 @@
         <v>214</v>
       </c>
       <c r="S36" s="105" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="T36" s="26" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="45">
@@ -7979,7 +7979,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K37" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L37" s="37">
         <f>L$36</f>
@@ -7997,7 +7997,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P37" s="96" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="Q37" s="37" t="str">
         <f t="shared" si="13"/>
@@ -8046,7 +8046,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K38" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L38" s="37">
         <f>L$36</f>
@@ -8065,7 +8065,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P38" s="96" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="12"/>
@@ -8106,7 +8106,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K39" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
@@ -8152,7 +8152,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K40" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
@@ -8197,7 +8197,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K41" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L41" s="34">
         <v>0</v>
@@ -8212,7 +8212,7 @@
         <v>126</v>
       </c>
       <c r="P41" s="96" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
       <c r="Q41" s="28"/>
       <c r="R41" s="28"/>
@@ -8255,7 +8255,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K42" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L42" s="34">
         <f>L$36</f>
@@ -8273,7 +8273,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P42" s="108" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="Q42" s="28" t="str">
         <f>Q$36</f>
@@ -8322,7 +8322,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K43" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L43" s="34">
         <f>L$36</f>
@@ -8340,7 +8340,7 @@
         <v>% increase in miles/gal</v>
       </c>
       <c r="P43" s="108" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="Q43" s="28" t="str">
         <f>Q$36</f>
@@ -8391,7 +8391,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K44" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="35"/>
@@ -8437,7 +8437,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K45" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="35"/>
@@ -8483,7 +8483,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K46" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M46" s="5"/>
       <c r="N46" s="5"/>
@@ -8526,7 +8526,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K47" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L47" s="34"/>
       <c r="M47" s="36"/>
@@ -8572,7 +8572,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K48" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L48" s="34"/>
       <c r="M48" s="36"/>
@@ -8618,7 +8618,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K49" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L49" s="34"/>
       <c r="M49" s="36"/>
@@ -8664,7 +8664,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K50" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L50" s="34"/>
       <c r="M50" s="36"/>
@@ -8712,14 +8712,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K51" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L51" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M51" s="36" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="N51" s="34">
         <f>N$36</f>
@@ -8781,7 +8781,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K52" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
@@ -8824,7 +8824,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K53" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L53" s="34"/>
       <c r="M53" s="36"/>
@@ -8870,7 +8870,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K54" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L54" s="34"/>
       <c r="M54" s="36"/>
@@ -8916,7 +8916,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K55" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L55" s="34"/>
       <c r="M55" s="36"/>
@@ -8962,7 +8962,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K56" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L56" s="34"/>
       <c r="M56" s="36"/>
@@ -9010,14 +9010,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K57" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L57" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M57" s="36" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="N57" s="34">
         <f>N$36</f>
@@ -9079,7 +9079,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K58" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
@@ -9122,7 +9122,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K59" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L59" s="34"/>
       <c r="M59" s="36"/>
@@ -9168,7 +9168,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K60" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L60" s="34"/>
       <c r="M60" s="36"/>
@@ -9214,7 +9214,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K61" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L61" s="34"/>
       <c r="M61" s="36"/>
@@ -9260,7 +9260,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K62" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L62" s="34"/>
       <c r="M62" s="36"/>
@@ -9308,14 +9308,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K63" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L63" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M63" s="36" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="N63" s="34">
         <f>N$36</f>
@@ -9377,7 +9377,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K64" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -9420,7 +9420,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K65" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L65" s="34"/>
       <c r="M65" s="36"/>
@@ -9468,14 +9468,14 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K66" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L66" s="34">
         <f>L$36</f>
         <v>0</v>
       </c>
       <c r="M66" s="36" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="N66" s="34">
         <f>N$36</f>
@@ -9537,7 +9537,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K67" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L67" s="34"/>
       <c r="M67" s="36"/>
@@ -9583,7 +9583,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K68" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L68" s="34"/>
       <c r="M68" s="36"/>
@@ -9629,7 +9629,7 @@
         <v>Vehicle Tailpipe Emissions Standards</v>
       </c>
       <c r="K69" s="64" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="L69" s="34"/>
       <c r="M69" s="36"/>
@@ -9680,7 +9680,7 @@
         <v>501</v>
       </c>
       <c r="P70" s="26" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="Q70" s="26" t="s">
         <v>502</v>
@@ -9738,7 +9738,7 @@
         <v>40</v>
       </c>
       <c r="P71" s="107" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="Q71" s="26" t="s">
         <v>215</v>
@@ -9802,7 +9802,7 @@
         <v>% of TDM package implemented</v>
       </c>
       <c r="P72" s="107" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="Q72" s="31" t="str">
         <f t="shared" si="18"/>
@@ -9861,7 +9861,7 @@
         <v>128</v>
       </c>
       <c r="P73" s="26" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="Q73" s="26" t="s">
         <v>217</v>
@@ -9923,7 +9923,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q74" s="31" t="str">
         <f t="shared" si="21"/>
@@ -9987,7 +9987,7 @@
         <v>% of newly sold non-electric building components</v>
       </c>
       <c r="P75" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q75" s="31" t="str">
         <f t="shared" si="21"/>
@@ -10047,7 +10047,7 @@
         <v>34</v>
       </c>
       <c r="P76" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q76" s="26" t="s">
         <v>219</v>
@@ -10116,7 +10116,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P77" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q77" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10193,7 +10193,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P78" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q78" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10270,7 +10270,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P79" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q79" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10347,7 +10347,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P80" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q80" s="28" t="str">
         <f t="shared" si="25"/>
@@ -10424,7 +10424,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P81" s="26" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="Q81" s="28" t="str">
         <f t="shared" si="25"/>
@@ -11422,7 +11422,7 @@
         <v>31</v>
       </c>
       <c r="P94" s="26" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="Q94" s="26" t="s">
         <v>221</v>
@@ -11475,7 +11475,7 @@
         <v>296</v>
       </c>
       <c r="P95" s="26" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="Q95" s="26" t="s">
         <v>297</v>
@@ -11484,7 +11484,7 @@
         <v>298</v>
       </c>
       <c r="S95" s="12" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="T95" s="12" t="s">
         <v>436</v>
@@ -11538,7 +11538,7 @@
         <v>301</v>
       </c>
       <c r="S96" s="101" t="s">
-        <v>1247</v>
+        <v>1241</v>
       </c>
       <c r="T96" s="28"/>
     </row>
@@ -11566,7 +11566,7 @@
         <v>1161</v>
       </c>
       <c r="K97" s="72" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="L97" s="38">
         <v>0</v>
@@ -13076,7 +13076,7 @@
         <v>37</v>
       </c>
       <c r="P125" s="26" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="Q125" s="26" t="s">
         <v>229</v>
@@ -13085,10 +13085,10 @@
         <v>230</v>
       </c>
       <c r="S125" s="105" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="T125" s="26" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="57" customHeight="1">
@@ -13684,7 +13684,7 @@
         <v>32</v>
       </c>
       <c r="P138" s="26" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="Q138" s="26" t="s">
         <v>233</v>
@@ -13693,7 +13693,7 @@
         <v>234</v>
       </c>
       <c r="S138" s="5" t="s">
-        <v>1248</v>
+        <v>1242</v>
       </c>
       <c r="T138" s="26" t="s">
         <v>186</v>
@@ -13729,7 +13729,7 @@
         <v>0</v>
       </c>
       <c r="M139" s="32" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="N139" s="32">
         <v>0.01</v>
@@ -13738,7 +13738,7 @@
         <v>148</v>
       </c>
       <c r="P139" s="26" t="s">
-        <v>1249</v>
+        <v>1243</v>
       </c>
       <c r="Q139" s="26" t="s">
         <v>235</v>
@@ -15708,7 +15708,7 @@
         <v>285</v>
       </c>
       <c r="P182" s="26" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="Q182" s="12" t="s">
         <v>548</v>
@@ -15717,7 +15717,7 @@
         <v>286</v>
       </c>
       <c r="S182" s="105" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
       <c r="T182" s="12"/>
     </row>
@@ -15726,7 +15726,7 @@
         <v>7</v>
       </c>
       <c r="B183" s="26" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="C183" s="26" t="s">
         <v>344</v>
@@ -15742,7 +15742,7 @@
         <v>49</v>
       </c>
       <c r="J183" s="50" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="K183" s="50" t="s">
         <v>610</v>
@@ -15760,7 +15760,7 @@
         <v>38</v>
       </c>
       <c r="P183" s="26" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="Q183" s="26" t="s">
         <v>238</v>
@@ -16365,7 +16365,7 @@
         <v>37</v>
       </c>
       <c r="P194" s="26" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="Q194" s="26" t="s">
         <v>242</v>
@@ -16525,7 +16525,7 @@
         <v>34</v>
       </c>
       <c r="P197" s="103" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
       <c r="Q197" s="26" t="s">
         <v>248</v>
@@ -16537,7 +16537,7 @@
         <v>561</v>
       </c>
       <c r="T197" s="105" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="198" spans="1:20" s="6" customFormat="1" ht="60">
@@ -16590,7 +16590,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P198" s="26" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="Q198" s="26" t="s">
         <v>248</v>
@@ -16658,7 +16658,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P199" s="26" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="Q199" s="26" t="s">
         <v>248</v>
@@ -16726,7 +16726,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P200" s="26" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="Q200" s="26" t="s">
         <v>248</v>
@@ -16794,7 +16794,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P201" s="26" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="Q201" s="26" t="s">
         <v>248</v>
@@ -16928,7 +16928,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P203" s="26" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="Q203" s="26" t="s">
         <v>248</v>
@@ -16996,7 +16996,7 @@
         <v>% reduction in energy use</v>
       </c>
       <c r="P204" s="26" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="Q204" s="26" t="s">
         <v>248</v>
@@ -17102,7 +17102,7 @@
         <v>33</v>
       </c>
       <c r="P206" s="26" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="Q206" s="26" t="s">
         <v>252</v>
@@ -17120,7 +17120,7 @@
         <v>8</v>
       </c>
       <c r="B207" s="26" t="s">
-        <v>1260</v>
+        <v>1254</v>
       </c>
       <c r="C207" s="26" t="s">
         <v>362</v>
@@ -17154,7 +17154,7 @@
         <v>363</v>
       </c>
       <c r="P207" s="26" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="Q207" s="26" t="s">
         <v>252</v>
@@ -17163,10 +17163,10 @@
         <v>253</v>
       </c>
       <c r="S207" s="54" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="T207" s="106" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="208" spans="1:20" ht="90">
@@ -17970,7 +17970,7 @@
         <v>37</v>
       </c>
       <c r="P223" s="26" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="Q223" s="26" t="s">
         <v>272</v>
@@ -17979,7 +17979,7 @@
         <v>273</v>
       </c>
       <c r="S223" s="54" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="T223" s="26"/>
     </row>
@@ -18026,7 +18026,7 @@
         <v>172</v>
       </c>
       <c r="P224" s="26" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="Q224" s="26" t="s">
         <v>274</v>
@@ -18092,7 +18092,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P225" s="26" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="Q225" s="28" t="str">
         <f t="shared" ref="Q225:R229" si="63">Q$224</f>
@@ -18156,7 +18156,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P226" s="26" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="Q226" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18220,7 +18220,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P227" s="26" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
       <c r="Q227" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18284,7 +18284,7 @@
         <v>$/metric ton CO2e</v>
       </c>
       <c r="P228" s="26" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="Q228" s="28" t="str">
         <f t="shared" si="63"/>
@@ -18488,7 +18488,7 @@
         <v>175</v>
       </c>
       <c r="P232" s="12" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="Q232" s="12" t="s">
         <v>278</v>
@@ -18552,7 +18552,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P233" s="12" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="Q233" s="12" t="s">
         <v>278</v>
@@ -18616,7 +18616,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P234" s="12" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="Q234" s="12" t="s">
         <v>278</v>
@@ -18768,7 +18768,7 @@
         <v>% reduction in BAU subsidies</v>
       </c>
       <c r="P237" s="12" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
       <c r="Q237" s="12" t="s">
         <v>278</v>
@@ -20040,7 +20040,7 @@
         <v>35</v>
       </c>
       <c r="P263" s="26" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="Q263" s="26" t="s">
         <v>282</v>
@@ -20104,7 +20104,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P264" s="26" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="Q264" s="26" t="s">
         <v>282</v>
@@ -20168,7 +20168,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P265" s="26" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="Q265" s="26" t="s">
         <v>282</v>
@@ -20232,7 +20232,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P266" s="26" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="Q266" s="26" t="s">
         <v>282</v>
@@ -20296,7 +20296,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P267" s="26" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="Q267" s="26" t="s">
         <v>282</v>
@@ -20360,7 +20360,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P268" s="26" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="Q268" s="26" t="s">
         <v>282</v>
@@ -20417,7 +20417,7 @@
         <v>35</v>
       </c>
       <c r="P269" s="12" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="Q269" s="26" t="s">
         <v>282</v>
@@ -20475,7 +20475,7 @@
         <v>35</v>
       </c>
       <c r="P270" s="12" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="Q270" s="26" t="s">
         <v>282</v>
@@ -20539,7 +20539,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P271" s="12" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="Q271" s="26" t="s">
         <v>282</v>
@@ -20603,7 +20603,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P272" s="12" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="Q272" s="26" t="s">
         <v>282</v>
@@ -20667,7 +20667,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P273" s="12" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="Q273" s="26" t="s">
         <v>282</v>
@@ -20731,7 +20731,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P274" s="12" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="Q274" s="26" t="s">
         <v>282</v>
@@ -20795,7 +20795,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P275" s="12" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="Q275" s="26" t="s">
         <v>282</v>
@@ -20859,7 +20859,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P276" s="12" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="Q276" s="26" t="s">
         <v>282</v>
@@ -20923,7 +20923,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P277" s="12" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="Q277" s="26" t="s">
         <v>282</v>
@@ -20987,7 +20987,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P278" s="12" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="Q278" s="26" t="s">
         <v>282</v>
@@ -21051,7 +21051,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P279" s="12" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="Q279" s="26" t="s">
         <v>282</v>
@@ -21115,7 +21115,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P280" s="12" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="Q280" s="26" t="s">
         <v>282</v>
@@ -21173,7 +21173,7 @@
         <v>35</v>
       </c>
       <c r="P281" s="12" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="Q281" s="26" t="s">
         <v>282</v>
@@ -21237,7 +21237,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P282" s="12" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="Q282" s="26" t="s">
         <v>282</v>
@@ -21301,7 +21301,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P283" s="12" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="Q283" s="26" t="s">
         <v>282</v>
@@ -21365,7 +21365,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P284" s="12" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="Q284" s="26" t="s">
         <v>282</v>
@@ -21429,7 +21429,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P285" s="12" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="Q285" s="26" t="s">
         <v>282</v>
@@ -21493,7 +21493,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P286" s="12" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="Q286" s="26" t="s">
         <v>282</v>
@@ -21557,7 +21557,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P287" s="12" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="Q287" s="26" t="s">
         <v>282</v>
@@ -21621,7 +21621,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P288" s="12" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="Q288" s="26" t="s">
         <v>282</v>
@@ -21679,7 +21679,7 @@
         <v>35</v>
       </c>
       <c r="P289" s="12" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="Q289" s="26" t="s">
         <v>282</v>
@@ -21743,7 +21743,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P290" s="12" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="Q290" s="26" t="s">
         <v>282</v>
@@ -21807,7 +21807,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P291" s="12" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="Q291" s="26" t="s">
         <v>282</v>
@@ -21871,7 +21871,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P292" s="12" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="Q292" s="26" t="s">
         <v>282</v>
@@ -21935,7 +21935,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P293" s="12" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="Q293" s="26" t="s">
         <v>282</v>
@@ -21999,7 +21999,7 @@
         <v>% reduction in cost</v>
       </c>
       <c r="P294" s="12" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="Q294" s="26" t="s">
         <v>282</v>
@@ -22055,7 +22055,7 @@
         <v>36</v>
       </c>
       <c r="P295" s="26" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="Q295" s="26" t="s">
         <v>282</v>
@@ -22119,7 +22119,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P296" s="26" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="Q296" s="26" t="s">
         <v>282</v>
@@ -22225,7 +22225,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P298" s="26" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="Q298" s="26" t="s">
         <v>282</v>
@@ -22289,7 +22289,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P299" s="26" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="Q299" s="26" t="s">
         <v>282</v>
@@ -22353,7 +22353,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P300" s="26" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="Q300" s="26" t="s">
         <v>282</v>
@@ -22409,7 +22409,7 @@
         <v>36</v>
       </c>
       <c r="P301" s="26" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="Q301" s="26" t="s">
         <v>282</v>
@@ -22467,7 +22467,7 @@
         <v>36</v>
       </c>
       <c r="P302" s="26" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="Q302" s="26" t="s">
         <v>282</v>
@@ -22531,7 +22531,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P303" s="26" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
       <c r="Q303" s="26" t="s">
         <v>282</v>
@@ -22595,7 +22595,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P304" s="26" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="Q304" s="26" t="s">
         <v>282</v>
@@ -22835,7 +22835,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P309" s="26" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="Q309" s="26" t="s">
         <v>282</v>
@@ -22899,7 +22899,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P310" s="26" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="Q310" s="26" t="s">
         <v>282</v>
@@ -22963,7 +22963,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P311" s="26" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
       <c r="Q311" s="26" t="s">
         <v>282</v>
@@ -23063,7 +23063,7 @@
         <v>36</v>
       </c>
       <c r="P313" s="26" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="Q313" s="26" t="s">
         <v>282</v>
@@ -23127,7 +23127,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P314" s="26" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="Q314" s="26" t="s">
         <v>282</v>
@@ -23191,7 +23191,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P315" s="26" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="Q315" s="26" t="s">
         <v>282</v>
@@ -23255,7 +23255,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P316" s="26" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="Q316" s="26" t="s">
         <v>282</v>
@@ -23319,7 +23319,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P317" s="26" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="Q317" s="26" t="s">
         <v>282</v>
@@ -23383,7 +23383,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P318" s="26" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="Q318" s="26" t="s">
         <v>282</v>
@@ -23447,7 +23447,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P319" s="26" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="Q319" s="26" t="s">
         <v>282</v>
@@ -23511,7 +23511,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P320" s="26" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="Q320" s="26" t="s">
         <v>282</v>
@@ -23569,7 +23569,7 @@
         <v>36</v>
       </c>
       <c r="P321" s="26" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="Q321" s="26" t="s">
         <v>282</v>
@@ -23633,7 +23633,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P322" s="26" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="Q322" s="26" t="s">
         <v>282</v>
@@ -23697,7 +23697,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P323" s="26" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="Q323" s="26" t="s">
         <v>282</v>
@@ -23761,7 +23761,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P324" s="26" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="Q324" s="26" t="s">
         <v>282</v>
@@ -23825,7 +23825,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P325" s="26" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="Q325" s="26" t="s">
         <v>282</v>
@@ -23889,7 +23889,7 @@
         <v>% reduction in fuel use</v>
       </c>
       <c r="P326" s="26" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="Q326" s="26" t="s">
         <v>282</v>
@@ -24044,8 +24044,8 @@
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24527,10 +24527,10 @@
         <v>422</v>
       </c>
       <c r="F21" s="52" t="s">
-        <v>1237</v>
+        <v>1387</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>1393</v>
+        <v>1386</v>
       </c>
       <c r="H21" s="72" t="s">
         <v>755</v>
@@ -24581,7 +24581,7 @@
         <v>427</v>
       </c>
       <c r="B24" s="102" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="C24" s="72" t="s">
         <v>74</v>
@@ -24593,7 +24593,7 @@
         <v>1126</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="H24" s="72"/>
     </row>
@@ -24654,7 +24654,7 @@
         <v>713</v>
       </c>
       <c r="B27" s="73" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>74</v>
@@ -24666,13 +24666,13 @@
         <v>1127</v>
       </c>
       <c r="F27" s="52" t="s">
-        <v>1253</v>
+        <v>1247</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
       <c r="H27" s="72" t="s">
-        <v>1255</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45">
@@ -24680,7 +24680,7 @@
         <v>713</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
       <c r="C28" s="72" t="s">
         <v>74</v>
@@ -24692,13 +24692,13 @@
         <v>1127</v>
       </c>
       <c r="F28" s="52" t="s">
-        <v>1256</v>
+        <v>1250</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>1257</v>
+        <v>1251</v>
       </c>
       <c r="H28" s="72" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="90">
@@ -24718,7 +24718,7 @@
         <v>1127</v>
       </c>
       <c r="F29" s="52" t="s">
-        <v>1259</v>
+        <v>1253</v>
       </c>
       <c r="G29" s="52" t="s">
         <v>782</v>
@@ -24786,10 +24786,10 @@
         <v>424</v>
       </c>
       <c r="F32" s="72" t="s">
-        <v>1238</v>
+        <v>1388</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="H32" s="72" t="s">
         <v>669</v>
@@ -24812,10 +24812,10 @@
         <v>424</v>
       </c>
       <c r="F33" s="72" t="s">
-        <v>1240</v>
+        <v>1389</v>
       </c>
       <c r="G33" s="52" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="H33" s="72" t="s">
         <v>670</v>
@@ -24838,10 +24838,10 @@
         <v>425</v>
       </c>
       <c r="F34" s="72" t="s">
-        <v>1242</v>
+        <v>1390</v>
       </c>
       <c r="G34" s="52" t="s">
-        <v>1243</v>
+        <v>1238</v>
       </c>
       <c r="H34" s="72" t="s">
         <v>476</v>
@@ -24864,10 +24864,10 @@
         <v>425</v>
       </c>
       <c r="F35" s="72" t="s">
-        <v>1244</v>
+        <v>1391</v>
       </c>
       <c r="G35" s="52" t="s">
-        <v>1245</v>
+        <v>1239</v>
       </c>
       <c r="H35" s="72" t="s">
         <v>477</v>
@@ -25358,10 +25358,10 @@
         <v>479</v>
       </c>
       <c r="F54" s="72" t="s">
-        <v>1236</v>
+        <v>1392</v>
       </c>
       <c r="G54" s="104" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="H54" s="72" t="s">
         <v>1205</v>
@@ -25540,13 +25540,13 @@
         <v>479</v>
       </c>
       <c r="F61" s="72" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="G61" s="52" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="H61" s="72" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -25575,7 +25575,7 @@
         <v>454</v>
       </c>
       <c r="B63" s="73" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>72</v>
@@ -25584,10 +25584,10 @@
         <v>73</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="F63" s="72" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="H63" s="72"/>
     </row>
@@ -25697,13 +25697,13 @@
         <v>1129</v>
       </c>
       <c r="F68" s="72" t="s">
-        <v>1387</v>
+        <v>1393</v>
       </c>
       <c r="G68" s="52" t="s">
-        <v>1388</v>
+        <v>1381</v>
       </c>
       <c r="H68" s="72" t="s">
-        <v>1389</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="75">
@@ -25775,13 +25775,13 @@
         <v>1131</v>
       </c>
       <c r="F71" s="72" t="s">
-        <v>1390</v>
+        <v>1383</v>
       </c>
       <c r="G71" s="52" t="s">
-        <v>1391</v>
+        <v>1384</v>
       </c>
       <c r="H71" s="72" t="s">
-        <v>1392</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="30">
@@ -25942,18 +25942,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Do not show "fixed electricity prices" Boolean lever in web interface (WebAppData)
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-california\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6534703-21C9-4FE0-AC47-1F3AFB26CFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="18960" windowHeight="5940" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,20 +24,30 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$T$326</definedName>
     <definedName name="Z_EACAC692_6FA5_4207_B9A8_44B823BD87B2_.wvu.FilterData" localSheetId="1" hidden="1">PolicyLevers!$A$1:$T$326</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Chris Busch - Personal View" guid="{EACAC692-6FA5-4207-B9A8-44B823BD87B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="434" activeSheetId="2"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jeffrey Rissman</author>
   </authors>
   <commentList>
-    <comment ref="K140" authorId="0">
+    <comment ref="K140" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K142" authorId="0">
+    <comment ref="K142" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,12 +100,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Chris Busch</author>
   </authors>
   <commentList>
-    <comment ref="G54" authorId="0">
+    <comment ref="G54" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -119,11 +135,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\OuputGraphSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\PolicyLeverSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -4321,7 +4337,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -5024,25 +5040,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="2x indented GHG Textfiels" xfId="10"/>
-    <cellStyle name="5x indented GHG Textfiels" xfId="11"/>
-    <cellStyle name="AggCels" xfId="12"/>
-    <cellStyle name="AggGreen_bld" xfId="15"/>
-    <cellStyle name="Body: normal cell 2" xfId="5"/>
-    <cellStyle name="Comma 6" xfId="6"/>
-    <cellStyle name="Constants" xfId="8"/>
-    <cellStyle name="CustomizationCells" xfId="17"/>
-    <cellStyle name="Empty_B_border" xfId="16"/>
-    <cellStyle name="Header: bottom row 2" xfId="4"/>
-    <cellStyle name="Headline" xfId="7"/>
+    <cellStyle name="2x indented GHG Textfiels" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="5x indented GHG Textfiels" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="AggCels" xfId="12" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="AggGreen_bld" xfId="15" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Constants" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="CustomizationCells" xfId="17" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Empty_B_border" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Headline" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="18"/>
-    <cellStyle name="Normal GHG Textfiels Bold" xfId="9"/>
-    <cellStyle name="Normal GHG-Shade" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal GHG Textfiels Bold" xfId="9" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal GHG-Shade" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Обычный_CRF2002 (1)" xfId="13"/>
+    <cellStyle name="Обычный_CRF2002 (1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -5288,7 +5304,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5349,7 +5365,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5410,7 +5426,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5471,7 +5487,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5786,14 +5802,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.86328125" style="11"/>
+    <col min="1" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5874,7 +5890,7 @@
     </customSheetView>
   </customSheetViews>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId2"/>
+    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -5882,39 +5898,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" style="5" customWidth="1"/>
-    <col min="2" max="2" width="28.3984375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.3984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.73046875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="8.265625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="8.1328125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.59765625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" style="23" customWidth="1"/>
-    <col min="9" max="9" width="21.265625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="21.265625" style="23" customWidth="1"/>
-    <col min="11" max="11" width="16.86328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="23" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" style="5" customWidth="1"/>
     <col min="12" max="12" width="19" style="5" customWidth="1"/>
-    <col min="13" max="14" width="19.1328125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="28.3984375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="117.265625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="52.3984375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="43.3984375" style="3" customWidth="1"/>
-    <col min="19" max="19" width="47.86328125" style="8" customWidth="1"/>
-    <col min="20" max="20" width="37.265625" style="9" customWidth="1"/>
-    <col min="21" max="16384" width="9.1328125" style="5"/>
+    <col min="13" max="14" width="19.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="117.28515625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="52.42578125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="43.42578125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="47.85546875" style="8" customWidth="1"/>
+    <col min="20" max="20" width="37.28515625" style="9" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="57">
+    <row r="1" spans="1:20" ht="60">
       <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
@@ -5976,7 +5992,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="2" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -6026,7 +6042,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="3" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A3" s="6" t="str">
         <f>A$2</f>
         <v>Transportation</v>
@@ -6086,7 +6102,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="4" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A4" s="6" t="str">
         <f t="shared" ref="A4:A7" si="2">A$2</f>
         <v>Transportation</v>
@@ -6146,7 +6162,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="5" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A5" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -6206,7 +6222,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
     </row>
-    <row r="6" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="6" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A6" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -6266,7 +6282,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="7" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A7" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Transportation</v>
@@ -6326,7 +6342,7 @@
         <v>conventional-pollutant-standards.html</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="8" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -6376,7 +6392,7 @@
       <c r="S8" s="47"/>
       <c r="T8" s="12"/>
     </row>
-    <row r="9" spans="1:20" s="3" customFormat="1" ht="99.75">
+    <row r="9" spans="1:20" s="3" customFormat="1" ht="120">
       <c r="A9" s="12" t="s">
         <v>4</v>
       </c>
@@ -6436,7 +6452,7 @@
       </c>
       <c r="T9" s="12"/>
     </row>
-    <row r="10" spans="1:20" s="3" customFormat="1" ht="156.75">
+    <row r="10" spans="1:20" s="3" customFormat="1" ht="195">
       <c r="A10" s="28" t="str">
         <f>A$9</f>
         <v>Transportation</v>
@@ -6503,7 +6519,7 @@
       <c r="S10" s="57"/>
       <c r="T10" s="12"/>
     </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" ht="114">
+    <row r="11" spans="1:20" s="3" customFormat="1" ht="135">
       <c r="A11" s="28" t="str">
         <f t="shared" ref="A11:A20" si="6">A$9</f>
         <v>Transportation</v>
@@ -6572,7 +6588,7 @@
       </c>
       <c r="T11" s="12"/>
     </row>
-    <row r="12" spans="1:20" s="3" customFormat="1" ht="114">
+    <row r="12" spans="1:20" s="3" customFormat="1" ht="135">
       <c r="A12" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6641,7 +6657,7 @@
       </c>
       <c r="T12" s="12"/>
     </row>
-    <row r="13" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="13" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A13" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6687,7 +6703,7 @@
       <c r="S13" s="104"/>
       <c r="T13" s="12"/>
     </row>
-    <row r="14" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="14" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A14" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6733,7 +6749,7 @@
       <c r="S14" s="57"/>
       <c r="T14" s="12"/>
     </row>
-    <row r="15" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="15" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A15" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6779,7 +6795,7 @@
       <c r="S15" s="57"/>
       <c r="T15" s="12"/>
     </row>
-    <row r="16" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="16" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A16" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6825,7 +6841,7 @@
       <c r="S16" s="57"/>
       <c r="T16" s="12"/>
     </row>
-    <row r="17" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="17" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A17" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6871,7 +6887,7 @@
       <c r="S17" s="57"/>
       <c r="T17" s="12"/>
     </row>
-    <row r="18" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="18" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A18" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6917,7 +6933,7 @@
       <c r="S18" s="57"/>
       <c r="T18" s="12"/>
     </row>
-    <row r="19" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="19" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A19" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -6985,7 +7001,7 @@
       <c r="S19" s="57"/>
       <c r="T19" s="12"/>
     </row>
-    <row r="20" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="20" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A20" s="28" t="str">
         <f t="shared" si="6"/>
         <v>Transportation</v>
@@ -7031,7 +7047,7 @@
       <c r="S20" s="57"/>
       <c r="T20" s="12"/>
     </row>
-    <row r="21" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="21" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A21" s="12" t="s">
         <v>4</v>
       </c>
@@ -7091,7 +7107,7 @@
       </c>
       <c r="T21" s="12"/>
     </row>
-    <row r="22" spans="1:20" s="52" customFormat="1" ht="57">
+    <row r="22" spans="1:20" s="52" customFormat="1" ht="60">
       <c r="A22" s="28" t="str">
         <f t="shared" ref="A22:C32" si="10">A$21</f>
         <v>Transportation</v>
@@ -7149,7 +7165,7 @@
       <c r="S22" s="58"/>
       <c r="T22" s="50"/>
     </row>
-    <row r="23" spans="1:20" s="52" customFormat="1" ht="57">
+    <row r="23" spans="1:20" s="52" customFormat="1" ht="60">
       <c r="A23" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7207,7 +7223,7 @@
       <c r="S23" s="58"/>
       <c r="T23" s="50"/>
     </row>
-    <row r="24" spans="1:20" s="52" customFormat="1">
+    <row r="24" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A24" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7253,7 +7269,7 @@
       <c r="S24" s="58"/>
       <c r="T24" s="50"/>
     </row>
-    <row r="25" spans="1:20" s="52" customFormat="1" ht="28.5">
+    <row r="25" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A25" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7299,7 +7315,7 @@
       <c r="S25" s="58"/>
       <c r="T25" s="50"/>
     </row>
-    <row r="26" spans="1:20" s="52" customFormat="1">
+    <row r="26" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A26" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7345,7 +7361,7 @@
       <c r="S26" s="58"/>
       <c r="T26" s="50"/>
     </row>
-    <row r="27" spans="1:20" s="52" customFormat="1" ht="28.5">
+    <row r="27" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A27" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7391,7 +7407,7 @@
       <c r="S27" s="58"/>
       <c r="T27" s="50"/>
     </row>
-    <row r="28" spans="1:20" s="52" customFormat="1">
+    <row r="28" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A28" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7437,7 +7453,7 @@
       <c r="S28" s="58"/>
       <c r="T28" s="50"/>
     </row>
-    <row r="29" spans="1:20" s="52" customFormat="1" ht="28.5">
+    <row r="29" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A29" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7483,7 +7499,7 @@
       <c r="S29" s="58"/>
       <c r="T29" s="50"/>
     </row>
-    <row r="30" spans="1:20" s="52" customFormat="1">
+    <row r="30" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A30" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7529,7 +7545,7 @@
       <c r="S30" s="58"/>
       <c r="T30" s="50"/>
     </row>
-    <row r="31" spans="1:20" s="52" customFormat="1" ht="28.5">
+    <row r="31" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A31" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7575,7 +7591,7 @@
       <c r="S31" s="58"/>
       <c r="T31" s="50"/>
     </row>
-    <row r="32" spans="1:20" s="52" customFormat="1" ht="28.5">
+    <row r="32" spans="1:20" s="52" customFormat="1" ht="30">
       <c r="A32" s="28" t="str">
         <f t="shared" si="10"/>
         <v>Transportation</v>
@@ -7621,7 +7637,7 @@
       <c r="S32" s="58"/>
       <c r="T32" s="50"/>
     </row>
-    <row r="33" spans="1:20" ht="85.5">
+    <row r="33" spans="1:20" ht="105">
       <c r="A33" s="26" t="s">
         <v>4</v>
       </c>
@@ -7675,7 +7691,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="42.75">
+    <row r="34" spans="1:20" ht="45">
       <c r="A34" s="26" t="s">
         <v>4</v>
       </c>
@@ -7714,7 +7730,7 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="1:20" ht="28.5">
+    <row r="35" spans="1:20" ht="45">
       <c r="A35" s="28" t="str">
         <f t="shared" ref="A35:C49" si="12">A$34</f>
         <v>Transportation</v>
@@ -7840,7 +7856,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="42.75">
+    <row r="37" spans="1:20" ht="45">
       <c r="A37" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -7907,7 +7923,7 @@
       <c r="S37" s="54"/>
       <c r="T37" s="26"/>
     </row>
-    <row r="38" spans="1:20" ht="42.75">
+    <row r="38" spans="1:20" ht="45">
       <c r="A38" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -7967,7 +7983,7 @@
       <c r="S38" s="54"/>
       <c r="T38" s="26"/>
     </row>
-    <row r="39" spans="1:20" ht="28.5">
+    <row r="39" spans="1:20" ht="45">
       <c r="A39" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8013,7 +8029,7 @@
       <c r="S39" s="54"/>
       <c r="T39" s="26"/>
     </row>
-    <row r="40" spans="1:20" ht="42.75">
+    <row r="40" spans="1:20" ht="45">
       <c r="A40" s="28" t="str">
         <f>A$34</f>
         <v>Transportation</v>
@@ -8056,7 +8072,7 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="1:20" ht="42.75">
+    <row r="41" spans="1:20" ht="45">
       <c r="A41" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8114,7 +8130,7 @@
       <c r="S41" s="54"/>
       <c r="T41" s="26"/>
     </row>
-    <row r="42" spans="1:20" ht="42.75">
+    <row r="42" spans="1:20" ht="45">
       <c r="A42" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8252,7 +8268,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="42.75">
+    <row r="44" spans="1:20" ht="45">
       <c r="A44" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8298,7 +8314,7 @@
       <c r="S44" s="54"/>
       <c r="T44" s="26"/>
     </row>
-    <row r="45" spans="1:20" ht="28.5">
+    <row r="45" spans="1:20" ht="45">
       <c r="A45" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8344,7 +8360,7 @@
       <c r="S45" s="54"/>
       <c r="T45" s="26"/>
     </row>
-    <row r="46" spans="1:20" ht="42.75">
+    <row r="46" spans="1:20" ht="45">
       <c r="A46" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8387,7 +8403,7 @@
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" spans="1:20" ht="28.5">
+    <row r="47" spans="1:20" ht="45">
       <c r="A47" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8433,7 +8449,7 @@
       <c r="S47" s="54"/>
       <c r="T47" s="26"/>
     </row>
-    <row r="48" spans="1:20" ht="28.5">
+    <row r="48" spans="1:20" ht="45">
       <c r="A48" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8479,7 +8495,7 @@
       <c r="S48" s="54"/>
       <c r="T48" s="26"/>
     </row>
-    <row r="49" spans="1:20" ht="28.5">
+    <row r="49" spans="1:20" ht="45">
       <c r="A49" s="28" t="str">
         <f t="shared" si="12"/>
         <v>Transportation</v>
@@ -8525,7 +8541,7 @@
       <c r="S49" s="54"/>
       <c r="T49" s="26"/>
     </row>
-    <row r="50" spans="1:20" ht="42.75">
+    <row r="50" spans="1:20" ht="45">
       <c r="A50" s="28" t="str">
         <f t="shared" ref="A50:C69" si="16">A$34</f>
         <v>Transportation</v>
@@ -8642,7 +8658,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="42.75">
+    <row r="52" spans="1:20" ht="45">
       <c r="A52" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8685,7 +8701,7 @@
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
     </row>
-    <row r="53" spans="1:20" ht="28.5">
+    <row r="53" spans="1:20" ht="45">
       <c r="A53" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8731,7 +8747,7 @@
       <c r="S53" s="54"/>
       <c r="T53" s="26"/>
     </row>
-    <row r="54" spans="1:20" ht="28.5">
+    <row r="54" spans="1:20" ht="45">
       <c r="A54" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8777,7 +8793,7 @@
       <c r="S54" s="54"/>
       <c r="T54" s="26"/>
     </row>
-    <row r="55" spans="1:20" ht="28.5">
+    <row r="55" spans="1:20" ht="45">
       <c r="A55" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8823,7 +8839,7 @@
       <c r="S55" s="54"/>
       <c r="T55" s="26"/>
     </row>
-    <row r="56" spans="1:20" ht="42.75">
+    <row r="56" spans="1:20" ht="45">
       <c r="A56" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8869,7 +8885,7 @@
       <c r="S56" s="54"/>
       <c r="T56" s="26"/>
     </row>
-    <row r="57" spans="1:20" ht="71.25">
+    <row r="57" spans="1:20" ht="75">
       <c r="A57" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8940,7 +8956,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="42.75">
+    <row r="58" spans="1:20" ht="45">
       <c r="A58" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -8983,7 +8999,7 @@
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
     </row>
-    <row r="59" spans="1:20" ht="28.5">
+    <row r="59" spans="1:20" ht="45">
       <c r="A59" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9029,7 +9045,7 @@
       <c r="S59" s="54"/>
       <c r="T59" s="26"/>
     </row>
-    <row r="60" spans="1:20" ht="28.5">
+    <row r="60" spans="1:20" ht="45">
       <c r="A60" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9075,7 +9091,7 @@
       <c r="S60" s="54"/>
       <c r="T60" s="26"/>
     </row>
-    <row r="61" spans="1:20" ht="28.5">
+    <row r="61" spans="1:20" ht="45">
       <c r="A61" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9121,7 +9137,7 @@
       <c r="S61" s="54"/>
       <c r="T61" s="26"/>
     </row>
-    <row r="62" spans="1:20" ht="42.75">
+    <row r="62" spans="1:20" ht="45">
       <c r="A62" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9167,7 +9183,7 @@
       <c r="S62" s="54"/>
       <c r="T62" s="26"/>
     </row>
-    <row r="63" spans="1:20" ht="99.75">
+    <row r="63" spans="1:20" ht="120">
       <c r="A63" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9238,7 +9254,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="42.75">
+    <row r="64" spans="1:20" ht="45">
       <c r="A64" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9281,7 +9297,7 @@
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
     </row>
-    <row r="65" spans="1:20" ht="28.5">
+    <row r="65" spans="1:20" ht="45">
       <c r="A65" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9327,7 +9343,7 @@
       <c r="S65" s="54"/>
       <c r="T65" s="26"/>
     </row>
-    <row r="66" spans="1:20" ht="99.75">
+    <row r="66" spans="1:20" ht="120">
       <c r="A66" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9398,7 +9414,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="28.5">
+    <row r="67" spans="1:20" ht="45">
       <c r="A67" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9444,7 +9460,7 @@
       <c r="S67" s="54"/>
       <c r="T67" s="26"/>
     </row>
-    <row r="68" spans="1:20" ht="42.75">
+    <row r="68" spans="1:20" ht="45">
       <c r="A68" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9490,7 +9506,7 @@
       <c r="S68" s="54"/>
       <c r="T68" s="26"/>
     </row>
-    <row r="69" spans="1:20" ht="28.5">
+    <row r="69" spans="1:20" ht="45">
       <c r="A69" s="28" t="str">
         <f t="shared" si="16"/>
         <v>Transportation</v>
@@ -9536,7 +9552,7 @@
       <c r="S69" s="54"/>
       <c r="T69" s="26"/>
     </row>
-    <row r="70" spans="1:20" s="3" customFormat="1" ht="99.75">
+    <row r="70" spans="1:20" s="3" customFormat="1" ht="105">
       <c r="A70" s="12" t="s">
         <v>4</v>
       </c>
@@ -9590,7 +9606,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="57">
+    <row r="71" spans="1:20" ht="60">
       <c r="A71" s="26" t="s">
         <v>4</v>
       </c>
@@ -9713,7 +9729,7 @@
       </c>
       <c r="T72" s="26"/>
     </row>
-    <row r="73" spans="1:20" ht="42.75">
+    <row r="73" spans="1:20" ht="45">
       <c r="A73" s="26" t="s">
         <v>80</v>
       </c>
@@ -9767,7 +9783,7 @@
       <c r="S73" s="54"/>
       <c r="T73" s="26"/>
     </row>
-    <row r="74" spans="1:20" ht="28.5">
+    <row r="74" spans="1:20" ht="45">
       <c r="A74" s="28" t="str">
         <f>A$73</f>
         <v>Buildings and Appliances</v>
@@ -9831,7 +9847,7 @@
       <c r="S74" s="56"/>
       <c r="T74" s="31"/>
     </row>
-    <row r="75" spans="1:20" ht="28.5">
+    <row r="75" spans="1:20" ht="45">
       <c r="A75" s="28" t="str">
         <f>A$73</f>
         <v>Buildings and Appliances</v>
@@ -11278,7 +11294,7 @@
 RESIDENTIAL SECTOR," http://www.energy.ca.gov/2007publications/CEC-500-2007-002/CEC-500-2007-002.PDF, p.33, Table 5-1</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="6" customFormat="1" ht="42.75">
+    <row r="94" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A94" s="26" t="s">
         <v>80</v>
       </c>
@@ -11437,7 +11453,7 @@
       </c>
       <c r="T96" s="28"/>
     </row>
-    <row r="97" spans="1:23" s="6" customFormat="1" ht="71.25">
+    <row r="97" spans="1:23" s="6" customFormat="1" ht="90">
       <c r="A97" s="26" t="s">
         <v>80</v>
       </c>
@@ -11490,7 +11506,7 @@
       <c r="T97" s="28"/>
       <c r="W97" s="100"/>
     </row>
-    <row r="98" spans="1:23" s="6" customFormat="1" ht="99.75">
+    <row r="98" spans="1:23" s="6" customFormat="1" ht="120">
       <c r="A98" s="26" t="s">
         <v>80</v>
       </c>
@@ -11549,7 +11565,7 @@
       </c>
       <c r="W98" s="71"/>
     </row>
-    <row r="99" spans="1:23" s="6" customFormat="1" ht="85.5">
+    <row r="99" spans="1:23" s="6" customFormat="1" ht="105">
       <c r="A99" s="28" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -11615,7 +11631,7 @@
       <c r="T99" s="28"/>
       <c r="W99" s="71"/>
     </row>
-    <row r="100" spans="1:23" s="6" customFormat="1" ht="85.5">
+    <row r="100" spans="1:23" s="6" customFormat="1" ht="105">
       <c r="A100" s="28" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -11681,7 +11697,7 @@
       <c r="T100" s="28"/>
       <c r="W100" s="11"/>
     </row>
-    <row r="101" spans="1:23" s="6" customFormat="1" ht="85.5">
+    <row r="101" spans="1:23" s="6" customFormat="1" ht="105">
       <c r="A101" s="28" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -11744,7 +11760,7 @@
       </c>
       <c r="T101" s="28"/>
     </row>
-    <row r="102" spans="1:23" s="6" customFormat="1" ht="85.5">
+    <row r="102" spans="1:23" s="6" customFormat="1" ht="90">
       <c r="A102" s="28" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -11809,7 +11825,7 @@
       </c>
       <c r="T102" s="28"/>
     </row>
-    <row r="103" spans="1:23" s="6" customFormat="1" ht="85.5">
+    <row r="103" spans="1:23" s="6" customFormat="1" ht="105">
       <c r="A103" s="28" t="str">
         <f>A$98</f>
         <v>Buildings and Appliances</v>
@@ -11874,7 +11890,7 @@
       </c>
       <c r="T103" s="28"/>
     </row>
-    <row r="104" spans="1:23" s="6" customFormat="1" ht="28.5">
+    <row r="104" spans="1:23" s="6" customFormat="1" ht="30">
       <c r="A104" s="26" t="s">
         <v>80</v>
       </c>
@@ -11930,7 +11946,7 @@
       </c>
       <c r="T104" s="28"/>
     </row>
-    <row r="105" spans="1:23" s="6" customFormat="1" ht="57">
+    <row r="105" spans="1:23" s="6" customFormat="1" ht="60">
       <c r="A105" s="28" t="str">
         <f>A$104</f>
         <v>Buildings and Appliances</v>
@@ -11994,7 +12010,7 @@
       </c>
       <c r="T105" s="28"/>
     </row>
-    <row r="106" spans="1:23" s="6" customFormat="1" ht="28.5">
+    <row r="106" spans="1:23" s="6" customFormat="1" ht="30">
       <c r="A106" s="28" t="str">
         <f>A$104</f>
         <v>Buildings and Appliances</v>
@@ -12038,7 +12054,7 @@
       <c r="S106" s="59"/>
       <c r="T106" s="28"/>
     </row>
-    <row r="107" spans="1:23" s="6" customFormat="1" ht="28.5">
+    <row r="107" spans="1:23" s="6" customFormat="1" ht="30">
       <c r="A107" s="28" t="str">
         <f>A$104</f>
         <v>Buildings and Appliances</v>
@@ -12082,7 +12098,7 @@
       <c r="S107" s="59"/>
       <c r="T107" s="28"/>
     </row>
-    <row r="108" spans="1:23" s="6" customFormat="1" ht="28.5">
+    <row r="108" spans="1:23" s="6" customFormat="1" ht="30">
       <c r="A108" s="28" t="str">
         <f>A$104</f>
         <v>Buildings and Appliances</v>
@@ -12146,7 +12162,7 @@
       </c>
       <c r="T108" s="28"/>
     </row>
-    <row r="109" spans="1:23" s="6" customFormat="1" ht="42.75">
+    <row r="109" spans="1:23" s="6" customFormat="1" ht="45">
       <c r="A109" s="28" t="str">
         <f>A$104</f>
         <v>Buildings and Appliances</v>
@@ -12190,7 +12206,7 @@
       <c r="S109" s="59"/>
       <c r="T109" s="28"/>
     </row>
-    <row r="110" spans="1:23" s="3" customFormat="1" ht="28.5">
+    <row r="110" spans="1:23" s="3" customFormat="1" ht="30">
       <c r="A110" s="12" t="s">
         <v>7</v>
       </c>
@@ -12244,7 +12260,7 @@
       <c r="S110" s="60"/>
       <c r="T110" s="12"/>
     </row>
-    <row r="111" spans="1:23" s="6" customFormat="1" ht="57">
+    <row r="111" spans="1:23" s="6" customFormat="1" ht="60">
       <c r="A111" s="28" t="str">
         <f>A$110</f>
         <v>Electricity Supply</v>
@@ -12308,7 +12324,7 @@
       <c r="S111" s="59"/>
       <c r="T111" s="28"/>
     </row>
-    <row r="112" spans="1:23" s="6" customFormat="1" ht="28.5">
+    <row r="112" spans="1:23" s="6" customFormat="1" ht="30">
       <c r="A112" s="28" t="str">
         <f t="shared" ref="A112:C121" si="40">A$110</f>
         <v>Electricity Supply</v>
@@ -12372,7 +12388,7 @@
       <c r="S112" s="59"/>
       <c r="T112" s="28"/>
     </row>
-    <row r="113" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="113" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A113" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12436,7 +12452,7 @@
       <c r="S113" s="59"/>
       <c r="T113" s="28"/>
     </row>
-    <row r="114" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="114" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A114" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12478,7 +12494,7 @@
       <c r="S114" s="59"/>
       <c r="T114" s="28"/>
     </row>
-    <row r="115" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="115" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A115" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12520,7 +12536,7 @@
       <c r="S115" s="59"/>
       <c r="T115" s="28"/>
     </row>
-    <row r="116" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="116" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A116" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12562,7 +12578,7 @@
       <c r="S116" s="59"/>
       <c r="T116" s="28"/>
     </row>
-    <row r="117" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="117" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A117" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12604,7 +12620,7 @@
       <c r="S117" s="59"/>
       <c r="T117" s="28"/>
     </row>
-    <row r="118" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="118" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A118" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12646,7 +12662,7 @@
       <c r="S118" s="59"/>
       <c r="T118" s="28"/>
     </row>
-    <row r="119" spans="1:20" s="6" customFormat="1" ht="42.75">
+    <row r="119" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A119" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12688,7 +12704,7 @@
       <c r="S119" s="59"/>
       <c r="T119" s="28"/>
     </row>
-    <row r="120" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="120" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A120" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12750,7 +12766,7 @@
       <c r="S120" s="59"/>
       <c r="T120" s="28"/>
     </row>
-    <row r="121" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="121" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A121" s="28" t="str">
         <f t="shared" si="40"/>
         <v>Electricity Supply</v>
@@ -12792,7 +12808,7 @@
       <c r="S121" s="59"/>
       <c r="T121" s="28"/>
     </row>
-    <row r="122" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="122" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A122" s="12" t="s">
         <v>7</v>
       </c>
@@ -12844,7 +12860,7 @@
       </c>
       <c r="T122" s="12"/>
     </row>
-    <row r="123" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="123" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A123" s="12" t="s">
         <v>7</v>
       </c>
@@ -12896,7 +12912,7 @@
       </c>
       <c r="T123" s="12"/>
     </row>
-    <row r="124" spans="1:20" ht="42.75">
+    <row r="124" spans="1:20" ht="45">
       <c r="A124" s="26" t="s">
         <v>7</v>
       </c>
@@ -12932,7 +12948,7 @@
       <c r="S124" s="54"/>
       <c r="T124" s="26"/>
     </row>
-    <row r="125" spans="1:20" ht="85.5">
+    <row r="125" spans="1:20" ht="90">
       <c r="A125" s="26" t="s">
         <v>7</v>
       </c>
@@ -13044,7 +13060,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="57">
+    <row r="127" spans="1:20" ht="60">
       <c r="A127" s="28" t="str">
         <f t="shared" ref="A127:C137" si="43">A$126</f>
         <v>Electricity Supply</v>
@@ -13088,7 +13104,7 @@
       <c r="S127" s="54"/>
       <c r="T127" s="26"/>
     </row>
-    <row r="128" spans="1:20" ht="42.75">
+    <row r="128" spans="1:20" ht="45">
       <c r="A128" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13152,7 +13168,7 @@
       </c>
       <c r="T128" s="26"/>
     </row>
-    <row r="129" spans="1:20" ht="42.75">
+    <row r="129" spans="1:20" ht="45">
       <c r="A129" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13196,7 +13212,7 @@
       <c r="S129" s="54"/>
       <c r="T129" s="26"/>
     </row>
-    <row r="130" spans="1:20" ht="42.75">
+    <row r="130" spans="1:20" ht="45">
       <c r="A130" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13240,7 +13256,7 @@
       <c r="S130" s="54"/>
       <c r="T130" s="26"/>
     </row>
-    <row r="131" spans="1:20" ht="42.75">
+    <row r="131" spans="1:20" ht="45">
       <c r="A131" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13284,7 +13300,7 @@
       <c r="S131" s="54"/>
       <c r="T131" s="26"/>
     </row>
-    <row r="132" spans="1:20" ht="42.75">
+    <row r="132" spans="1:20" ht="45">
       <c r="A132" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13328,7 +13344,7 @@
       <c r="S132" s="54"/>
       <c r="T132" s="26"/>
     </row>
-    <row r="133" spans="1:20" ht="42.75">
+    <row r="133" spans="1:20" ht="45">
       <c r="A133" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13372,7 +13388,7 @@
       <c r="S133" s="54"/>
       <c r="T133" s="26"/>
     </row>
-    <row r="134" spans="1:20" ht="42.75">
+    <row r="134" spans="1:20" ht="45">
       <c r="A134" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13414,7 +13430,7 @@
       <c r="S134" s="54"/>
       <c r="T134" s="26"/>
     </row>
-    <row r="135" spans="1:20" ht="42.75">
+    <row r="135" spans="1:20" ht="45">
       <c r="A135" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13456,7 +13472,7 @@
       <c r="S135" s="54"/>
       <c r="T135" s="26"/>
     </row>
-    <row r="136" spans="1:20" ht="42.75">
+    <row r="136" spans="1:20" ht="45">
       <c r="A136" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13498,7 +13514,7 @@
       <c r="S136" s="54"/>
       <c r="T136" s="26"/>
     </row>
-    <row r="137" spans="1:20" ht="42.75">
+    <row r="137" spans="1:20" ht="45">
       <c r="A137" s="28" t="str">
         <f t="shared" si="43"/>
         <v>Electricity Supply</v>
@@ -13648,7 +13664,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="140" spans="1:20" s="6" customFormat="1" ht="85.5">
+    <row r="140" spans="1:20" s="6" customFormat="1" ht="90">
       <c r="A140" s="26" t="s">
         <v>7</v>
       </c>
@@ -13698,7 +13714,7 @@
       </c>
       <c r="T140" s="28"/>
     </row>
-    <row r="141" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="141" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A141" s="26" t="s">
         <v>7</v>
       </c>
@@ -13734,7 +13750,7 @@
       <c r="S141" s="59"/>
       <c r="T141" s="28"/>
     </row>
-    <row r="142" spans="1:20" s="6" customFormat="1" ht="85.5">
+    <row r="142" spans="1:20" s="6" customFormat="1" ht="90">
       <c r="A142" s="26" t="s">
         <v>7</v>
       </c>
@@ -13786,7 +13802,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="143" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A143" s="12" t="s">
         <v>7</v>
       </c>
@@ -13824,7 +13840,7 @@
       <c r="S143" s="60"/>
       <c r="T143" s="12"/>
     </row>
-    <row r="144" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="144" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A144" s="30" t="str">
         <f t="shared" ref="A144:C173" si="45">A$143</f>
         <v>Electricity Supply</v>
@@ -13866,7 +13882,7 @@
       <c r="S144" s="60"/>
       <c r="T144" s="12"/>
     </row>
-    <row r="145" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="145" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A145" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -13908,7 +13924,7 @@
       <c r="S145" s="60"/>
       <c r="T145" s="12"/>
     </row>
-    <row r="146" spans="1:20" s="3" customFormat="1" ht="71.25">
+    <row r="146" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A146" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -13972,7 +13988,7 @@
       </c>
       <c r="T146" s="12"/>
     </row>
-    <row r="147" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="147" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A147" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14014,7 +14030,7 @@
       <c r="S147" s="60"/>
       <c r="T147" s="12"/>
     </row>
-    <row r="148" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="148" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A148" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14056,7 +14072,7 @@
       <c r="S148" s="60"/>
       <c r="T148" s="12"/>
     </row>
-    <row r="149" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="149" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A149" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14098,7 +14114,7 @@
       <c r="S149" s="60"/>
       <c r="T149" s="12"/>
     </row>
-    <row r="150" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="150" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A150" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14140,7 +14156,7 @@
       <c r="S150" s="60"/>
       <c r="T150" s="12"/>
     </row>
-    <row r="151" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="151" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A151" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14182,7 +14198,7 @@
       <c r="S151" s="60"/>
       <c r="T151" s="12"/>
     </row>
-    <row r="152" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="152" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A152" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14224,7 +14240,7 @@
       <c r="S152" s="60"/>
       <c r="T152" s="12"/>
     </row>
-    <row r="153" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="153" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A153" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14266,7 +14282,7 @@
       <c r="S153" s="60"/>
       <c r="T153" s="12"/>
     </row>
-    <row r="154" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="154" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A154" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14308,7 +14324,7 @@
       <c r="S154" s="60"/>
       <c r="T154" s="12"/>
     </row>
-    <row r="155" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="155" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A155" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14350,7 +14366,7 @@
       <c r="S155" s="60"/>
       <c r="T155" s="12"/>
     </row>
-    <row r="156" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="156" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A156" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14392,7 +14408,7 @@
       <c r="S156" s="60"/>
       <c r="T156" s="12"/>
     </row>
-    <row r="157" spans="1:20" s="3" customFormat="1" ht="71.25">
+    <row r="157" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A157" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14456,7 +14472,7 @@
       </c>
       <c r="T157" s="12"/>
     </row>
-    <row r="158" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="158" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A158" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14498,7 +14514,7 @@
       <c r="S158" s="60"/>
       <c r="T158" s="12"/>
     </row>
-    <row r="159" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="159" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A159" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14540,7 +14556,7 @@
       <c r="S159" s="60"/>
       <c r="T159" s="12"/>
     </row>
-    <row r="160" spans="1:20" s="3" customFormat="1" ht="71.25">
+    <row r="160" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A160" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14604,7 +14620,7 @@
       </c>
       <c r="T160" s="12"/>
     </row>
-    <row r="161" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="161" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A161" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14646,7 +14662,7 @@
       <c r="S161" s="60"/>
       <c r="T161" s="12"/>
     </row>
-    <row r="162" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="162" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A162" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14688,7 +14704,7 @@
       <c r="S162" s="60"/>
       <c r="T162" s="12"/>
     </row>
-    <row r="163" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="163" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A163" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14730,7 +14746,7 @@
       <c r="S163" s="60"/>
       <c r="T163" s="12"/>
     </row>
-    <row r="164" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="164" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A164" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14772,7 +14788,7 @@
       <c r="S164" s="60"/>
       <c r="T164" s="12"/>
     </row>
-    <row r="165" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="165" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A165" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14814,7 +14830,7 @@
       <c r="S165" s="60"/>
       <c r="T165" s="12"/>
     </row>
-    <row r="166" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="166" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A166" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14856,7 +14872,7 @@
       <c r="S166" s="60"/>
       <c r="T166" s="12"/>
     </row>
-    <row r="167" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="167" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A167" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14898,7 +14914,7 @@
       <c r="S167" s="60"/>
       <c r="T167" s="12"/>
     </row>
-    <row r="168" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="168" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A168" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14940,7 +14956,7 @@
       <c r="S168" s="60"/>
       <c r="T168" s="12"/>
     </row>
-    <row r="169" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="169" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A169" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -14982,7 +14998,7 @@
       <c r="S169" s="60"/>
       <c r="T169" s="12"/>
     </row>
-    <row r="170" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="170" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A170" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -15024,7 +15040,7 @@
       <c r="S170" s="60"/>
       <c r="T170" s="12"/>
     </row>
-    <row r="171" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="171" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A171" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -15066,7 +15082,7 @@
       <c r="S171" s="60"/>
       <c r="T171" s="12"/>
     </row>
-    <row r="172" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="172" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A172" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -15108,7 +15124,7 @@
       <c r="S172" s="60"/>
       <c r="T172" s="12"/>
     </row>
-    <row r="173" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="173" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A173" s="30" t="str">
         <f t="shared" si="45"/>
         <v>Electricity Supply</v>
@@ -15150,7 +15166,7 @@
       <c r="S173" s="60"/>
       <c r="T173" s="12"/>
     </row>
-    <row r="174" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="174" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A174" s="30" t="str">
         <f t="shared" ref="A174:C178" si="47">A$143</f>
         <v>Electricity Supply</v>
@@ -15192,7 +15208,7 @@
       <c r="S174" s="60"/>
       <c r="T174" s="12"/>
     </row>
-    <row r="175" spans="1:20" s="3" customFormat="1" ht="28.5">
+    <row r="175" spans="1:20" s="3" customFormat="1" ht="30">
       <c r="A175" s="30" t="str">
         <f t="shared" si="47"/>
         <v>Electricity Supply</v>
@@ -15234,7 +15250,7 @@
       <c r="S175" s="60"/>
       <c r="T175" s="12"/>
     </row>
-    <row r="176" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="176" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A176" s="30" t="str">
         <f t="shared" si="47"/>
         <v>Electricity Supply</v>
@@ -15276,7 +15292,7 @@
       <c r="S176" s="60"/>
       <c r="T176" s="12"/>
     </row>
-    <row r="177" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="177" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A177" s="30" t="str">
         <f t="shared" si="47"/>
         <v>Electricity Supply</v>
@@ -15318,7 +15334,7 @@
       <c r="S177" s="60"/>
       <c r="T177" s="12"/>
     </row>
-    <row r="178" spans="1:20" s="3" customFormat="1" ht="71.25">
+    <row r="178" spans="1:20" s="3" customFormat="1" ht="90">
       <c r="A178" s="30" t="str">
         <f t="shared" si="47"/>
         <v>Electricity Supply</v>
@@ -15382,7 +15398,7 @@
       </c>
       <c r="T178" s="12"/>
     </row>
-    <row r="179" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="179" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A179" s="12" t="s">
         <v>7</v>
       </c>
@@ -15436,7 +15452,7 @@
       <c r="S179" s="60"/>
       <c r="T179" s="12"/>
     </row>
-    <row r="180" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="180" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A180" s="30" t="str">
         <f>A$179</f>
         <v>Electricity Supply</v>
@@ -15500,7 +15516,7 @@
       <c r="S180" s="60"/>
       <c r="T180" s="12"/>
     </row>
-    <row r="181" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="181" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A181" s="30" t="str">
         <f>A$179</f>
         <v>Electricity Supply</v>
@@ -15564,7 +15580,7 @@
       <c r="S181" s="60"/>
       <c r="T181" s="12"/>
     </row>
-    <row r="182" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="182" spans="1:20" s="3" customFormat="1" ht="45">
       <c r="A182" s="12" t="s">
         <v>7</v>
       </c>
@@ -15668,7 +15684,7 @@
       </c>
       <c r="T183" s="26"/>
     </row>
-    <row r="184" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="184" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A184" s="26" t="s">
         <v>7</v>
       </c>
@@ -15708,7 +15724,7 @@
       <c r="S184" s="60"/>
       <c r="T184" s="28"/>
     </row>
-    <row r="185" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="185" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A185" s="28" t="str">
         <f t="shared" ref="A185:C193" si="52">A$184</f>
         <v>Electricity Supply</v>
@@ -15752,7 +15768,7 @@
       <c r="S185" s="60"/>
       <c r="T185" s="28"/>
     </row>
-    <row r="186" spans="1:20" s="6" customFormat="1" ht="128.25">
+    <row r="186" spans="1:20" s="6" customFormat="1" ht="135">
       <c r="A186" s="28" t="str">
         <f t="shared" si="52"/>
         <v>Electricity Supply</v>
@@ -15812,7 +15828,7 @@
       </c>
       <c r="T186" s="26"/>
     </row>
-    <row r="187" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="187" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A187" s="28" t="str">
         <f t="shared" si="52"/>
         <v>Electricity Supply</v>
@@ -16114,7 +16130,7 @@
       </c>
       <c r="T191" s="26"/>
     </row>
-    <row r="192" spans="1:20" ht="28.5">
+    <row r="192" spans="1:20" ht="30">
       <c r="A192" s="28" t="str">
         <f t="shared" si="52"/>
         <v>Electricity Supply</v>
@@ -16221,7 +16237,7 @@
       </c>
       <c r="T193" s="26"/>
     </row>
-    <row r="194" spans="1:20" ht="71.25">
+    <row r="194" spans="1:20" ht="90">
       <c r="A194" s="26" t="s">
         <v>8</v>
       </c>
@@ -16273,7 +16289,7 @@
       </c>
       <c r="T194" s="26"/>
     </row>
-    <row r="195" spans="1:20" s="6" customFormat="1" ht="42.75">
+    <row r="195" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A195" s="26" t="s">
         <v>8</v>
       </c>
@@ -16325,7 +16341,7 @@
       </c>
       <c r="T195" s="28"/>
     </row>
-    <row r="196" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="196" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A196" s="26" t="s">
         <v>8</v>
       </c>
@@ -16377,7 +16393,7 @@
       </c>
       <c r="T196" s="28"/>
     </row>
-    <row r="197" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="197" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A197" s="26" t="s">
         <v>8</v>
       </c>
@@ -16435,7 +16451,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="198" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="198" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A198" s="28" t="str">
         <f>A$197</f>
         <v>Industry</v>
@@ -16502,7 +16518,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="199" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="199" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A199" s="28" t="str">
         <f t="shared" ref="A199:A204" si="59">A$197</f>
         <v>Industry</v>
@@ -16570,7 +16586,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="200" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="200" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A200" s="28" t="str">
         <f t="shared" si="59"/>
         <v>Industry</v>
@@ -16638,7 +16654,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="201" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="201" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A201" s="28" t="str">
         <f t="shared" si="59"/>
         <v>Industry</v>
@@ -16706,7 +16722,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="202" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="202" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A202" s="28" t="str">
         <f t="shared" si="59"/>
         <v>Industry</v>
@@ -16772,7 +16788,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="57">
+    <row r="203" spans="1:20" ht="60">
       <c r="A203" s="28" t="str">
         <f t="shared" si="59"/>
         <v>Industry</v>
@@ -16840,7 +16856,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="204" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="204" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A204" s="28" t="str">
         <f t="shared" si="59"/>
         <v>Industry</v>
@@ -16908,7 +16924,7 @@
         <v>https://ww3.arb.ca.gov/cc/scopingplan/2030sp_appd_pathways_final.pdf</v>
       </c>
     </row>
-    <row r="205" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="205" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A205" s="26" t="s">
         <v>8</v>
       </c>
@@ -16958,7 +16974,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="57">
+    <row r="206" spans="1:20" ht="60">
       <c r="A206" s="26" t="s">
         <v>8</v>
       </c>
@@ -17010,7 +17026,7 @@
       </c>
       <c r="T206" s="26"/>
     </row>
-    <row r="207" spans="1:20" ht="57">
+    <row r="207" spans="1:20" ht="60">
       <c r="A207" s="26" t="s">
         <v>8</v>
       </c>
@@ -17064,7 +17080,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="71.25">
+    <row r="208" spans="1:20" ht="90">
       <c r="A208" s="26" t="s">
         <v>8</v>
       </c>
@@ -17116,7 +17132,7 @@
       </c>
       <c r="T208" s="26"/>
     </row>
-    <row r="209" spans="1:20" ht="57">
+    <row r="209" spans="1:20" ht="60">
       <c r="A209" s="26" t="s">
         <v>8</v>
       </c>
@@ -17168,7 +17184,7 @@
       </c>
       <c r="T209" s="26"/>
     </row>
-    <row r="210" spans="1:20" ht="71.25">
+    <row r="210" spans="1:20" ht="90">
       <c r="A210" s="26" t="s">
         <v>8</v>
       </c>
@@ -17220,7 +17236,7 @@
       </c>
       <c r="T210" s="26"/>
     </row>
-    <row r="211" spans="1:20" ht="42.75">
+    <row r="211" spans="1:20" ht="60">
       <c r="A211" s="26" t="s">
         <v>8</v>
       </c>
@@ -17272,7 +17288,7 @@
       </c>
       <c r="T211" s="26"/>
     </row>
-    <row r="212" spans="1:20" ht="42.75">
+    <row r="212" spans="1:20" ht="60">
       <c r="A212" s="26" t="s">
         <v>165</v>
       </c>
@@ -17326,7 +17342,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="57">
+    <row r="213" spans="1:20" ht="60">
       <c r="A213" s="26" t="s">
         <v>165</v>
       </c>
@@ -17378,7 +17394,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="28.5">
+    <row r="214" spans="1:20" ht="30">
       <c r="A214" s="26" t="s">
         <v>165</v>
       </c>
@@ -17414,7 +17430,7 @@
       <c r="S214" s="54"/>
       <c r="T214" s="26"/>
     </row>
-    <row r="215" spans="1:20" ht="28.5">
+    <row r="215" spans="1:20" ht="45">
       <c r="A215" s="26" t="s">
         <v>165</v>
       </c>
@@ -17466,7 +17482,7 @@
       </c>
       <c r="T215" s="26"/>
     </row>
-    <row r="216" spans="1:20" ht="71.25">
+    <row r="216" spans="1:20" ht="90">
       <c r="A216" s="26" t="s">
         <v>165</v>
       </c>
@@ -17518,7 +17534,7 @@
       </c>
       <c r="T216" s="26"/>
     </row>
-    <row r="217" spans="1:20" ht="71.25">
+    <row r="217" spans="1:20" ht="75">
       <c r="A217" s="26" t="s">
         <v>165</v>
       </c>
@@ -17572,7 +17588,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="71.25">
+    <row r="218" spans="1:20" ht="75">
       <c r="A218" s="26" t="s">
         <v>165</v>
       </c>
@@ -17624,7 +17640,7 @@
       </c>
       <c r="T218" s="26"/>
     </row>
-    <row r="219" spans="1:20" ht="42.75">
+    <row r="219" spans="1:20" ht="60">
       <c r="A219" s="26" t="s">
         <v>165</v>
       </c>
@@ -17670,7 +17686,7 @@
       <c r="S219" s="54"/>
       <c r="T219" s="26"/>
     </row>
-    <row r="220" spans="1:20" ht="42.75">
+    <row r="220" spans="1:20" ht="45">
       <c r="A220" s="26" t="s">
         <v>165</v>
       </c>
@@ -17722,7 +17738,7 @@
       </c>
       <c r="T220" s="26"/>
     </row>
-    <row r="221" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="221" spans="1:20" s="3" customFormat="1" ht="75">
       <c r="A221" s="12" t="s">
         <v>404</v>
       </c>
@@ -17774,7 +17790,7 @@
       </c>
       <c r="T221" s="12"/>
     </row>
-    <row r="222" spans="1:20" s="3" customFormat="1" ht="42.75">
+    <row r="222" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A222" s="12" t="s">
         <v>404</v>
       </c>
@@ -17826,7 +17842,7 @@
       </c>
       <c r="T222" s="12"/>
     </row>
-    <row r="223" spans="1:20" ht="57">
+    <row r="223" spans="1:20" ht="60">
       <c r="A223" s="26" t="s">
         <v>9</v>
       </c>
@@ -17878,7 +17894,7 @@
       </c>
       <c r="T223" s="26"/>
     </row>
-    <row r="224" spans="1:20" s="6" customFormat="1" ht="71.25">
+    <row r="224" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A224" s="26" t="s">
         <v>9</v>
       </c>
@@ -17936,7 +17952,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="225" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="225" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A225" s="28" t="str">
         <f>A$224</f>
         <v>Cross-Sector</v>
@@ -18000,7 +18016,7 @@
       <c r="S225" s="60"/>
       <c r="T225" s="28"/>
     </row>
-    <row r="226" spans="1:20" s="6" customFormat="1" ht="71.25">
+    <row r="226" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A226" s="28" t="str">
         <f t="shared" ref="A226:C230" si="64">A$224</f>
         <v>Cross-Sector</v>
@@ -18064,7 +18080,7 @@
       <c r="S226" s="60"/>
       <c r="T226" s="28"/>
     </row>
-    <row r="227" spans="1:20" s="6" customFormat="1" ht="71.25">
+    <row r="227" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A227" s="28" t="str">
         <f t="shared" si="64"/>
         <v>Cross-Sector</v>
@@ -18128,7 +18144,7 @@
       <c r="S227" s="60"/>
       <c r="T227" s="28"/>
     </row>
-    <row r="228" spans="1:20" s="6" customFormat="1" ht="57">
+    <row r="228" spans="1:20" s="6" customFormat="1" ht="75">
       <c r="A228" s="28" t="str">
         <f t="shared" si="64"/>
         <v>Cross-Sector</v>
@@ -18192,7 +18208,7 @@
       <c r="S228" s="60"/>
       <c r="T228" s="28"/>
     </row>
-    <row r="229" spans="1:20" s="6" customFormat="1" ht="42.75">
+    <row r="229" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A229" s="28" t="str">
         <f t="shared" si="64"/>
         <v>Cross-Sector</v>
@@ -18254,7 +18270,7 @@
       <c r="S229" s="60"/>
       <c r="T229" s="28"/>
     </row>
-    <row r="230" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="230" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A230" s="28" t="str">
         <f t="shared" si="64"/>
         <v>Cross-Sector</v>
@@ -18296,7 +18312,7 @@
       <c r="S230" s="60"/>
       <c r="T230" s="28"/>
     </row>
-    <row r="231" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="231" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A231" s="26" t="s">
         <v>9</v>
       </c>
@@ -18336,7 +18352,7 @@
       <c r="S231" s="59"/>
       <c r="T231" s="28"/>
     </row>
-    <row r="232" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="232" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A232" s="28" t="str">
         <f>A$231</f>
         <v>Cross-Sector</v>
@@ -18396,7 +18412,7 @@
       </c>
       <c r="T232" s="28"/>
     </row>
-    <row r="233" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="233" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A233" s="28" t="str">
         <f t="shared" ref="A233:A246" si="67">A$231</f>
         <v>Cross-Sector</v>
@@ -18460,7 +18476,7 @@
       </c>
       <c r="T233" s="28"/>
     </row>
-    <row r="234" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="234" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A234" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18524,7 +18540,7 @@
       </c>
       <c r="T234" s="28"/>
     </row>
-    <row r="235" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="235" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A235" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18568,7 +18584,7 @@
       <c r="S235" s="54"/>
       <c r="T235" s="28"/>
     </row>
-    <row r="236" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="236" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A236" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18612,7 +18628,7 @@
       <c r="S236" s="54"/>
       <c r="T236" s="28"/>
     </row>
-    <row r="237" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="237" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A237" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18676,7 +18692,7 @@
       </c>
       <c r="T237" s="28"/>
     </row>
-    <row r="238" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="238" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A238" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18720,7 +18736,7 @@
       <c r="S238" s="59"/>
       <c r="T238" s="28"/>
     </row>
-    <row r="239" spans="1:20" s="6" customFormat="1" ht="42.75">
+    <row r="239" spans="1:20" s="6" customFormat="1" ht="60">
       <c r="A239" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18784,7 +18800,7 @@
       </c>
       <c r="T239" s="28"/>
     </row>
-    <row r="240" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="240" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A240" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18848,7 +18864,7 @@
       </c>
       <c r="T240" s="28"/>
     </row>
-    <row r="241" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="241" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A241" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18892,7 +18908,7 @@
       <c r="S241" s="59"/>
       <c r="T241" s="28"/>
     </row>
-    <row r="242" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="242" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A242" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18936,7 +18952,7 @@
       <c r="S242" s="59"/>
       <c r="T242" s="28"/>
     </row>
-    <row r="243" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="243" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A243" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -18978,7 +18994,7 @@
       <c r="S243" s="54"/>
       <c r="T243" s="28"/>
     </row>
-    <row r="244" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="244" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A244" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -19022,7 +19038,7 @@
       <c r="S244" s="59"/>
       <c r="T244" s="28"/>
     </row>
-    <row r="245" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="245" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A245" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -19064,7 +19080,7 @@
       <c r="S245" s="59"/>
       <c r="T245" s="28"/>
     </row>
-    <row r="246" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="246" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A246" s="28" t="str">
         <f t="shared" si="67"/>
         <v>Cross-Sector</v>
@@ -19106,7 +19122,7 @@
       <c r="S246" s="59"/>
       <c r="T246" s="28"/>
     </row>
-    <row r="247" spans="1:20" s="3" customFormat="1" ht="57">
+    <row r="247" spans="1:20" s="3" customFormat="1" ht="60">
       <c r="A247" s="12" t="s">
         <v>9</v>
       </c>
@@ -19122,7 +19138,7 @@
       <c r="G247" s="12"/>
       <c r="H247" s="27"/>
       <c r="I247" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J247" s="49" t="s">
         <v>178</v>
@@ -19140,7 +19156,7 @@
       <c r="S247" s="54"/>
       <c r="T247" s="12"/>
     </row>
-    <row r="248" spans="1:20" s="6" customFormat="1" ht="99.75">
+    <row r="248" spans="1:20" s="6" customFormat="1" ht="105">
       <c r="A248" s="26" t="s">
         <v>9</v>
       </c>
@@ -19196,7 +19212,7 @@
       </c>
       <c r="T248" s="28"/>
     </row>
-    <row r="249" spans="1:20" s="6" customFormat="1" ht="99.75">
+    <row r="249" spans="1:20" s="6" customFormat="1" ht="105">
       <c r="A249" s="31" t="str">
         <f t="shared" ref="A249:C262" si="70">A$248</f>
         <v>Cross-Sector</v>
@@ -19326,7 +19342,7 @@
       </c>
       <c r="T250" s="28"/>
     </row>
-    <row r="251" spans="1:20" s="6" customFormat="1">
+    <row r="251" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A251" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19370,7 +19386,7 @@
       <c r="S251" s="59"/>
       <c r="T251" s="28"/>
     </row>
-    <row r="252" spans="1:20" s="6" customFormat="1">
+    <row r="252" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A252" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19414,7 +19430,7 @@
       <c r="S252" s="59"/>
       <c r="T252" s="28"/>
     </row>
-    <row r="253" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="253" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A253" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19458,7 +19474,7 @@
       <c r="S253" s="59"/>
       <c r="T253" s="28"/>
     </row>
-    <row r="254" spans="1:20" s="6" customFormat="1">
+    <row r="254" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A254" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19502,7 +19518,7 @@
       <c r="S254" s="59"/>
       <c r="T254" s="28"/>
     </row>
-    <row r="255" spans="1:20" s="6" customFormat="1">
+    <row r="255" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A255" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19546,7 +19562,7 @@
       <c r="S255" s="59"/>
       <c r="T255" s="28"/>
     </row>
-    <row r="256" spans="1:20" s="6" customFormat="1" ht="99.75">
+    <row r="256" spans="1:20" s="6" customFormat="1" ht="105">
       <c r="A256" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19611,7 +19627,7 @@
       </c>
       <c r="T256" s="28"/>
     </row>
-    <row r="257" spans="1:20" s="6" customFormat="1" ht="99.75">
+    <row r="257" spans="1:20" s="6" customFormat="1" ht="105">
       <c r="A257" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19676,7 +19692,7 @@
       </c>
       <c r="T257" s="28"/>
     </row>
-    <row r="258" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="258" spans="1:20" s="6" customFormat="1" ht="45">
       <c r="A258" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19720,7 +19736,7 @@
       <c r="S258" s="59"/>
       <c r="T258" s="28"/>
     </row>
-    <row r="259" spans="1:20" s="6" customFormat="1" ht="28.5">
+    <row r="259" spans="1:20" s="6" customFormat="1" ht="30">
       <c r="A259" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19764,7 +19780,7 @@
       <c r="S259" s="59"/>
       <c r="T259" s="28"/>
     </row>
-    <row r="260" spans="1:20">
+    <row r="260" spans="1:20" ht="30">
       <c r="A260" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19806,7 +19822,7 @@
       <c r="S260" s="59"/>
       <c r="T260" s="26"/>
     </row>
-    <row r="261" spans="1:20">
+    <row r="261" spans="1:20" ht="30">
       <c r="A261" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19850,7 +19866,7 @@
       <c r="S261" s="54"/>
       <c r="T261" s="26"/>
     </row>
-    <row r="262" spans="1:20">
+    <row r="262" spans="1:20" ht="30">
       <c r="A262" s="31" t="str">
         <f t="shared" si="70"/>
         <v>Cross-Sector</v>
@@ -19892,7 +19908,7 @@
       <c r="S262" s="54"/>
       <c r="T262" s="26"/>
     </row>
-    <row r="263" spans="1:20" ht="85.5">
+    <row r="263" spans="1:20" ht="105">
       <c r="A263" s="26" t="s">
         <v>28</v>
       </c>
@@ -19948,7 +19964,7 @@
       </c>
       <c r="T263" s="26"/>
     </row>
-    <row r="264" spans="1:20" ht="85.5">
+    <row r="264" spans="1:20" ht="105">
       <c r="A264" s="28" t="str">
         <f t="shared" ref="A264:A269" si="74">A$263</f>
         <v>R&amp;D</v>
@@ -20012,7 +20028,7 @@
       </c>
       <c r="T264" s="26"/>
     </row>
-    <row r="265" spans="1:20" ht="85.5">
+    <row r="265" spans="1:20" ht="105">
       <c r="A265" s="28" t="str">
         <f t="shared" si="74"/>
         <v>R&amp;D</v>
@@ -20076,7 +20092,7 @@
       </c>
       <c r="T265" s="26"/>
     </row>
-    <row r="266" spans="1:20" ht="85.5">
+    <row r="266" spans="1:20" ht="105">
       <c r="A266" s="28" t="str">
         <f t="shared" si="74"/>
         <v>R&amp;D</v>
@@ -20140,7 +20156,7 @@
       </c>
       <c r="T266" s="26"/>
     </row>
-    <row r="267" spans="1:20" ht="85.5">
+    <row r="267" spans="1:20" ht="105">
       <c r="A267" s="28" t="str">
         <f t="shared" si="74"/>
         <v>R&amp;D</v>
@@ -20204,7 +20220,7 @@
       </c>
       <c r="T267" s="26"/>
     </row>
-    <row r="268" spans="1:20" ht="99.75">
+    <row r="268" spans="1:20" ht="105">
       <c r="A268" s="28" t="str">
         <f t="shared" si="74"/>
         <v>R&amp;D</v>
@@ -20268,7 +20284,7 @@
       </c>
       <c r="T268" s="26"/>
     </row>
-    <row r="269" spans="1:20" ht="99.75">
+    <row r="269" spans="1:20" ht="105">
       <c r="A269" s="28" t="str">
         <f t="shared" si="74"/>
         <v>R&amp;D</v>
@@ -20325,7 +20341,7 @@
       </c>
       <c r="T269" s="26"/>
     </row>
-    <row r="270" spans="1:20" ht="85.5">
+    <row r="270" spans="1:20" ht="105">
       <c r="A270" s="26" t="s">
         <v>28</v>
       </c>
@@ -20383,7 +20399,7 @@
       </c>
       <c r="T270" s="26"/>
     </row>
-    <row r="271" spans="1:20" ht="85.5">
+    <row r="271" spans="1:20" ht="105">
       <c r="A271" s="28" t="str">
         <f>A$270</f>
         <v>R&amp;D</v>
@@ -20447,7 +20463,7 @@
       </c>
       <c r="T271" s="26"/>
     </row>
-    <row r="272" spans="1:20" ht="85.5">
+    <row r="272" spans="1:20" ht="105">
       <c r="A272" s="28" t="str">
         <f t="shared" ref="A272:C280" si="80">A$270</f>
         <v>R&amp;D</v>
@@ -20511,7 +20527,7 @@
       </c>
       <c r="T272" s="26"/>
     </row>
-    <row r="273" spans="1:20" ht="85.5">
+    <row r="273" spans="1:20" ht="105">
       <c r="A273" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20575,7 +20591,7 @@
       </c>
       <c r="T273" s="26"/>
     </row>
-    <row r="274" spans="1:20" ht="85.5">
+    <row r="274" spans="1:20" ht="105">
       <c r="A274" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20639,7 +20655,7 @@
       </c>
       <c r="T274" s="26"/>
     </row>
-    <row r="275" spans="1:20" ht="85.5">
+    <row r="275" spans="1:20" ht="105">
       <c r="A275" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20703,7 +20719,7 @@
       </c>
       <c r="T275" s="26"/>
     </row>
-    <row r="276" spans="1:20" ht="85.5">
+    <row r="276" spans="1:20" ht="105">
       <c r="A276" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20767,7 +20783,7 @@
       </c>
       <c r="T276" s="26"/>
     </row>
-    <row r="277" spans="1:20" ht="85.5">
+    <row r="277" spans="1:20" ht="105">
       <c r="A277" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20831,7 +20847,7 @@
       </c>
       <c r="T277" s="26"/>
     </row>
-    <row r="278" spans="1:20" ht="85.5">
+    <row r="278" spans="1:20" ht="105">
       <c r="A278" s="28" t="str">
         <f>A$270</f>
         <v>R&amp;D</v>
@@ -20895,7 +20911,7 @@
       </c>
       <c r="T278" s="26"/>
     </row>
-    <row r="279" spans="1:20" ht="85.5">
+    <row r="279" spans="1:20" ht="105">
       <c r="A279" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -20959,7 +20975,7 @@
       </c>
       <c r="T279" s="26"/>
     </row>
-    <row r="280" spans="1:20" ht="85.5">
+    <row r="280" spans="1:20" ht="105">
       <c r="A280" s="28" t="str">
         <f t="shared" si="80"/>
         <v>R&amp;D</v>
@@ -21023,7 +21039,7 @@
       </c>
       <c r="T280" s="26"/>
     </row>
-    <row r="281" spans="1:20" ht="85.5">
+    <row r="281" spans="1:20" ht="105">
       <c r="A281" s="26" t="s">
         <v>28</v>
       </c>
@@ -21081,7 +21097,7 @@
       </c>
       <c r="T281" s="26"/>
     </row>
-    <row r="282" spans="1:20" ht="99.75">
+    <row r="282" spans="1:20" ht="105">
       <c r="A282" s="28" t="str">
         <f>A$281</f>
         <v>R&amp;D</v>
@@ -21145,7 +21161,7 @@
       </c>
       <c r="T282" s="26"/>
     </row>
-    <row r="283" spans="1:20" ht="99.75">
+    <row r="283" spans="1:20" ht="105">
       <c r="A283" s="28" t="str">
         <f t="shared" ref="A283:A288" si="83">A$281</f>
         <v>R&amp;D</v>
@@ -21209,7 +21225,7 @@
       </c>
       <c r="T283" s="26"/>
     </row>
-    <row r="284" spans="1:20" ht="99.75">
+    <row r="284" spans="1:20" ht="105">
       <c r="A284" s="28" t="str">
         <f t="shared" si="83"/>
         <v>R&amp;D</v>
@@ -21273,7 +21289,7 @@
       </c>
       <c r="T284" s="26"/>
     </row>
-    <row r="285" spans="1:20" ht="85.5">
+    <row r="285" spans="1:20" ht="105">
       <c r="A285" s="28" t="str">
         <f t="shared" si="83"/>
         <v>R&amp;D</v>
@@ -21337,7 +21353,7 @@
       </c>
       <c r="T285" s="26"/>
     </row>
-    <row r="286" spans="1:20" ht="99.75">
+    <row r="286" spans="1:20" ht="105">
       <c r="A286" s="28" t="str">
         <f t="shared" si="83"/>
         <v>R&amp;D</v>
@@ -21401,7 +21417,7 @@
       </c>
       <c r="T286" s="26"/>
     </row>
-    <row r="287" spans="1:20" ht="99.75">
+    <row r="287" spans="1:20" ht="105">
       <c r="A287" s="28" t="str">
         <f t="shared" si="83"/>
         <v>R&amp;D</v>
@@ -21465,7 +21481,7 @@
       </c>
       <c r="T287" s="26"/>
     </row>
-    <row r="288" spans="1:20" ht="85.5">
+    <row r="288" spans="1:20" ht="105">
       <c r="A288" s="28" t="str">
         <f t="shared" si="83"/>
         <v>R&amp;D</v>
@@ -21529,7 +21545,7 @@
       </c>
       <c r="T288" s="26"/>
     </row>
-    <row r="289" spans="1:20" ht="85.5">
+    <row r="289" spans="1:20" ht="105">
       <c r="A289" s="12" t="s">
         <v>28</v>
       </c>
@@ -21587,7 +21603,7 @@
       </c>
       <c r="T289" s="26"/>
     </row>
-    <row r="290" spans="1:20" ht="85.5">
+    <row r="290" spans="1:20" ht="105">
       <c r="A290" s="28" t="str">
         <f>A$289</f>
         <v>R&amp;D</v>
@@ -21651,7 +21667,7 @@
       </c>
       <c r="T290" s="26"/>
     </row>
-    <row r="291" spans="1:20" ht="99.75">
+    <row r="291" spans="1:20" ht="120">
       <c r="A291" s="28" t="str">
         <f>A$289</f>
         <v>R&amp;D</v>
@@ -21715,7 +21731,7 @@
       </c>
       <c r="T291" s="26"/>
     </row>
-    <row r="292" spans="1:20" ht="99.75">
+    <row r="292" spans="1:20" ht="120">
       <c r="A292" s="28" t="str">
         <f>A$289</f>
         <v>R&amp;D</v>
@@ -21779,7 +21795,7 @@
       </c>
       <c r="T292" s="26"/>
     </row>
-    <row r="293" spans="1:20" ht="85.5">
+    <row r="293" spans="1:20" ht="105">
       <c r="A293" s="28" t="str">
         <f>A$289</f>
         <v>R&amp;D</v>
@@ -21843,7 +21859,7 @@
       </c>
       <c r="T293" s="26"/>
     </row>
-    <row r="294" spans="1:20" ht="85.5">
+    <row r="294" spans="1:20" ht="105">
       <c r="A294" s="28" t="str">
         <f>A$289</f>
         <v>R&amp;D</v>
@@ -21907,7 +21923,7 @@
       </c>
       <c r="T294" s="26"/>
     </row>
-    <row r="295" spans="1:20" ht="85.5">
+    <row r="295" spans="1:20" ht="105">
       <c r="A295" s="26" t="s">
         <v>28</v>
       </c>
@@ -21963,7 +21979,7 @@
       </c>
       <c r="T295" s="26"/>
     </row>
-    <row r="296" spans="1:20" ht="85.5">
+    <row r="296" spans="1:20" ht="105">
       <c r="A296" s="28" t="str">
         <f>A$295</f>
         <v>R&amp;D</v>
@@ -22027,7 +22043,7 @@
       </c>
       <c r="T296" s="26"/>
     </row>
-    <row r="297" spans="1:20" ht="42.75">
+    <row r="297" spans="1:20" ht="60">
       <c r="A297" s="28" t="str">
         <f>A$295</f>
         <v>R&amp;D</v>
@@ -22069,7 +22085,7 @@
       <c r="S297" s="54"/>
       <c r="T297" s="26"/>
     </row>
-    <row r="298" spans="1:20" ht="85.5">
+    <row r="298" spans="1:20" ht="105">
       <c r="A298" s="28" t="str">
         <f>A$295</f>
         <v>R&amp;D</v>
@@ -22133,7 +22149,7 @@
       </c>
       <c r="T298" s="26"/>
     </row>
-    <row r="299" spans="1:20" ht="85.5">
+    <row r="299" spans="1:20" ht="105">
       <c r="A299" s="28" t="str">
         <f>A$295</f>
         <v>R&amp;D</v>
@@ -22197,7 +22213,7 @@
       </c>
       <c r="T299" s="26"/>
     </row>
-    <row r="300" spans="1:20" ht="85.5">
+    <row r="300" spans="1:20" ht="105">
       <c r="A300" s="28" t="str">
         <f>A$295</f>
         <v>R&amp;D</v>
@@ -22261,7 +22277,7 @@
       </c>
       <c r="T300" s="26"/>
     </row>
-    <row r="301" spans="1:20" ht="99.75">
+    <row r="301" spans="1:20" ht="105">
       <c r="A301" s="26" t="s">
         <v>28</v>
       </c>
@@ -22317,7 +22333,7 @@
       </c>
       <c r="T301" s="26"/>
     </row>
-    <row r="302" spans="1:20" ht="85.5">
+    <row r="302" spans="1:20" ht="105">
       <c r="A302" s="26" t="s">
         <v>28</v>
       </c>
@@ -22375,7 +22391,7 @@
       </c>
       <c r="T302" s="26"/>
     </row>
-    <row r="303" spans="1:20" ht="85.5">
+    <row r="303" spans="1:20" ht="105">
       <c r="A303" s="28" t="str">
         <f>A$302</f>
         <v>R&amp;D</v>
@@ -22439,7 +22455,7 @@
       </c>
       <c r="T303" s="26"/>
     </row>
-    <row r="304" spans="1:20" ht="85.5">
+    <row r="304" spans="1:20" ht="105">
       <c r="A304" s="28" t="str">
         <f t="shared" ref="A304:C312" si="91">A$302</f>
         <v>R&amp;D</v>
@@ -22503,7 +22519,7 @@
       </c>
       <c r="T304" s="26"/>
     </row>
-    <row r="305" spans="1:20" ht="28.5">
+    <row r="305" spans="1:20" ht="45">
       <c r="A305" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22547,7 +22563,7 @@
       <c r="S305" s="54"/>
       <c r="T305" s="26"/>
     </row>
-    <row r="306" spans="1:20" ht="57">
+    <row r="306" spans="1:20" ht="60">
       <c r="A306" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22591,7 +22607,7 @@
       <c r="S306" s="54"/>
       <c r="T306" s="26"/>
     </row>
-    <row r="307" spans="1:20" ht="42.75">
+    <row r="307" spans="1:20" ht="45">
       <c r="A307" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22635,7 +22651,7 @@
       <c r="S307" s="54"/>
       <c r="T307" s="26"/>
     </row>
-    <row r="308" spans="1:20" ht="42.75">
+    <row r="308" spans="1:20" ht="60">
       <c r="A308" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22679,7 +22695,7 @@
       <c r="S308" s="54"/>
       <c r="T308" s="26"/>
     </row>
-    <row r="309" spans="1:20" ht="85.5">
+    <row r="309" spans="1:20" ht="105">
       <c r="A309" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22743,7 +22759,7 @@
       </c>
       <c r="T309" s="26"/>
     </row>
-    <row r="310" spans="1:20" ht="85.5">
+    <row r="310" spans="1:20" ht="105">
       <c r="A310" s="28" t="str">
         <f>A$302</f>
         <v>R&amp;D</v>
@@ -22807,7 +22823,7 @@
       </c>
       <c r="T310" s="26"/>
     </row>
-    <row r="311" spans="1:20" ht="85.5">
+    <row r="311" spans="1:20" ht="105">
       <c r="A311" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22871,7 +22887,7 @@
       </c>
       <c r="T311" s="26"/>
     </row>
-    <row r="312" spans="1:20" ht="57">
+    <row r="312" spans="1:20" ht="60">
       <c r="A312" s="28" t="str">
         <f t="shared" si="91"/>
         <v>R&amp;D</v>
@@ -22913,7 +22929,7 @@
       <c r="S312" s="54"/>
       <c r="T312" s="26"/>
     </row>
-    <row r="313" spans="1:20" ht="99.75">
+    <row r="313" spans="1:20" ht="105">
       <c r="A313" s="26" t="s">
         <v>28</v>
       </c>
@@ -22971,7 +22987,7 @@
       </c>
       <c r="T313" s="26"/>
     </row>
-    <row r="314" spans="1:20" ht="99.75">
+    <row r="314" spans="1:20" ht="120">
       <c r="A314" s="28" t="str">
         <f>A$313</f>
         <v>R&amp;D</v>
@@ -23035,7 +23051,7 @@
       </c>
       <c r="T314" s="26"/>
     </row>
-    <row r="315" spans="1:20" ht="99.75">
+    <row r="315" spans="1:20" ht="105">
       <c r="A315" s="28" t="str">
         <f t="shared" ref="A315:A320" si="95">A$313</f>
         <v>R&amp;D</v>
@@ -23099,7 +23115,7 @@
       </c>
       <c r="T315" s="26"/>
     </row>
-    <row r="316" spans="1:20" ht="99.75">
+    <row r="316" spans="1:20" ht="105">
       <c r="A316" s="28" t="str">
         <f t="shared" si="95"/>
         <v>R&amp;D</v>
@@ -23163,7 +23179,7 @@
       </c>
       <c r="T316" s="26"/>
     </row>
-    <row r="317" spans="1:20" ht="99.75">
+    <row r="317" spans="1:20" ht="105">
       <c r="A317" s="28" t="str">
         <f t="shared" si="95"/>
         <v>R&amp;D</v>
@@ -23227,7 +23243,7 @@
       </c>
       <c r="T317" s="26"/>
     </row>
-    <row r="318" spans="1:20" ht="99.75">
+    <row r="318" spans="1:20" ht="105">
       <c r="A318" s="28" t="str">
         <f t="shared" si="95"/>
         <v>R&amp;D</v>
@@ -23291,7 +23307,7 @@
       </c>
       <c r="T318" s="26"/>
     </row>
-    <row r="319" spans="1:20" ht="99.75">
+    <row r="319" spans="1:20" ht="105">
       <c r="A319" s="28" t="str">
         <f t="shared" si="95"/>
         <v>R&amp;D</v>
@@ -23355,7 +23371,7 @@
       </c>
       <c r="T319" s="26"/>
     </row>
-    <row r="320" spans="1:20" ht="99.75">
+    <row r="320" spans="1:20" ht="105">
       <c r="A320" s="28" t="str">
         <f t="shared" si="95"/>
         <v>R&amp;D</v>
@@ -23419,7 +23435,7 @@
       </c>
       <c r="T320" s="26"/>
     </row>
-    <row r="321" spans="1:20" ht="85.5">
+    <row r="321" spans="1:20" ht="105">
       <c r="A321" s="26" t="s">
         <v>28</v>
       </c>
@@ -23477,7 +23493,7 @@
       </c>
       <c r="T321" s="26"/>
     </row>
-    <row r="322" spans="1:20" ht="85.5">
+    <row r="322" spans="1:20" ht="105">
       <c r="A322" s="28" t="str">
         <f>A$321</f>
         <v>R&amp;D</v>
@@ -23541,7 +23557,7 @@
       </c>
       <c r="T322" s="26"/>
     </row>
-    <row r="323" spans="1:20" ht="99.75">
+    <row r="323" spans="1:20" ht="120">
       <c r="A323" s="28" t="str">
         <f>A$321</f>
         <v>R&amp;D</v>
@@ -23605,7 +23621,7 @@
       </c>
       <c r="T323" s="26"/>
     </row>
-    <row r="324" spans="1:20" ht="99.75">
+    <row r="324" spans="1:20" ht="120">
       <c r="A324" s="28" t="str">
         <f>A$321</f>
         <v>R&amp;D</v>
@@ -23669,7 +23685,7 @@
       </c>
       <c r="T324" s="26"/>
     </row>
-    <row r="325" spans="1:20" ht="85.5">
+    <row r="325" spans="1:20" ht="105">
       <c r="A325" s="28" t="str">
         <f>A$321</f>
         <v>R&amp;D</v>
@@ -23733,7 +23749,7 @@
       </c>
       <c r="T325" s="26"/>
     </row>
-    <row r="326" spans="1:20" ht="85.5">
+    <row r="326" spans="1:20" ht="105">
       <c r="A326" s="28" t="str">
         <f>A$321</f>
         <v>R&amp;D</v>
@@ -23801,8 +23817,8 @@
       <c r="I333" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T326"/>
-  <sortState ref="A119:I139">
+  <autoFilter ref="A1:T326" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A119:I139">
     <sortCondition ref="B119:B139"/>
   </sortState>
   <customSheetViews>
@@ -23811,7 +23827,7 @@
       <selection pane="bottomLeft" activeCell="P71" sqref="P71"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-      <autoFilter ref="A1:T326"/>
+      <autoFilter ref="A1:T326" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="I1 I36 I43 I57 I63 I279:I309 I311 I313:I332 I334:I1048576 I38:I39 I21:I33 I66:I277">
@@ -23920,14 +23936,14 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S9" r:id="rId2"/>
-    <hyperlink ref="T197" r:id="rId3"/>
-    <hyperlink ref="T207" r:id="rId4"/>
-    <hyperlink ref="S36" r:id="rId5"/>
-    <hyperlink ref="S125" r:id="rId6"/>
-    <hyperlink ref="S182" r:id="rId7"/>
-    <hyperlink ref="S95" r:id="rId8" display="https://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/irp/2018/2019 IRP Proposed Reference System Plan_20191106.pdf"/>
-    <hyperlink ref="S12" r:id="rId9"/>
+    <hyperlink ref="S9" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="T197" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="T207" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="S36" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S125" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="S182" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="S95" r:id="rId8" display="https://www.cpuc.ca.gov/uploadedFiles/CPUCWebsite/Content/UtilitiesIndustries/Energy/EnergyPrograms/ElectPowerProcurementGeneration/irp/2018/2019 IRP Proposed Reference System Plan_20191106.pdf" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="S12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
@@ -23936,7 +23952,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23944,20 +23960,20 @@
       <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.265625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" style="52" customWidth="1"/>
-    <col min="3" max="3" width="18.73046875" style="52" customWidth="1"/>
-    <col min="4" max="4" width="16.3984375" style="52" customWidth="1"/>
-    <col min="5" max="5" width="30.1328125" style="52" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="52" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="52" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" style="52" customWidth="1"/>
     <col min="6" max="6" width="95" style="52" customWidth="1"/>
-    <col min="7" max="7" width="37.3984375" style="52" customWidth="1"/>
-    <col min="8" max="8" width="34.265625" style="52" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="52"/>
+    <col min="7" max="7" width="37.42578125" style="52" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" style="52" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="68" customFormat="1" ht="28.5">
+    <row r="1" spans="1:8" s="68" customFormat="1" ht="30">
       <c r="A1" s="65" t="s">
         <v>635</v>
       </c>
@@ -24024,7 +24040,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57">
+    <row r="4" spans="1:8" ht="60">
       <c r="A4" s="74" t="s">
         <v>662</v>
       </c>
@@ -24050,7 +24066,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="74" t="s">
         <v>662</v>
       </c>
@@ -24076,7 +24092,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5">
+    <row r="6" spans="1:8" ht="30">
       <c r="A6" s="74" t="s">
         <v>662</v>
       </c>
@@ -24354,7 +24370,7 @@
       </c>
       <c r="H18" s="72"/>
     </row>
-    <row r="19" spans="1:8" ht="57">
+    <row r="19" spans="1:8" ht="60">
       <c r="A19" s="73" t="s">
         <v>669</v>
       </c>
@@ -24380,7 +24396,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="71.25">
+    <row r="20" spans="1:8" ht="90">
       <c r="A20" s="73" t="s">
         <v>669</v>
       </c>
@@ -24406,7 +24422,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.5">
+    <row r="21" spans="1:8" ht="30">
       <c r="A21" s="73" t="s">
         <v>669</v>
       </c>
@@ -24451,7 +24467,7 @@
       </c>
       <c r="H22" s="72"/>
     </row>
-    <row r="23" spans="1:8" ht="42.75">
+    <row r="23" spans="1:8" ht="45">
       <c r="A23" s="73" t="s">
         <v>420</v>
       </c>
@@ -24472,7 +24488,7 @@
       </c>
       <c r="H23" s="72"/>
     </row>
-    <row r="24" spans="1:8" ht="42.75">
+    <row r="24" spans="1:8" ht="45">
       <c r="A24" s="73" t="s">
         <v>420</v>
       </c>
@@ -24493,7 +24509,7 @@
       </c>
       <c r="H24" s="72"/>
     </row>
-    <row r="25" spans="1:8" ht="42.75">
+    <row r="25" spans="1:8" ht="45">
       <c r="A25" s="73" t="s">
         <v>673</v>
       </c>
@@ -24519,7 +24535,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="42.75">
+    <row r="26" spans="1:8" ht="45">
       <c r="A26" s="73" t="s">
         <v>673</v>
       </c>
@@ -24545,7 +24561,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28.5">
+    <row r="27" spans="1:8" ht="45">
       <c r="A27" s="73" t="s">
         <v>673</v>
       </c>
@@ -24571,7 +24587,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="28.5">
+    <row r="28" spans="1:8" ht="45">
       <c r="A28" s="73" t="s">
         <v>673</v>
       </c>
@@ -24597,7 +24613,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="71.25">
+    <row r="29" spans="1:8" ht="90">
       <c r="A29" s="73" t="s">
         <v>673</v>
       </c>
@@ -24623,7 +24639,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="28.5">
+    <row r="30" spans="1:8" ht="30">
       <c r="A30" s="73" t="s">
         <v>677</v>
       </c>
@@ -24644,7 +24660,7 @@
       </c>
       <c r="H30" s="72"/>
     </row>
-    <row r="31" spans="1:8" ht="28.5">
+    <row r="31" spans="1:8" ht="30">
       <c r="A31" s="73" t="s">
         <v>677</v>
       </c>
@@ -24665,7 +24681,7 @@
       </c>
       <c r="H31" s="72"/>
     </row>
-    <row r="32" spans="1:8" ht="99.75">
+    <row r="32" spans="1:8" ht="105">
       <c r="A32" s="73" t="s">
         <v>680</v>
       </c>
@@ -24691,7 +24707,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="114">
+    <row r="33" spans="1:8" ht="135">
       <c r="A33" s="73" t="s">
         <v>680</v>
       </c>
@@ -24717,7 +24733,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="85.5">
+    <row r="34" spans="1:8" ht="120">
       <c r="A34" s="73" t="s">
         <v>680</v>
       </c>
@@ -24743,7 +24759,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="114">
+    <row r="35" spans="1:8" ht="135">
       <c r="A35" s="73" t="s">
         <v>680</v>
       </c>
@@ -24769,7 +24785,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="71.25">
+    <row r="36" spans="1:8" ht="90">
       <c r="A36" s="73" t="s">
         <v>685</v>
       </c>
@@ -24795,7 +24811,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="28.5">
+    <row r="37" spans="1:8" ht="30">
       <c r="A37" s="73" t="s">
         <v>685</v>
       </c>
@@ -24821,7 +24837,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="42.75">
+    <row r="38" spans="1:8" ht="45">
       <c r="A38" s="73" t="s">
         <v>688</v>
       </c>
@@ -24847,7 +24863,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="42.75">
+    <row r="39" spans="1:8" ht="45">
       <c r="A39" s="73" t="s">
         <v>688</v>
       </c>
@@ -24873,7 +24889,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="42.75">
+    <row r="40" spans="1:8" ht="45">
       <c r="A40" s="73" t="s">
         <v>691</v>
       </c>
@@ -24899,7 +24915,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="42.75">
+    <row r="41" spans="1:8" ht="60">
       <c r="A41" s="73" t="s">
         <v>691</v>
       </c>
@@ -24925,7 +24941,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="42.75">
+    <row r="42" spans="1:8" ht="45">
       <c r="A42" s="73" t="s">
         <v>691</v>
       </c>
@@ -24951,7 +24967,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="28.5">
+    <row r="43" spans="1:8" ht="30">
       <c r="A43" s="73" t="s">
         <v>691</v>
       </c>
@@ -24977,7 +24993,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="28.5">
+    <row r="44" spans="1:8" ht="30">
       <c r="A44" s="73" t="s">
         <v>691</v>
       </c>
@@ -25003,7 +25019,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="42.75">
+    <row r="45" spans="1:8" ht="45">
       <c r="A45" s="75" t="s">
         <v>694</v>
       </c>
@@ -25029,7 +25045,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="42.75">
+    <row r="46" spans="1:8" ht="45">
       <c r="A46" s="75" t="s">
         <v>694</v>
       </c>
@@ -25055,7 +25071,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="42.75">
+    <row r="47" spans="1:8" ht="45">
       <c r="A47" s="75" t="s">
         <v>694</v>
       </c>
@@ -25081,7 +25097,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="28.5">
+    <row r="48" spans="1:8" ht="30">
       <c r="A48" s="75" t="s">
         <v>694</v>
       </c>
@@ -25107,7 +25123,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="28.5">
+    <row r="49" spans="1:8" ht="30">
       <c r="A49" s="75" t="s">
         <v>694</v>
       </c>
@@ -25133,7 +25149,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="114">
+    <row r="50" spans="1:8" ht="150">
       <c r="A50" s="73" t="s">
         <v>711</v>
       </c>
@@ -25159,7 +25175,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="57">
+    <row r="51" spans="1:8" ht="75">
       <c r="A51" s="73" t="s">
         <v>711</v>
       </c>
@@ -25185,7 +25201,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="114">
+    <row r="52" spans="1:8" ht="135">
       <c r="A52" s="73" t="s">
         <v>711</v>
       </c>
@@ -25211,7 +25227,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="71.25">
+    <row r="53" spans="1:8" ht="75">
       <c r="A53" s="75" t="s">
         <v>697</v>
       </c>
@@ -25237,7 +25253,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42.75">
+    <row r="54" spans="1:8" ht="45">
       <c r="A54" s="75" t="s">
         <v>697</v>
       </c>
@@ -25263,7 +25279,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="57">
+    <row r="55" spans="1:8" ht="75">
       <c r="A55" s="75" t="s">
         <v>1133</v>
       </c>
@@ -25289,7 +25305,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="42.75">
+    <row r="56" spans="1:8" ht="45">
       <c r="A56" s="75" t="s">
         <v>1133</v>
       </c>
@@ -25315,7 +25331,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="57">
+    <row r="57" spans="1:8" ht="60">
       <c r="A57" s="75" t="s">
         <v>1133</v>
       </c>
@@ -25341,7 +25357,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="28.5">
+    <row r="58" spans="1:8" ht="45">
       <c r="A58" s="75" t="s">
         <v>1133</v>
       </c>
@@ -25367,7 +25383,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="42.75">
+    <row r="59" spans="1:8" ht="60">
       <c r="A59" s="75" t="s">
         <v>700</v>
       </c>
@@ -25393,7 +25409,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="28.5">
+    <row r="60" spans="1:8" ht="30">
       <c r="A60" s="75" t="s">
         <v>700</v>
       </c>
@@ -25419,7 +25435,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="42.75">
+    <row r="61" spans="1:8" ht="45">
       <c r="A61" s="75" t="s">
         <v>700</v>
       </c>
@@ -25550,7 +25566,7 @@
       </c>
       <c r="H66" s="72"/>
     </row>
-    <row r="67" spans="1:8" ht="42.75">
+    <row r="67" spans="1:8" ht="60">
       <c r="A67" s="75" t="s">
         <v>705</v>
       </c>
@@ -25576,7 +25592,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="28.5">
+    <row r="68" spans="1:8" ht="30">
       <c r="A68" s="75" t="s">
         <v>705</v>
       </c>
@@ -25602,7 +25618,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="71.25">
+    <row r="69" spans="1:8" ht="75">
       <c r="A69" s="75" t="s">
         <v>705</v>
       </c>
@@ -25654,7 +25670,7 @@
         <v>969696</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="57">
+    <row r="71" spans="1:8" ht="75">
       <c r="A71" s="75" t="s">
         <v>705</v>
       </c>
@@ -25680,7 +25696,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" ht="30">
       <c r="A72" s="75" t="s">
         <v>706</v>
       </c>
@@ -25701,7 +25717,7 @@
       </c>
       <c r="H72" s="72"/>
     </row>
-    <row r="73" spans="1:8" ht="28.5">
+    <row r="73" spans="1:8" ht="30">
       <c r="A73" s="75" t="s">
         <v>706</v>
       </c>
@@ -25785,16 +25801,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.265625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="34.1328125" style="11" customWidth="1"/>
-    <col min="3" max="16384" width="8.86328125" style="11"/>
+    <col min="1" max="1" width="43.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -25843,24 +25859,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I905"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.265625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.86328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.73046875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="73.3984375" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.86328125" style="11"/>
+    <col min="1" max="1" width="49.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="42.75">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="45">
       <c r="A1" s="1" t="s">
         <v>384</v>
       </c>
@@ -25877,7 +25893,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="5" t="s">
         <v>755</v>
       </c>
@@ -25896,7 +25912,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="5" t="s">
         <v>761</v>
       </c>
@@ -26135,7 +26151,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" ht="28.5">
+    <row r="37" spans="1:4" ht="30">
       <c r="A37" s="21" t="s">
         <v>1047</v>
       </c>
@@ -26217,12 +26233,12 @@
       </c>
       <c r="D42" s="7"/>
     </row>
-    <row r="43" spans="1:4" ht="14.65" thickBot="1">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
       <c r="A43" s="11"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" ht="14.65" thickBot="1">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
       <c r="A44" s="85" t="s">
         <v>1052</v>
       </c>
@@ -50969,7 +50985,7 @@
     </customSheetView>
   </customSheetViews>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$C$44:$C$45</formula1>
     </dataValidation>
   </dataValidations>
@@ -50979,33 +50995,33 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="79.73046875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="79.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="11" customWidth="1"/>
     <col min="4" max="4" width="22" style="11" customWidth="1"/>
-    <col min="5" max="5" width="19.3984375" style="11" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="26.1328125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="26.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.3984375" style="11" customWidth="1"/>
-    <col min="11" max="16" width="9.1328125" style="11"/>
-    <col min="17" max="17" width="25.86328125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="12.3984375" style="11" customWidth="1"/>
-    <col min="19" max="19" width="19.86328125" style="11" customWidth="1"/>
-    <col min="20" max="21" width="12.3984375" style="11" customWidth="1"/>
-    <col min="22" max="23" width="16.265625" style="11" customWidth="1"/>
-    <col min="24" max="24" width="10.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.1328125" style="11"/>
+    <col min="5" max="5" width="19.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="11" customWidth="1"/>
+    <col min="11" max="16" width="9.140625" style="11"/>
+    <col min="17" max="17" width="25.85546875" style="11" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="11" customWidth="1"/>
+    <col min="19" max="19" width="19.85546875" style="11" customWidth="1"/>
+    <col min="20" max="21" width="12.42578125" style="11" customWidth="1"/>
+    <col min="22" max="23" width="16.28515625" style="11" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -51070,12 +51086,12 @@
       <c r="D40" s="110"/>
       <c r="E40" s="110"/>
     </row>
-    <row r="57" spans="1:2" ht="14.65" thickBot="1">
+    <row r="57" spans="1:2" ht="15.75" thickBot="1">
       <c r="A57" s="11" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="14.65" thickBot="1">
+    <row r="58" spans="1:2" ht="15.75" thickBot="1">
       <c r="A58" s="13">
         <v>194000</v>
       </c>
@@ -51100,7 +51116,7 @@
         <v>972.7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="14.65" thickBot="1">
+    <row r="84" spans="1:2" ht="15.75" thickBot="1">
       <c r="A84" s="15" t="s">
         <v>427</v>
       </c>
@@ -51109,7 +51125,7 @@
         <v>4124.8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="14.65" thickBot="1">
+    <row r="85" spans="1:2" ht="15.75" thickBot="1">
       <c r="A85" s="15" t="s">
         <v>428</v>
       </c>

</xml_diff>

<commit_message>
Correct erroneously enabled policy in WebAppData (reduction in downtime for lignite plants, which don't exist in California)
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-california\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6534703-21C9-4FE0-AC47-1F3AFB26CFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356FB92B-CF75-4353-A4D2-D86C4CE50ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2490" yWindow="1020" windowWidth="24765" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -15231,7 +15231,7 @@
       <c r="G175" s="12"/>
       <c r="H175" s="29"/>
       <c r="I175" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J175" s="64" t="str">
         <f t="shared" si="46"/>

</xml_diff>

<commit_message>
take out output coal
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\California\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBA82D63-A2D6-4C92-AA7D-F3B0490972B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6CBE81-CBDD-47F5-9B4D-FF50328A3A5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="2175" windowWidth="25080" windowHeight="15135" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="1515" windowWidth="22860" windowHeight="15135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -5068,12 +5068,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -5084,6 +5078,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="2x indented GHG Textfiels" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -5967,9 +5967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W333"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24021,9 +24021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S75"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -24046,7 +24046,7 @@
       <c r="B1" s="66" t="s">
         <v>635</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="C1" s="109" t="s">
         <v>1390</v>
       </c>
       <c r="D1" s="66" t="s">
@@ -24098,66 +24098,66 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="116" customFormat="1">
-      <c r="A2" s="113" t="s">
+    <row r="2" spans="1:19" s="114" customFormat="1">
+      <c r="A2" s="111" t="s">
         <v>661</v>
       </c>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="112" t="s">
         <v>663</v>
       </c>
       <c r="C2" s="76">
         <v>1</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="115" t="s">
+      <c r="E2" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="115" t="s">
+      <c r="F2" s="113" t="s">
         <v>415</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="112" t="s">
         <v>633</v>
       </c>
-      <c r="I2" s="114"/>
-      <c r="J2" s="116" t="str">
+      <c r="I2" s="112"/>
+      <c r="J2" s="114" t="str">
         <f>'Target Calculations'!A2</f>
         <v>2020 Target from AB 32</v>
       </c>
-      <c r="K2" s="116">
+      <c r="K2" s="114">
         <f>'Target Calculations'!B2</f>
         <v>2020</v>
       </c>
-      <c r="L2" s="116">
+      <c r="L2" s="114">
         <f>'Target Calculations'!C2</f>
         <v>430.72400412319996</v>
       </c>
-      <c r="M2" s="116">
+      <c r="M2" s="114">
         <f>'Target Calculations'!D2</f>
         <v>430.72400412319996</v>
       </c>
-      <c r="N2" s="116" t="str">
+      <c r="N2" s="114" t="str">
         <f>'Target Calculations'!E2</f>
         <v>In the California Global Warming Solutions Act of 2006 (AB 32), California committed to reduce greenhouse gas emissions to 1990 levels by 2020.</v>
       </c>
-      <c r="O2" s="116" t="str">
+      <c r="O2" s="114" t="str">
         <f>'Target Calculations'!A3</f>
         <v>2030 Target from SB 32</v>
       </c>
-      <c r="P2" s="116">
+      <c r="P2" s="114">
         <f>'Target Calculations'!B3</f>
         <v>2030</v>
       </c>
-      <c r="Q2" s="116">
+      <c r="Q2" s="114">
         <f>'Target Calculations'!C3</f>
         <v>258.43440247391999</v>
       </c>
-      <c r="R2" s="116">
+      <c r="R2" s="114">
         <f>'Target Calculations'!D3</f>
         <v>258.43440247391999</v>
       </c>
-      <c r="S2" s="116" t="str">
+      <c r="S2" s="114" t="str">
         <f>'Target Calculations'!E3</f>
         <v>In SB 32 (enacted in 2016), California committed to reduce greenhouse gas emissions 40 percent below 1990 levels by 2030.</v>
       </c>
@@ -24169,7 +24169,7 @@
       <c r="B3" s="72" t="s">
         <v>662</v>
       </c>
-      <c r="C3" s="112">
+      <c r="C3" s="110">
         <v>1</v>
       </c>
       <c r="D3" s="72" t="s">
@@ -24192,7 +24192,7 @@
       <c r="B4" s="73" t="s">
         <v>664</v>
       </c>
-      <c r="C4" s="112">
+      <c r="C4" s="110">
         <v>1</v>
       </c>
       <c r="D4" s="72" t="s">
@@ -24221,7 +24221,7 @@
       <c r="B5" s="73" t="s">
         <v>665</v>
       </c>
-      <c r="C5" s="112">
+      <c r="C5" s="110">
         <v>1</v>
       </c>
       <c r="D5" s="72" t="s">
@@ -24250,7 +24250,7 @@
       <c r="B6" s="73" t="s">
         <v>666</v>
       </c>
-      <c r="C6" s="112">
+      <c r="C6" s="110">
         <v>1</v>
       </c>
       <c r="D6" s="72" t="s">
@@ -24279,7 +24279,7 @@
       <c r="B7" s="73" t="s">
         <v>525</v>
       </c>
-      <c r="C7" s="112">
+      <c r="C7" s="110">
         <v>1</v>
       </c>
       <c r="D7" s="72" t="s">
@@ -24303,7 +24303,7 @@
       <c r="B8" s="74" t="s">
         <v>532</v>
       </c>
-      <c r="C8" s="112">
+      <c r="C8" s="110">
         <v>1</v>
       </c>
       <c r="D8" s="72" t="s">
@@ -24327,7 +24327,7 @@
       <c r="B9" s="74" t="s">
         <v>533</v>
       </c>
-      <c r="C9" s="112">
+      <c r="C9" s="110">
         <v>1</v>
       </c>
       <c r="D9" s="72" t="s">
@@ -24351,7 +24351,7 @@
       <c r="B10" s="74" t="s">
         <v>642</v>
       </c>
-      <c r="C10" s="112">
+      <c r="C10" s="110">
         <v>1</v>
       </c>
       <c r="D10" s="72" t="s">
@@ -24375,7 +24375,7 @@
       <c r="B11" s="74" t="s">
         <v>641</v>
       </c>
-      <c r="C11" s="112">
+      <c r="C11" s="110">
         <v>1</v>
       </c>
       <c r="D11" s="72" t="s">
@@ -24399,7 +24399,7 @@
       <c r="B12" s="74" t="s">
         <v>528</v>
       </c>
-      <c r="C12" s="112">
+      <c r="C12" s="110">
         <v>1</v>
       </c>
       <c r="D12" s="72" t="s">
@@ -24423,7 +24423,7 @@
       <c r="B13" s="74" t="s">
         <v>530</v>
       </c>
-      <c r="C13" s="112">
+      <c r="C13" s="110">
         <v>1</v>
       </c>
       <c r="D13" s="72" t="s">
@@ -24447,7 +24447,7 @@
       <c r="B14" s="74" t="s">
         <v>531</v>
       </c>
-      <c r="C14" s="112">
+      <c r="C14" s="110">
         <v>1</v>
       </c>
       <c r="D14" s="72" t="s">
@@ -24471,7 +24471,7 @@
       <c r="B15" s="74" t="s">
         <v>527</v>
       </c>
-      <c r="C15" s="112">
+      <c r="C15" s="110">
         <v>1</v>
       </c>
       <c r="D15" s="72" t="s">
@@ -24495,7 +24495,7 @@
       <c r="B16" s="74" t="s">
         <v>526</v>
       </c>
-      <c r="C16" s="112">
+      <c r="C16" s="110">
         <v>1</v>
       </c>
       <c r="D16" s="72" t="s">
@@ -24519,7 +24519,7 @@
       <c r="B17" s="74" t="s">
         <v>529</v>
       </c>
-      <c r="C17" s="112">
+      <c r="C17" s="110">
         <v>1</v>
       </c>
       <c r="D17" s="72" t="s">
@@ -24543,7 +24543,7 @@
       <c r="B18" s="74" t="s">
         <v>504</v>
       </c>
-      <c r="C18" s="112">
+      <c r="C18" s="110">
         <v>1</v>
       </c>
       <c r="D18" s="72" t="s">
@@ -24567,7 +24567,7 @@
       <c r="B19" s="73" t="s">
         <v>664</v>
       </c>
-      <c r="C19" s="112">
+      <c r="C19" s="110">
         <v>1</v>
       </c>
       <c r="D19" s="72" t="s">
@@ -24596,7 +24596,7 @@
       <c r="B20" s="73" t="s">
         <v>669</v>
       </c>
-      <c r="C20" s="112">
+      <c r="C20" s="110">
         <v>1</v>
       </c>
       <c r="D20" s="72" t="s">
@@ -24625,7 +24625,7 @@
       <c r="B21" s="73" t="s">
         <v>670</v>
       </c>
-      <c r="C21" s="112">
+      <c r="C21" s="110">
         <v>1</v>
       </c>
       <c r="D21" s="72" t="s">
@@ -24652,7 +24652,7 @@
         <v>419</v>
       </c>
       <c r="B22" s="73"/>
-      <c r="C22" s="112">
+      <c r="C22" s="110">
         <v>1</v>
       </c>
       <c r="D22" s="72" t="s">
@@ -24676,7 +24676,7 @@
       <c r="B23" s="73" t="s">
         <v>671</v>
       </c>
-      <c r="C23" s="112">
+      <c r="C23" s="110">
         <v>1</v>
       </c>
       <c r="D23" s="72" t="s">
@@ -24700,7 +24700,7 @@
       <c r="B24" s="102" t="s">
         <v>1158</v>
       </c>
-      <c r="C24" s="112">
+      <c r="C24" s="110">
         <v>1</v>
       </c>
       <c r="D24" s="72" t="s">
@@ -24724,7 +24724,7 @@
       <c r="B25" s="73" t="s">
         <v>673</v>
       </c>
-      <c r="C25" s="112">
+      <c r="C25" s="110">
         <v>1</v>
       </c>
       <c r="D25" s="72" t="s">
@@ -24753,7 +24753,7 @@
       <c r="B26" s="73" t="s">
         <v>674</v>
       </c>
-      <c r="C26" s="112">
+      <c r="C26" s="110">
         <v>1</v>
       </c>
       <c r="D26" s="72" t="s">
@@ -24782,7 +24782,7 @@
       <c r="B27" s="73" t="s">
         <v>1156</v>
       </c>
-      <c r="C27" s="112">
+      <c r="C27" s="110">
         <v>1</v>
       </c>
       <c r="D27" s="72" t="s">
@@ -24811,7 +24811,7 @@
       <c r="B28" s="73" t="s">
         <v>1157</v>
       </c>
-      <c r="C28" s="112">
+      <c r="C28" s="110">
         <v>1</v>
       </c>
       <c r="D28" s="72" t="s">
@@ -24840,7 +24840,7 @@
       <c r="B29" s="73" t="s">
         <v>675</v>
       </c>
-      <c r="C29" s="112">
+      <c r="C29" s="110">
         <v>1</v>
       </c>
       <c r="D29" s="72" t="s">
@@ -24869,7 +24869,7 @@
       <c r="B30" s="73" t="s">
         <v>677</v>
       </c>
-      <c r="C30" s="112">
+      <c r="C30" s="110">
         <v>1</v>
       </c>
       <c r="D30" s="72" t="s">
@@ -24893,7 +24893,7 @@
       <c r="B31" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="C31" s="112">
+      <c r="C31" s="110">
         <v>1</v>
       </c>
       <c r="D31" s="72" t="s">
@@ -24917,7 +24917,7 @@
       <c r="B32" s="73" t="s">
         <v>680</v>
       </c>
-      <c r="C32" s="112">
+      <c r="C32" s="110">
         <v>1</v>
       </c>
       <c r="D32" s="72" t="s">
@@ -24946,7 +24946,7 @@
       <c r="B33" s="73" t="s">
         <v>681</v>
       </c>
-      <c r="C33" s="112">
+      <c r="C33" s="110">
         <v>1</v>
       </c>
       <c r="D33" s="72" t="s">
@@ -24975,7 +24975,7 @@
       <c r="B34" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="C34" s="112">
+      <c r="C34" s="110">
         <v>1</v>
       </c>
       <c r="D34" s="72" t="s">
@@ -25004,7 +25004,7 @@
       <c r="B35" s="73" t="s">
         <v>683</v>
       </c>
-      <c r="C35" s="112">
+      <c r="C35" s="110">
         <v>1</v>
       </c>
       <c r="D35" s="72" t="s">
@@ -25033,7 +25033,7 @@
       <c r="B36" s="73" t="s">
         <v>685</v>
       </c>
-      <c r="C36" s="112">
+      <c r="C36" s="110">
         <v>1</v>
       </c>
       <c r="D36" s="72" t="s">
@@ -25062,7 +25062,7 @@
       <c r="B37" s="73" t="s">
         <v>686</v>
       </c>
-      <c r="C37" s="112">
+      <c r="C37" s="110">
         <v>1</v>
       </c>
       <c r="D37" s="72" t="s">
@@ -25091,7 +25091,7 @@
       <c r="B38" s="73" t="s">
         <v>688</v>
       </c>
-      <c r="C38" s="112">
+      <c r="C38" s="110">
         <v>1</v>
       </c>
       <c r="D38" s="72" t="s">
@@ -25120,7 +25120,7 @@
       <c r="B39" s="73" t="s">
         <v>689</v>
       </c>
-      <c r="C39" s="112">
+      <c r="C39" s="110">
         <v>1</v>
       </c>
       <c r="D39" s="72" t="s">
@@ -25149,7 +25149,7 @@
       <c r="B40" s="73" t="s">
         <v>691</v>
       </c>
-      <c r="C40" s="112">
+      <c r="C40" s="110">
         <v>1</v>
       </c>
       <c r="D40" s="72" t="s">
@@ -25178,7 +25178,7 @@
       <c r="B41" s="73" t="s">
         <v>692</v>
       </c>
-      <c r="C41" s="112">
+      <c r="C41" s="110">
         <v>1</v>
       </c>
       <c r="D41" s="72" t="s">
@@ -25207,7 +25207,7 @@
       <c r="B42" s="73" t="s">
         <v>1061</v>
       </c>
-      <c r="C42" s="112">
+      <c r="C42" s="110">
         <v>1</v>
       </c>
       <c r="D42" s="72" t="s">
@@ -25236,7 +25236,7 @@
       <c r="B43" s="73" t="s">
         <v>1062</v>
       </c>
-      <c r="C43" s="112">
+      <c r="C43" s="110">
         <v>1</v>
       </c>
       <c r="D43" s="72" t="s">
@@ -25265,7 +25265,7 @@
       <c r="B44" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="C44" s="112">
+      <c r="C44" s="110">
         <v>1</v>
       </c>
       <c r="D44" s="72" t="s">
@@ -25294,7 +25294,7 @@
       <c r="B45" s="73" t="s">
         <v>691</v>
       </c>
-      <c r="C45" s="112">
+      <c r="C45" s="110">
         <v>1</v>
       </c>
       <c r="D45" s="72" t="s">
@@ -25323,7 +25323,7 @@
       <c r="B46" s="73" t="s">
         <v>692</v>
       </c>
-      <c r="C46" s="112">
+      <c r="C46" s="110">
         <v>1</v>
       </c>
       <c r="D46" s="72" t="s">
@@ -25352,7 +25352,7 @@
       <c r="B47" s="73" t="s">
         <v>1061</v>
       </c>
-      <c r="C47" s="112">
+      <c r="C47" s="110">
         <v>1</v>
       </c>
       <c r="D47" s="72" t="s">
@@ -25381,7 +25381,7 @@
       <c r="B48" s="73" t="s">
         <v>1062</v>
       </c>
-      <c r="C48" s="112">
+      <c r="C48" s="110">
         <v>1</v>
       </c>
       <c r="D48" s="72" t="s">
@@ -25410,7 +25410,7 @@
       <c r="B49" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="C49" s="112">
+      <c r="C49" s="110">
         <v>1</v>
       </c>
       <c r="D49" s="72" t="s">
@@ -25439,7 +25439,7 @@
       <c r="B50" s="73" t="s">
         <v>694</v>
       </c>
-      <c r="C50" s="112">
+      <c r="C50" s="110">
         <v>1</v>
       </c>
       <c r="D50" s="72" t="s">
@@ -25468,7 +25468,7 @@
       <c r="B51" s="73" t="s">
         <v>695</v>
       </c>
-      <c r="C51" s="112">
+      <c r="C51" s="110">
         <v>1</v>
       </c>
       <c r="D51" s="72" t="s">
@@ -25497,7 +25497,7 @@
       <c r="B52" s="73" t="s">
         <v>1130</v>
       </c>
-      <c r="C52" s="112">
+      <c r="C52" s="110">
         <v>1</v>
       </c>
       <c r="D52" s="72" t="s">
@@ -25526,7 +25526,7 @@
       <c r="B53" s="73" t="s">
         <v>697</v>
       </c>
-      <c r="C53" s="112">
+      <c r="C53" s="110">
         <v>1</v>
       </c>
       <c r="D53" s="72" t="s">
@@ -25555,7 +25555,7 @@
       <c r="B54" s="73" t="s">
         <v>698</v>
       </c>
-      <c r="C54" s="112">
+      <c r="C54" s="110">
         <v>1</v>
       </c>
       <c r="D54" s="72" t="s">
@@ -25584,7 +25584,7 @@
       <c r="B55" s="73" t="s">
         <v>1135</v>
       </c>
-      <c r="C55" s="112">
+      <c r="C55" s="110">
         <v>1</v>
       </c>
       <c r="D55" s="72" t="s">
@@ -25613,7 +25613,7 @@
       <c r="B56" s="73" t="s">
         <v>1139</v>
       </c>
-      <c r="C56" s="112">
+      <c r="C56" s="110">
         <v>1</v>
       </c>
       <c r="D56" s="72" t="s">
@@ -25642,7 +25642,7 @@
       <c r="B57" s="73" t="s">
         <v>1133</v>
       </c>
-      <c r="C57" s="112">
+      <c r="C57" s="110">
         <v>1</v>
       </c>
       <c r="D57" s="72" t="s">
@@ -25671,7 +25671,7 @@
       <c r="B58" s="73" t="s">
         <v>1134</v>
       </c>
-      <c r="C58" s="112">
+      <c r="C58" s="110">
         <v>1</v>
       </c>
       <c r="D58" s="72" t="s">
@@ -25700,7 +25700,7 @@
       <c r="B59" s="73" t="s">
         <v>700</v>
       </c>
-      <c r="C59" s="112">
+      <c r="C59" s="110">
         <v>1</v>
       </c>
       <c r="D59" s="72" t="s">
@@ -25729,7 +25729,7 @@
       <c r="B60" s="73" t="s">
         <v>701</v>
       </c>
-      <c r="C60" s="112">
+      <c r="C60" s="110">
         <v>1</v>
       </c>
       <c r="D60" s="72" t="s">
@@ -25758,7 +25758,7 @@
       <c r="B61" s="73" t="s">
         <v>702</v>
       </c>
-      <c r="C61" s="112">
+      <c r="C61" s="110">
         <v>1</v>
       </c>
       <c r="D61" s="72" t="s">
@@ -25787,7 +25787,7 @@
       <c r="B62" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="C62" s="112">
+      <c r="C62" s="110">
         <v>1</v>
       </c>
       <c r="D62" s="72" t="s">
@@ -25811,8 +25811,8 @@
       <c r="B63" s="73" t="s">
         <v>1179</v>
       </c>
-      <c r="C63" s="112">
-        <v>1</v>
+      <c r="C63" s="110">
+        <v>0</v>
       </c>
       <c r="D63" s="72" t="s">
         <v>72</v>
@@ -25835,7 +25835,7 @@
       <c r="B64" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="112">
+      <c r="C64" s="110">
         <v>1</v>
       </c>
       <c r="D64" s="72" t="s">
@@ -25859,7 +25859,7 @@
       <c r="B65" s="73" t="s">
         <v>636</v>
       </c>
-      <c r="C65" s="112">
+      <c r="C65" s="110">
         <v>1</v>
       </c>
       <c r="D65" s="72" t="s">
@@ -25883,7 +25883,7 @@
       <c r="B66" s="73" t="s">
         <v>703</v>
       </c>
-      <c r="C66" s="112">
+      <c r="C66" s="110">
         <v>1</v>
       </c>
       <c r="D66" s="72" t="s">
@@ -25907,7 +25907,7 @@
       <c r="B67" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="C67" s="112">
+      <c r="C67" s="110">
         <v>1</v>
       </c>
       <c r="D67" s="72" t="s">
@@ -25936,7 +25936,7 @@
       <c r="B68" s="73" t="s">
         <v>903</v>
       </c>
-      <c r="C68" s="112">
+      <c r="C68" s="110">
         <v>1</v>
       </c>
       <c r="D68" s="72" t="s">
@@ -25965,7 +25965,7 @@
       <c r="B69" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C69" s="112">
+      <c r="C69" s="110">
         <v>1</v>
       </c>
       <c r="D69" s="72" t="s">
@@ -25994,7 +25994,7 @@
       <c r="B70" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="C70" s="112">
+      <c r="C70" s="110">
         <v>1</v>
       </c>
       <c r="D70" s="72" t="s">
@@ -26023,7 +26023,7 @@
       <c r="B71" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="C71" s="112">
+      <c r="C71" s="110">
         <v>1</v>
       </c>
       <c r="D71" s="72" t="s">
@@ -26052,7 +26052,7 @@
       <c r="B72" s="73" t="s">
         <v>706</v>
       </c>
-      <c r="C72" s="112">
+      <c r="C72" s="110">
         <v>1</v>
       </c>
       <c r="D72" s="72" t="s">
@@ -26076,7 +26076,7 @@
       <c r="B73" s="73" t="s">
         <v>707</v>
       </c>
-      <c r="C73" s="112">
+      <c r="C73" s="110">
         <v>1</v>
       </c>
       <c r="D73" s="72" t="s">
@@ -26105,7 +26105,7 @@
       <c r="B74" s="73" t="s">
         <v>708</v>
       </c>
-      <c r="C74" s="112">
+      <c r="C74" s="110">
         <v>1</v>
       </c>
       <c r="D74" s="72" t="s">
@@ -26129,7 +26129,7 @@
       <c r="B75" s="73" t="s">
         <v>709</v>
       </c>
-      <c r="C75" s="112">
+      <c r="C75" s="110">
         <v>1</v>
       </c>
       <c r="D75" s="72" t="s">
@@ -51396,22 +51396,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
+      <c r="B2" s="116"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="11" t="s">
@@ -51427,13 +51427,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="110"/>
-      <c r="C21" s="110"/>
-      <c r="D21" s="110"/>
-      <c r="E21" s="110"/>
+      <c r="B21" s="116"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="116"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
@@ -51449,13 +51449,13 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="110" t="s">
+      <c r="A40" s="116" t="s">
         <v>193</v>
       </c>
-      <c r="B40" s="110"/>
-      <c r="C40" s="110"/>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
+      <c r="B40" s="116"/>
+      <c r="C40" s="116"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="116"/>
     </row>
     <row r="57" spans="1:2" ht="15.75" thickBot="1">
       <c r="A57" s="11" t="s">
@@ -51474,10 +51474,10 @@
       <c r="B81" s="17"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="109" t="s">
+      <c r="A82" s="115" t="s">
         <v>425</v>
       </c>
-      <c r="B82" s="109"/>
+      <c r="B82" s="115"/>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="15" t="s">

</xml_diff>